<commit_message>
More work on JPADCore_v2 concerning ACPerformanceManager and ACAnalysisManager.
</commit_message>
<xml_diff>
--- a/JPADSandBox_v2/out/ATR-72/PERFORMANCE/Performance.xlsx
+++ b/JPADSandBox_v2/out/ATR-72/PERFORMANCE/Performance.xlsx
@@ -11,14 +11,15 @@
     <sheet name="CRUISE" r:id="rId5" sheetId="3"/>
     <sheet name="DESCENT" r:id="rId6" sheetId="4"/>
     <sheet name="LANDING" r:id="rId7" sheetId="5"/>
-    <sheet name="PAYLOAD-RANGE" r:id="rId8" sheetId="6"/>
-    <sheet name="V-n DIAGRAM" r:id="rId9" sheetId="7"/>
+    <sheet name="MISSION PROFILE" r:id="rId8" sheetId="6"/>
+    <sheet name="PAYLOAD-RANGE" r:id="rId9" sheetId="7"/>
+    <sheet name="V-n DIAGRAM" r:id="rId10" sheetId="8"/>
   </sheets>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="344" uniqueCount="107">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="418" uniqueCount="140">
   <si>
     <t>Description</t>
   </si>
@@ -194,6 +195,108 @@
     <t>Landing duration</t>
   </si>
   <si>
+    <t>Total mission distance</t>
+  </si>
+  <si>
+    <t>Total mission duration</t>
+  </si>
+  <si>
+    <t>Aircraft mass at mission start</t>
+  </si>
+  <si>
+    <t>kg</t>
+  </si>
+  <si>
+    <t>Aircraft mass at mission end</t>
+  </si>
+  <si>
+    <t>Initial fuel mass for the assigned mission</t>
+  </si>
+  <si>
+    <t>Total fuel used</t>
+  </si>
+  <si>
+    <t>Fuel reserve</t>
+  </si>
+  <si>
+    <t>%</t>
+  </si>
+  <si>
+    <t>Take-off range</t>
+  </si>
+  <si>
+    <t>Climb range</t>
+  </si>
+  <si>
+    <t>Cruise range</t>
+  </si>
+  <si>
+    <t>First descent range</t>
+  </si>
+  <si>
+    <t>Alternate cruise range</t>
+  </si>
+  <si>
+    <t>Second descent range</t>
+  </si>
+  <si>
+    <t>Holding range</t>
+  </si>
+  <si>
+    <t>Third descent range</t>
+  </si>
+  <si>
+    <t>Landing range</t>
+  </si>
+  <si>
+    <t>Climb duration</t>
+  </si>
+  <si>
+    <t>Cruise duration</t>
+  </si>
+  <si>
+    <t>First descent duration</t>
+  </si>
+  <si>
+    <t>Alternate cruise duration</t>
+  </si>
+  <si>
+    <t>Second descent duration</t>
+  </si>
+  <si>
+    <t>Holding duration</t>
+  </si>
+  <si>
+    <t>Third descent duration</t>
+  </si>
+  <si>
+    <t>Take-off used fuel</t>
+  </si>
+  <si>
+    <t>Climb used fuel</t>
+  </si>
+  <si>
+    <t>Cruise used fuel</t>
+  </si>
+  <si>
+    <t>First descent used fuel</t>
+  </si>
+  <si>
+    <t>Alternate cruise used fuel</t>
+  </si>
+  <si>
+    <t>Second descent used fuel</t>
+  </si>
+  <si>
+    <t>Holding used fuel</t>
+  </si>
+  <si>
+    <t>Third descent used fuel</t>
+  </si>
+  <si>
+    <t>Landing used fuel</t>
+  </si>
+  <si>
     <t>CURRENT MACH CONDITION</t>
   </si>
   <si>
@@ -204,9 +307,6 @@
   </si>
   <si>
     <t>Aircraft mass</t>
-  </si>
-  <si>
-    <t>kg</t>
   </si>
   <si>
     <t>Payload mass</t>
@@ -1092,35 +1192,44 @@
       <c r="A2" t="s">
         <v>58</v>
       </c>
-      <c r="B2" t="n">
-        <v>0.42</v>
+      <c r="B2" t="s">
+        <v>47</v>
+      </c>
+      <c r="C2" t="n">
+        <v>286.99999999999994</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="s">
         <v>59</v>
       </c>
+      <c r="B3" t="s">
+        <v>26</v>
+      </c>
+      <c r="C3" t="n">
+        <v>126.00884291877313</v>
+      </c>
     </row>
     <row r="4">
       <c r="A4" t="s">
         <v>60</v>
       </c>
       <c r="B4" t="s">
-        <v>47</v>
+        <v>61</v>
       </c>
       <c r="C4" t="n">
-        <v>547.8151918716816</v>
+        <v>20578.704104989465</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="B5" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="C5" t="n">
-        <v>22500.0</v>
+        <v>19468.438264161327</v>
       </c>
     </row>
     <row r="6">
@@ -1128,10 +1237,10 @@
         <v>63</v>
       </c>
       <c r="B6" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="C6" t="n">
-        <v>7127.999999999999</v>
+        <v>1168.704104989471</v>
       </c>
     </row>
     <row r="7">
@@ -1139,10 +1248,10 @@
         <v>64</v>
       </c>
       <c r="B7" t="s">
-        <v>41</v>
+        <v>61</v>
       </c>
       <c r="C7" t="n">
-        <v>72.0</v>
+        <v>1110.2688997399976</v>
       </c>
     </row>
     <row r="8">
@@ -1150,612 +1259,322 @@
         <v>65</v>
       </c>
       <c r="B8" t="s">
-        <v>62</v>
+        <v>66</v>
       </c>
       <c r="C8" t="n">
-        <v>2421.999999999999</v>
+        <v>5.0</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="s">
-        <v>66</v>
-      </c>
-      <c r="B9" t="s">
-        <v>67</v>
-      </c>
-      <c r="C9" t="n">
-        <v>0.415677770382276</v>
+        <v>10</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="B10" t="s">
-        <v>41</v>
+        <v>47</v>
       </c>
       <c r="C10" t="n">
-        <v>0.6203642627648358</v>
+        <v>0.569205266926289</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="B11" t="s">
-        <v>41</v>
+        <v>47</v>
       </c>
       <c r="C11" t="n">
-        <v>0.04516033630403128</v>
+        <v>48.96645839353306</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="B12" t="s">
-        <v>41</v>
+        <v>47</v>
       </c>
       <c r="C12" t="n">
-        <v>13.736927435357881</v>
+        <v>84.19980568589754</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="s">
-        <v>41</v>
+        <v>70</v>
+      </c>
+      <c r="B13" t="s">
+        <v>47</v>
+      </c>
+      <c r="C13" t="n">
+        <v>37.563288450841625</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="s">
         <v>71</v>
       </c>
+      <c r="B14" t="s">
+        <v>47</v>
+      </c>
+      <c r="C14" t="n">
+        <v>86.99999999999994</v>
+      </c>
     </row>
     <row r="15">
       <c r="A15" t="s">
-        <v>60</v>
+        <v>72</v>
       </c>
       <c r="B15" t="s">
         <v>47</v>
       </c>
       <c r="C15" t="n">
-        <v>1731.7316551665067</v>
+        <v>24.68246722684944</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="s">
-        <v>61</v>
+        <v>73</v>
       </c>
       <c r="B16" t="s">
-        <v>62</v>
+        <v>47</v>
       </c>
       <c r="C16" t="n">
-        <v>22500.0</v>
+        <v>0.0</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" t="s">
-        <v>63</v>
+        <v>74</v>
       </c>
       <c r="B17" t="s">
-        <v>62</v>
+        <v>47</v>
       </c>
       <c r="C17" t="n">
-        <v>4549.999999999998</v>
+        <v>3.6104053632563193</v>
       </c>
     </row>
     <row r="18">
       <c r="A18" t="s">
-        <v>64</v>
+        <v>75</v>
       </c>
       <c r="B18" t="s">
-        <v>41</v>
+        <v>47</v>
       </c>
       <c r="C18" t="n">
-        <v>45.959595959595944</v>
+        <v>0.40887108794120763</v>
       </c>
     </row>
     <row r="19">
       <c r="A19" t="s">
-        <v>65</v>
-      </c>
-      <c r="B19" t="s">
-        <v>62</v>
-      </c>
-      <c r="C19" t="n">
-        <v>5000.0</v>
+        <v>10</v>
       </c>
     </row>
     <row r="20">
       <c r="A20" t="s">
-        <v>66</v>
+        <v>18</v>
       </c>
       <c r="B20" t="s">
-        <v>67</v>
+        <v>26</v>
       </c>
       <c r="C20" t="n">
-        <v>0.415677770382276</v>
+        <v>0.47835131276440124</v>
       </c>
     </row>
     <row r="21">
       <c r="A21" t="s">
-        <v>68</v>
+        <v>76</v>
       </c>
       <c r="B21" t="s">
-        <v>41</v>
+        <v>26</v>
       </c>
       <c r="C21" t="n">
-        <v>0.6203642627648358</v>
+        <v>17.362705019142627</v>
       </c>
     </row>
     <row r="22">
       <c r="A22" t="s">
-        <v>69</v>
+        <v>77</v>
       </c>
       <c r="B22" t="s">
-        <v>41</v>
+        <v>26</v>
       </c>
       <c r="C22" t="n">
-        <v>0.04516033630403128</v>
+        <v>19.554382445255904</v>
       </c>
     </row>
     <row r="23">
       <c r="A23" t="s">
-        <v>70</v>
+        <v>78</v>
       </c>
       <c r="B23" t="s">
-        <v>41</v>
+        <v>26</v>
       </c>
       <c r="C23" t="n">
-        <v>13.736927435357881</v>
+        <v>6.456692913385822</v>
       </c>
     </row>
     <row r="24">
       <c r="A24" t="s">
-        <v>41</v>
+        <v>79</v>
+      </c>
+      <c r="B24" t="s">
+        <v>26</v>
+      </c>
+      <c r="C24" t="n">
+        <v>30.28666944794869</v>
       </c>
     </row>
     <row r="25">
       <c r="A25" t="s">
-        <v>72</v>
+        <v>80</v>
+      </c>
+      <c r="B25" t="s">
+        <v>26</v>
+      </c>
+      <c r="C25" t="n">
+        <v>5.666666666666657</v>
       </c>
     </row>
     <row r="26">
       <c r="A26" t="s">
-        <v>60</v>
+        <v>81</v>
       </c>
       <c r="B26" t="s">
-        <v>47</v>
+        <v>26</v>
       </c>
       <c r="C26" t="n">
-        <v>2129.028741320142</v>
+        <v>44.999999999999986</v>
       </c>
     </row>
     <row r="27">
       <c r="A27" t="s">
-        <v>61</v>
+        <v>82</v>
       </c>
       <c r="B27" t="s">
-        <v>62</v>
+        <v>26</v>
       </c>
       <c r="C27" t="n">
-        <v>17949.999999999996</v>
+        <v>0.9666666666666615</v>
       </c>
     </row>
     <row r="28">
       <c r="A28" t="s">
-        <v>63</v>
+        <v>57</v>
       </c>
       <c r="B28" t="s">
-        <v>62</v>
+        <v>26</v>
       </c>
       <c r="C28" t="n">
-        <v>0.0</v>
+        <v>0.23670844694236592</v>
       </c>
     </row>
     <row r="29">
       <c r="A29" t="s">
-        <v>64</v>
-      </c>
-      <c r="B29" t="s">
-        <v>41</v>
-      </c>
-      <c r="C29" t="n">
-        <v>0.0</v>
+        <v>10</v>
       </c>
     </row>
     <row r="30">
       <c r="A30" t="s">
-        <v>65</v>
+        <v>83</v>
       </c>
       <c r="B30" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="C30" t="n">
-        <v>5000.0</v>
+        <v>8.939145363973067</v>
       </c>
     </row>
     <row r="31">
       <c r="A31" t="s">
-        <v>66</v>
+        <v>84</v>
       </c>
       <c r="B31" t="s">
-        <v>67</v>
+        <v>61</v>
       </c>
       <c r="C31" t="n">
-        <v>0.415677770382276</v>
+        <v>248.41740482016655</v>
       </c>
     </row>
     <row r="32">
       <c r="A32" t="s">
-        <v>68</v>
+        <v>85</v>
       </c>
       <c r="B32" t="s">
-        <v>41</v>
+        <v>61</v>
       </c>
       <c r="C32" t="n">
-        <v>0.4949128229612801</v>
+        <v>220.4545177395933</v>
       </c>
     </row>
     <row r="33">
       <c r="A33" t="s">
-        <v>69</v>
+        <v>86</v>
       </c>
       <c r="B33" t="s">
-        <v>41</v>
+        <v>61</v>
       </c>
       <c r="C33" t="n">
-        <v>0.04026495821920595</v>
+        <v>-0.9341677944122182</v>
       </c>
     </row>
     <row r="34">
       <c r="A34" t="s">
-        <v>70</v>
+        <v>87</v>
       </c>
       <c r="B34" t="s">
-        <v>41</v>
+        <v>61</v>
       </c>
       <c r="C34" t="n">
-        <v>12.291402868641548</v>
+        <v>428.70685516737757</v>
       </c>
     </row>
     <row r="35">
       <c r="A35" t="s">
-        <v>41</v>
+        <v>88</v>
+      </c>
+      <c r="B35" t="s">
+        <v>61</v>
+      </c>
+      <c r="C35" t="n">
+        <v>20.50336323875655</v>
       </c>
     </row>
     <row r="36">
       <c r="A36" t="s">
-        <v>41</v>
+        <v>89</v>
+      </c>
+      <c r="B36" t="s">
+        <v>61</v>
+      </c>
+      <c r="C36" t="n">
+        <v>180.02772892857894</v>
       </c>
     </row>
     <row r="37">
       <c r="A37" t="s">
-        <v>73</v>
-      </c>
-      <c r="B37" t="n">
-        <v>0.0</v>
+        <v>90</v>
+      </c>
+      <c r="B37" t="s">
+        <v>61</v>
+      </c>
+      <c r="C37" t="n">
+        <v>3.5267748915665607</v>
       </c>
     </row>
     <row r="38">
       <c r="A38" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="39">
-      <c r="A39" t="s">
-        <v>60</v>
-      </c>
-      <c r="B39" t="s">
-        <v>47</v>
-      </c>
-      <c r="C39" t="n">
-        <v>0.0</v>
-      </c>
-    </row>
-    <row r="40">
-      <c r="A40" t="s">
-        <v>61</v>
-      </c>
-      <c r="B40" t="s">
-        <v>62</v>
-      </c>
-      <c r="C40" t="n">
-        <v>22500.0</v>
-      </c>
-    </row>
-    <row r="41">
-      <c r="A41" t="s">
-        <v>63</v>
-      </c>
-      <c r="B41" t="s">
-        <v>62</v>
-      </c>
-      <c r="C41" t="n">
-        <v>7127.999999999999</v>
-      </c>
-    </row>
-    <row r="42">
-      <c r="A42" t="s">
-        <v>64</v>
-      </c>
-      <c r="B42" t="s">
-        <v>41</v>
-      </c>
-      <c r="C42" t="n">
-        <v>72.0</v>
-      </c>
-    </row>
-    <row r="43">
-      <c r="A43" t="s">
-        <v>65</v>
-      </c>
-      <c r="B43" t="s">
-        <v>62</v>
-      </c>
-      <c r="C43" t="n">
-        <v>2421.999999999999</v>
-      </c>
-    </row>
-    <row r="44">
-      <c r="A44" t="s">
-        <v>66</v>
-      </c>
-      <c r="B44" t="s">
-        <v>67</v>
-      </c>
-      <c r="C44" t="n">
-        <v>0.25789643494623077</v>
-      </c>
-    </row>
-    <row r="45">
-      <c r="A45" t="s">
-        <v>68</v>
-      </c>
-      <c r="B45" t="s">
-        <v>41</v>
-      </c>
-      <c r="C45" t="n">
-        <v>0.0</v>
-      </c>
-    </row>
-    <row r="46">
-      <c r="A46" t="s">
-        <v>69</v>
-      </c>
-      <c r="B46" t="s">
-        <v>41</v>
-      </c>
-      <c r="C46" t="n">
-        <v>0.06340116491073258</v>
-      </c>
-    </row>
-    <row r="47">
-      <c r="A47" t="s">
-        <v>70</v>
-      </c>
-      <c r="B47" t="s">
-        <v>41</v>
-      </c>
-      <c r="C47" t="n">
-        <v>0.0</v>
-      </c>
-    </row>
-    <row r="48">
-      <c r="A48" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="49">
-      <c r="A49" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="50">
-      <c r="A50" t="s">
-        <v>60</v>
-      </c>
-      <c r="B50" t="s">
-        <v>47</v>
-      </c>
-      <c r="C50" t="n">
-        <v>0.0</v>
-      </c>
-    </row>
-    <row r="51">
-      <c r="A51" t="s">
-        <v>61</v>
-      </c>
-      <c r="B51" t="s">
-        <v>62</v>
-      </c>
-      <c r="C51" t="n">
-        <v>22500.0</v>
-      </c>
-    </row>
-    <row r="52">
-      <c r="A52" t="s">
-        <v>63</v>
-      </c>
-      <c r="B52" t="s">
-        <v>62</v>
-      </c>
-      <c r="C52" t="n">
-        <v>4549.999999999998</v>
-      </c>
-    </row>
-    <row r="53">
-      <c r="A53" t="s">
-        <v>64</v>
-      </c>
-      <c r="B53" t="s">
-        <v>41</v>
-      </c>
-      <c r="C53" t="n">
-        <v>45.959595959595944</v>
-      </c>
-    </row>
-    <row r="54">
-      <c r="A54" t="s">
-        <v>65</v>
-      </c>
-      <c r="B54" t="s">
-        <v>62</v>
-      </c>
-      <c r="C54" t="n">
-        <v>5000.0</v>
-      </c>
-    </row>
-    <row r="55">
-      <c r="A55" t="s">
-        <v>66</v>
-      </c>
-      <c r="B55" t="s">
-        <v>67</v>
-      </c>
-      <c r="C55" t="n">
-        <v>0.25789643494623077</v>
-      </c>
-    </row>
-    <row r="56">
-      <c r="A56" t="s">
-        <v>68</v>
-      </c>
-      <c r="B56" t="s">
-        <v>41</v>
-      </c>
-      <c r="C56" t="n">
-        <v>0.0</v>
-      </c>
-    </row>
-    <row r="57">
-      <c r="A57" t="s">
-        <v>69</v>
-      </c>
-      <c r="B57" t="s">
-        <v>41</v>
-      </c>
-      <c r="C57" t="n">
-        <v>0.06340116491073258</v>
-      </c>
-    </row>
-    <row r="58">
-      <c r="A58" t="s">
-        <v>70</v>
-      </c>
-      <c r="B58" t="s">
-        <v>41</v>
-      </c>
-      <c r="C58" t="n">
-        <v>0.0</v>
-      </c>
-    </row>
-    <row r="59">
-      <c r="A59" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="60">
-      <c r="A60" t="s">
-        <v>72</v>
-      </c>
-    </row>
-    <row r="61">
-      <c r="A61" t="s">
-        <v>60</v>
-      </c>
-      <c r="B61" t="s">
-        <v>47</v>
-      </c>
-      <c r="C61" t="n">
-        <v>0.0</v>
-      </c>
-    </row>
-    <row r="62">
-      <c r="A62" t="s">
-        <v>61</v>
-      </c>
-      <c r="B62" t="s">
-        <v>62</v>
-      </c>
-      <c r="C62" t="n">
-        <v>17949.999999999996</v>
-      </c>
-    </row>
-    <row r="63">
-      <c r="A63" t="s">
-        <v>63</v>
-      </c>
-      <c r="B63" t="s">
-        <v>62</v>
-      </c>
-      <c r="C63" t="n">
-        <v>0.0</v>
-      </c>
-    </row>
-    <row r="64">
-      <c r="A64" t="s">
-        <v>64</v>
-      </c>
-      <c r="B64" t="s">
-        <v>41</v>
-      </c>
-      <c r="C64" t="n">
-        <v>0.0</v>
-      </c>
-    </row>
-    <row r="65">
-      <c r="A65" t="s">
-        <v>65</v>
-      </c>
-      <c r="B65" t="s">
-        <v>62</v>
-      </c>
-      <c r="C65" t="n">
-        <v>5000.0</v>
-      </c>
-    </row>
-    <row r="66">
-      <c r="A66" t="s">
-        <v>66</v>
-      </c>
-      <c r="B66" t="s">
-        <v>67</v>
-      </c>
-      <c r="C66" t="n">
-        <v>0.25789643494623077</v>
-      </c>
-    </row>
-    <row r="67">
-      <c r="A67" t="s">
-        <v>68</v>
-      </c>
-      <c r="B67" t="s">
-        <v>41</v>
-      </c>
-      <c r="C67" t="n">
-        <v>0.0</v>
-      </c>
-    </row>
-    <row r="68">
-      <c r="A68" t="s">
-        <v>69</v>
-      </c>
-      <c r="B68" t="s">
-        <v>41</v>
-      </c>
-      <c r="C68" t="n">
-        <v>0.06340116491073258</v>
-      </c>
-    </row>
-    <row r="69">
-      <c r="A69" t="s">
-        <v>70</v>
-      </c>
-      <c r="B69" t="s">
-        <v>41</v>
-      </c>
-      <c r="C69" t="n">
-        <v>0.0</v>
+        <v>91</v>
+      </c>
+      <c r="B38" t="s">
+        <v>61</v>
+      </c>
+      <c r="C38" t="n">
+        <v>0.627277384397189</v>
       </c>
     </row>
   </sheetData>
@@ -1784,18 +1603,712 @@
     </row>
     <row r="2">
       <c r="A2" t="s">
-        <v>74</v>
-      </c>
-      <c r="B2" t="s">
-        <v>75</v>
+        <v>92</v>
+      </c>
+      <c r="B2" t="n">
+        <v>0.42</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="s">
-        <v>76</v>
+        <v>93</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="s">
+        <v>94</v>
+      </c>
+      <c r="B4" t="s">
+        <v>47</v>
+      </c>
+      <c r="C4" t="n">
+        <v>672.2851867445149</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="s">
+        <v>95</v>
+      </c>
+      <c r="B5" t="s">
+        <v>61</v>
+      </c>
+      <c r="C5" t="n">
+        <v>22500.0</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="s">
+        <v>96</v>
+      </c>
+      <c r="B6" t="s">
+        <v>61</v>
+      </c>
+      <c r="C6" t="n">
+        <v>6839.999999999999</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="s">
+        <v>97</v>
+      </c>
+      <c r="B7" t="s">
+        <v>41</v>
+      </c>
+      <c r="C7" t="n">
+        <v>72.0</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="s">
+        <v>98</v>
+      </c>
+      <c r="B8" t="s">
+        <v>61</v>
+      </c>
+      <c r="C8" t="n">
+        <v>2709.999999999999</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="s">
+        <v>99</v>
+      </c>
+      <c r="B9" t="s">
+        <v>100</v>
+      </c>
+      <c r="C9" t="n">
+        <v>0.415677770382276</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="s">
+        <v>101</v>
+      </c>
+      <c r="B10" t="s">
+        <v>41</v>
+      </c>
+      <c r="C10" t="n">
+        <v>0.6203642627648358</v>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="s">
+        <v>102</v>
+      </c>
+      <c r="B11" t="s">
+        <v>41</v>
+      </c>
+      <c r="C11" t="n">
+        <v>0.04516033630403128</v>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" t="s">
+        <v>103</v>
+      </c>
+      <c r="B12" t="s">
+        <v>41</v>
+      </c>
+      <c r="C12" t="n">
+        <v>13.736927435357881</v>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" t="s">
+        <v>94</v>
+      </c>
+      <c r="B15" t="s">
+        <v>47</v>
+      </c>
+      <c r="C15" t="n">
+        <v>1731.7316551665067</v>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" t="s">
+        <v>95</v>
+      </c>
+      <c r="B16" t="s">
+        <v>61</v>
+      </c>
+      <c r="C16" t="n">
+        <v>22500.0</v>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" t="s">
+        <v>96</v>
+      </c>
+      <c r="B17" t="s">
+        <v>61</v>
+      </c>
+      <c r="C17" t="n">
+        <v>4549.999999999996</v>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" t="s">
+        <v>97</v>
+      </c>
+      <c r="B18" t="s">
+        <v>41</v>
+      </c>
+      <c r="C18" t="n">
+        <v>47.89473684210524</v>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" t="s">
+        <v>98</v>
+      </c>
+      <c r="B19" t="s">
+        <v>61</v>
+      </c>
+      <c r="C19" t="n">
+        <v>5000.0</v>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" t="s">
+        <v>99</v>
+      </c>
+      <c r="B20" t="s">
+        <v>100</v>
+      </c>
+      <c r="C20" t="n">
+        <v>0.415677770382276</v>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" t="s">
+        <v>101</v>
+      </c>
+      <c r="B21" t="s">
+        <v>41</v>
+      </c>
+      <c r="C21" t="n">
+        <v>0.6203642627648358</v>
+      </c>
+    </row>
+    <row r="22">
+      <c r="A22" t="s">
+        <v>102</v>
+      </c>
+      <c r="B22" t="s">
+        <v>41</v>
+      </c>
+      <c r="C22" t="n">
+        <v>0.04516033630403128</v>
+      </c>
+    </row>
+    <row r="23">
+      <c r="A23" t="s">
+        <v>103</v>
+      </c>
+      <c r="B23" t="s">
+        <v>41</v>
+      </c>
+      <c r="C23" t="n">
+        <v>13.736927435357881</v>
+      </c>
+    </row>
+    <row r="24">
+      <c r="A24" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="25">
+      <c r="A25" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="26">
+      <c r="A26" t="s">
+        <v>94</v>
+      </c>
+      <c r="B26" t="s">
+        <v>47</v>
+      </c>
+      <c r="C26" t="n">
+        <v>2129.028741320142</v>
+      </c>
+    </row>
+    <row r="27">
+      <c r="A27" t="s">
+        <v>95</v>
+      </c>
+      <c r="B27" t="s">
+        <v>61</v>
+      </c>
+      <c r="C27" t="n">
+        <v>17949.999999999996</v>
+      </c>
+    </row>
+    <row r="28">
+      <c r="A28" t="s">
+        <v>96</v>
+      </c>
+      <c r="B28" t="s">
+        <v>61</v>
+      </c>
+      <c r="C28" t="n">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="29">
+      <c r="A29" t="s">
+        <v>97</v>
+      </c>
+      <c r="B29" t="s">
+        <v>41</v>
+      </c>
+      <c r="C29" t="n">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="30">
+      <c r="A30" t="s">
+        <v>98</v>
+      </c>
+      <c r="B30" t="s">
+        <v>61</v>
+      </c>
+      <c r="C30" t="n">
+        <v>5000.0</v>
+      </c>
+    </row>
+    <row r="31">
+      <c r="A31" t="s">
+        <v>99</v>
+      </c>
+      <c r="B31" t="s">
+        <v>100</v>
+      </c>
+      <c r="C31" t="n">
+        <v>0.415677770382276</v>
+      </c>
+    </row>
+    <row r="32">
+      <c r="A32" t="s">
+        <v>101</v>
+      </c>
+      <c r="B32" t="s">
+        <v>41</v>
+      </c>
+      <c r="C32" t="n">
+        <v>0.4949128229612801</v>
+      </c>
+    </row>
+    <row r="33">
+      <c r="A33" t="s">
+        <v>102</v>
+      </c>
+      <c r="B33" t="s">
+        <v>41</v>
+      </c>
+      <c r="C33" t="n">
+        <v>0.04026495821920595</v>
+      </c>
+    </row>
+    <row r="34">
+      <c r="A34" t="s">
+        <v>103</v>
+      </c>
+      <c r="B34" t="s">
+        <v>41</v>
+      </c>
+      <c r="C34" t="n">
+        <v>12.291402868641548</v>
+      </c>
+    </row>
+    <row r="35">
+      <c r="A35" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="36">
+      <c r="A36" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="37">
+      <c r="A37" t="s">
+        <v>106</v>
+      </c>
+      <c r="B37" t="n">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="38">
+      <c r="A38" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="39">
+      <c r="A39" t="s">
+        <v>94</v>
+      </c>
+      <c r="B39" t="s">
+        <v>47</v>
+      </c>
+      <c r="C39" t="n">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="40">
+      <c r="A40" t="s">
+        <v>95</v>
+      </c>
+      <c r="B40" t="s">
+        <v>61</v>
+      </c>
+      <c r="C40" t="n">
+        <v>22500.0</v>
+      </c>
+    </row>
+    <row r="41">
+      <c r="A41" t="s">
+        <v>96</v>
+      </c>
+      <c r="B41" t="s">
+        <v>61</v>
+      </c>
+      <c r="C41" t="n">
+        <v>6839.999999999999</v>
+      </c>
+    </row>
+    <row r="42">
+      <c r="A42" t="s">
+        <v>97</v>
+      </c>
+      <c r="B42" t="s">
+        <v>41</v>
+      </c>
+      <c r="C42" t="n">
+        <v>72.0</v>
+      </c>
+    </row>
+    <row r="43">
+      <c r="A43" t="s">
+        <v>98</v>
+      </c>
+      <c r="B43" t="s">
+        <v>61</v>
+      </c>
+      <c r="C43" t="n">
+        <v>2709.999999999999</v>
+      </c>
+    </row>
+    <row r="44">
+      <c r="A44" t="s">
+        <v>99</v>
+      </c>
+      <c r="B44" t="s">
+        <v>100</v>
+      </c>
+      <c r="C44" t="n">
+        <v>0.25789643494623077</v>
+      </c>
+    </row>
+    <row r="45">
+      <c r="A45" t="s">
+        <v>101</v>
+      </c>
+      <c r="B45" t="s">
+        <v>41</v>
+      </c>
+      <c r="C45" t="n">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="46">
+      <c r="A46" t="s">
+        <v>102</v>
+      </c>
+      <c r="B46" t="s">
+        <v>41</v>
+      </c>
+      <c r="C46" t="n">
+        <v>0.06340116491073258</v>
+      </c>
+    </row>
+    <row r="47">
+      <c r="A47" t="s">
+        <v>103</v>
+      </c>
+      <c r="B47" t="s">
+        <v>41</v>
+      </c>
+      <c r="C47" t="n">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="48">
+      <c r="A48" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="49">
+      <c r="A49" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="50">
+      <c r="A50" t="s">
+        <v>94</v>
+      </c>
+      <c r="B50" t="s">
+        <v>47</v>
+      </c>
+      <c r="C50" t="n">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="51">
+      <c r="A51" t="s">
+        <v>95</v>
+      </c>
+      <c r="B51" t="s">
+        <v>61</v>
+      </c>
+      <c r="C51" t="n">
+        <v>22500.0</v>
+      </c>
+    </row>
+    <row r="52">
+      <c r="A52" t="s">
+        <v>96</v>
+      </c>
+      <c r="B52" t="s">
+        <v>61</v>
+      </c>
+      <c r="C52" t="n">
+        <v>4549.999999999996</v>
+      </c>
+    </row>
+    <row r="53">
+      <c r="A53" t="s">
+        <v>97</v>
+      </c>
+      <c r="B53" t="s">
+        <v>41</v>
+      </c>
+      <c r="C53" t="n">
+        <v>47.89473684210524</v>
+      </c>
+    </row>
+    <row r="54">
+      <c r="A54" t="s">
+        <v>98</v>
+      </c>
+      <c r="B54" t="s">
+        <v>61</v>
+      </c>
+      <c r="C54" t="n">
+        <v>5000.0</v>
+      </c>
+    </row>
+    <row r="55">
+      <c r="A55" t="s">
+        <v>99</v>
+      </c>
+      <c r="B55" t="s">
+        <v>100</v>
+      </c>
+      <c r="C55" t="n">
+        <v>0.25789643494623077</v>
+      </c>
+    </row>
+    <row r="56">
+      <c r="A56" t="s">
+        <v>101</v>
+      </c>
+      <c r="B56" t="s">
+        <v>41</v>
+      </c>
+      <c r="C56" t="n">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="57">
+      <c r="A57" t="s">
+        <v>102</v>
+      </c>
+      <c r="B57" t="s">
+        <v>41</v>
+      </c>
+      <c r="C57" t="n">
+        <v>0.06340116491073258</v>
+      </c>
+    </row>
+    <row r="58">
+      <c r="A58" t="s">
+        <v>103</v>
+      </c>
+      <c r="B58" t="s">
+        <v>41</v>
+      </c>
+      <c r="C58" t="n">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="59">
+      <c r="A59" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="60">
+      <c r="A60" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="61">
+      <c r="A61" t="s">
+        <v>94</v>
+      </c>
+      <c r="B61" t="s">
+        <v>47</v>
+      </c>
+      <c r="C61" t="n">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="62">
+      <c r="A62" t="s">
+        <v>95</v>
+      </c>
+      <c r="B62" t="s">
+        <v>61</v>
+      </c>
+      <c r="C62" t="n">
+        <v>17949.999999999996</v>
+      </c>
+    </row>
+    <row r="63">
+      <c r="A63" t="s">
+        <v>96</v>
+      </c>
+      <c r="B63" t="s">
+        <v>61</v>
+      </c>
+      <c r="C63" t="n">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="64">
+      <c r="A64" t="s">
+        <v>97</v>
+      </c>
+      <c r="B64" t="s">
+        <v>41</v>
+      </c>
+      <c r="C64" t="n">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="65">
+      <c r="A65" t="s">
+        <v>98</v>
+      </c>
+      <c r="B65" t="s">
+        <v>61</v>
+      </c>
+      <c r="C65" t="n">
+        <v>5000.0</v>
+      </c>
+    </row>
+    <row r="66">
+      <c r="A66" t="s">
+        <v>99</v>
+      </c>
+      <c r="B66" t="s">
+        <v>100</v>
+      </c>
+      <c r="C66" t="n">
+        <v>0.25789643494623077</v>
+      </c>
+    </row>
+    <row r="67">
+      <c r="A67" t="s">
+        <v>101</v>
+      </c>
+      <c r="B67" t="s">
+        <v>41</v>
+      </c>
+      <c r="C67" t="n">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="68">
+      <c r="A68" t="s">
+        <v>102</v>
+      </c>
+      <c r="B68" t="s">
+        <v>41</v>
+      </c>
+      <c r="C68" t="n">
+        <v>0.06340116491073258</v>
+      </c>
+    </row>
+    <row r="69">
+      <c r="A69" t="s">
+        <v>103</v>
+      </c>
+      <c r="B69" t="s">
+        <v>41</v>
+      </c>
+      <c r="C69" t="n">
+        <v>0.0</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15.0" baseColWidth="35"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="s">
+        <v>107</v>
+      </c>
+      <c r="B2" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="s">
+        <v>109</v>
       </c>
       <c r="B3" t="s">
-        <v>77</v>
+        <v>110</v>
       </c>
     </row>
     <row r="4">
@@ -1810,12 +2323,12 @@
     </row>
     <row r="6">
       <c r="A6" t="s">
-        <v>78</v>
+        <v>111</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="s">
-        <v>79</v>
+        <v>112</v>
       </c>
       <c r="B7" t="s">
         <v>12</v>
@@ -1826,7 +2339,7 @@
     </row>
     <row r="8">
       <c r="A8" t="s">
-        <v>80</v>
+        <v>113</v>
       </c>
       <c r="B8" t="s">
         <v>12</v>
@@ -1837,12 +2350,12 @@
     </row>
     <row r="9">
       <c r="A9" t="s">
-        <v>81</v>
+        <v>114</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="s">
-        <v>82</v>
+        <v>115</v>
       </c>
       <c r="B10" t="s">
         <v>12</v>
@@ -1853,7 +2366,7 @@
     </row>
     <row r="11">
       <c r="A11" t="s">
-        <v>83</v>
+        <v>116</v>
       </c>
       <c r="B11" t="s">
         <v>41</v>
@@ -1864,12 +2377,12 @@
     </row>
     <row r="12">
       <c r="A12" t="s">
-        <v>84</v>
+        <v>117</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="s">
-        <v>85</v>
+        <v>118</v>
       </c>
       <c r="B13" t="s">
         <v>12</v>
@@ -1880,7 +2393,7 @@
     </row>
     <row r="14">
       <c r="A14" t="s">
-        <v>83</v>
+        <v>116</v>
       </c>
       <c r="B14" t="s">
         <v>41</v>
@@ -1891,12 +2404,12 @@
     </row>
     <row r="15">
       <c r="A15" t="s">
-        <v>86</v>
+        <v>119</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="s">
-        <v>87</v>
+        <v>120</v>
       </c>
       <c r="B16" t="s">
         <v>12</v>
@@ -1907,7 +2420,7 @@
     </row>
     <row r="17">
       <c r="A17" t="s">
-        <v>83</v>
+        <v>116</v>
       </c>
       <c r="B17" t="s">
         <v>41</v>
@@ -1918,12 +2431,12 @@
     </row>
     <row r="18">
       <c r="A18" t="s">
-        <v>88</v>
+        <v>121</v>
       </c>
     </row>
     <row r="19">
       <c r="A19" t="s">
-        <v>87</v>
+        <v>120</v>
       </c>
       <c r="B19" t="s">
         <v>12</v>
@@ -1934,7 +2447,7 @@
     </row>
     <row r="20">
       <c r="A20" t="s">
-        <v>83</v>
+        <v>116</v>
       </c>
       <c r="B20" t="s">
         <v>41</v>
@@ -1945,12 +2458,12 @@
     </row>
     <row r="21">
       <c r="A21" t="s">
-        <v>89</v>
+        <v>122</v>
       </c>
     </row>
     <row r="22">
       <c r="A22" t="s">
-        <v>85</v>
+        <v>118</v>
       </c>
       <c r="B22" t="s">
         <v>12</v>
@@ -1961,7 +2474,7 @@
     </row>
     <row r="23">
       <c r="A23" t="s">
-        <v>83</v>
+        <v>116</v>
       </c>
       <c r="B23" t="s">
         <v>41</v>
@@ -1972,12 +2485,12 @@
     </row>
     <row r="24">
       <c r="A24" t="s">
-        <v>90</v>
+        <v>123</v>
       </c>
     </row>
     <row r="25">
       <c r="A25" t="s">
-        <v>91</v>
+        <v>124</v>
       </c>
       <c r="B25" t="s">
         <v>12</v>
@@ -1988,7 +2501,7 @@
     </row>
     <row r="26">
       <c r="A26" t="s">
-        <v>83</v>
+        <v>116</v>
       </c>
       <c r="B26" t="s">
         <v>41</v>
@@ -2004,17 +2517,17 @@
     </row>
     <row r="28">
       <c r="A28" t="s">
-        <v>92</v>
+        <v>125</v>
       </c>
     </row>
     <row r="29">
       <c r="A29" t="s">
-        <v>93</v>
+        <v>126</v>
       </c>
     </row>
     <row r="30">
       <c r="A30" t="s">
-        <v>82</v>
+        <v>115</v>
       </c>
       <c r="B30" t="s">
         <v>12</v>
@@ -2025,7 +2538,7 @@
     </row>
     <row r="31">
       <c r="A31" t="s">
-        <v>83</v>
+        <v>116</v>
       </c>
       <c r="B31" t="s">
         <v>41</v>
@@ -2036,12 +2549,12 @@
     </row>
     <row r="32">
       <c r="A32" t="s">
-        <v>94</v>
+        <v>127</v>
       </c>
     </row>
     <row r="33">
       <c r="A33" t="s">
-        <v>85</v>
+        <v>118</v>
       </c>
       <c r="B33" t="s">
         <v>12</v>
@@ -2052,7 +2565,7 @@
     </row>
     <row r="34">
       <c r="A34" t="s">
-        <v>83</v>
+        <v>116</v>
       </c>
       <c r="B34" t="s">
         <v>41</v>
@@ -2063,12 +2576,12 @@
     </row>
     <row r="35">
       <c r="A35" t="s">
-        <v>95</v>
+        <v>128</v>
       </c>
     </row>
     <row r="36">
       <c r="A36" t="s">
-        <v>87</v>
+        <v>120</v>
       </c>
       <c r="B36" t="s">
         <v>12</v>
@@ -2079,7 +2592,7 @@
     </row>
     <row r="37">
       <c r="A37" t="s">
-        <v>83</v>
+        <v>116</v>
       </c>
       <c r="B37" t="s">
         <v>41</v>
@@ -2090,12 +2603,12 @@
     </row>
     <row r="38">
       <c r="A38" t="s">
-        <v>96</v>
+        <v>129</v>
       </c>
     </row>
     <row r="39">
       <c r="A39" t="s">
-        <v>87</v>
+        <v>120</v>
       </c>
       <c r="B39" t="s">
         <v>12</v>
@@ -2106,7 +2619,7 @@
     </row>
     <row r="40">
       <c r="A40" t="s">
-        <v>83</v>
+        <v>116</v>
       </c>
       <c r="B40" t="s">
         <v>41</v>
@@ -2117,12 +2630,12 @@
     </row>
     <row r="41">
       <c r="A41" t="s">
-        <v>97</v>
+        <v>130</v>
       </c>
     </row>
     <row r="42">
       <c r="A42" t="s">
-        <v>85</v>
+        <v>118</v>
       </c>
       <c r="B42" t="s">
         <v>12</v>
@@ -2133,7 +2646,7 @@
     </row>
     <row r="43">
       <c r="A43" t="s">
-        <v>83</v>
+        <v>116</v>
       </c>
       <c r="B43" t="s">
         <v>41</v>
@@ -2144,12 +2657,12 @@
     </row>
     <row r="44">
       <c r="A44" t="s">
-        <v>98</v>
+        <v>131</v>
       </c>
     </row>
     <row r="45">
       <c r="A45" t="s">
-        <v>91</v>
+        <v>124</v>
       </c>
       <c r="B45" t="s">
         <v>12</v>
@@ -2160,7 +2673,7 @@
     </row>
     <row r="46">
       <c r="A46" t="s">
-        <v>83</v>
+        <v>116</v>
       </c>
       <c r="B46" t="s">
         <v>41</v>
@@ -2181,12 +2694,12 @@
     </row>
     <row r="49">
       <c r="A49" t="s">
-        <v>99</v>
+        <v>132</v>
       </c>
     </row>
     <row r="50">
       <c r="A50" t="s">
-        <v>100</v>
+        <v>133</v>
       </c>
       <c r="B50" t="s">
         <v>12</v>
@@ -2197,12 +2710,12 @@
     </row>
     <row r="51">
       <c r="A51" t="s">
-        <v>101</v>
+        <v>134</v>
       </c>
     </row>
     <row r="52">
       <c r="A52" t="s">
-        <v>102</v>
+        <v>135</v>
       </c>
       <c r="B52" t="s">
         <v>12</v>
@@ -2213,7 +2726,7 @@
     </row>
     <row r="53">
       <c r="A53" t="s">
-        <v>83</v>
+        <v>116</v>
       </c>
       <c r="B53" t="s">
         <v>41</v>
@@ -2224,12 +2737,12 @@
     </row>
     <row r="54">
       <c r="A54" t="s">
-        <v>103</v>
+        <v>136</v>
       </c>
     </row>
     <row r="55">
       <c r="A55" t="s">
-        <v>82</v>
+        <v>115</v>
       </c>
       <c r="B55" t="s">
         <v>12</v>
@@ -2240,7 +2753,7 @@
     </row>
     <row r="56">
       <c r="A56" t="s">
-        <v>83</v>
+        <v>116</v>
       </c>
       <c r="B56" t="s">
         <v>41</v>
@@ -2256,17 +2769,17 @@
     </row>
     <row r="58">
       <c r="A58" t="s">
-        <v>104</v>
+        <v>137</v>
       </c>
     </row>
     <row r="59">
       <c r="A59" t="s">
-        <v>105</v>
+        <v>138</v>
       </c>
     </row>
     <row r="60">
       <c r="A60" t="s">
-        <v>102</v>
+        <v>135</v>
       </c>
       <c r="B60" t="s">
         <v>12</v>
@@ -2277,7 +2790,7 @@
     </row>
     <row r="61">
       <c r="A61" t="s">
-        <v>83</v>
+        <v>116</v>
       </c>
       <c r="B61" t="s">
         <v>41</v>
@@ -2288,12 +2801,12 @@
     </row>
     <row r="62">
       <c r="A62" t="s">
-        <v>106</v>
+        <v>139</v>
       </c>
     </row>
     <row r="63">
       <c r="A63" t="s">
-        <v>82</v>
+        <v>115</v>
       </c>
       <c r="B63" t="s">
         <v>12</v>
@@ -2304,7 +2817,7 @@
     </row>
     <row r="64">
       <c r="A64" t="s">
-        <v>83</v>
+        <v>116</v>
       </c>
       <c r="B64" t="s">
         <v>41</v>

</xml_diff>

<commit_message>
More tests on ACPerformanceManager.
</commit_message>
<xml_diff>
--- a/JPADSandBox_v2/out/ATR-72/PERFORMANCE/Performance.xlsx
+++ b/JPADSandBox_v2/out/ATR-72/PERFORMANCE/Performance.xlsx
@@ -6,13 +6,13 @@
     <workbookView activeTab="0"/>
   </bookViews>
   <sheets>
-    <sheet name="CRUISE" r:id="rId3" sheetId="1"/>
+    <sheet name="LANDING" r:id="rId3" sheetId="1"/>
   </sheets>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="17">
   <si>
     <t>Description</t>
   </si>
@@ -23,58 +23,46 @@
     <t>Value</t>
   </si>
   <si>
-    <t>Thrust at cruise altitude and Mach</t>
-  </si>
-  <si>
-    <t>N</t>
-  </si>
-  <si>
-    <t>Drag at cruise altitude and Mach</t>
+    <t>Ground roll distance</t>
+  </si>
+  <si>
+    <t>m</t>
+  </si>
+  <si>
+    <t>Flare distance</t>
+  </si>
+  <si>
+    <t>Airborne distance</t>
+  </si>
+  <si>
+    <t>Landing distance</t>
+  </si>
+  <si>
+    <t>FAR-25 landing field length</t>
   </si>
   <si>
     <t xml:space="preserve"> </t>
   </si>
   <si>
-    <t>Power available at cruise altitude and Mach</t>
-  </si>
-  <si>
-    <t>W</t>
-  </si>
-  <si>
-    <t>Power needed at cruise altitude and Mach</t>
-  </si>
-  <si>
-    <t>Min speed at cruise altitude (CAS)</t>
+    <t>Stall speed landing (VsLND)</t>
   </si>
   <si>
     <t>m/s</t>
   </si>
   <si>
-    <t>Max speed at cruise altitude (CAS)</t>
-  </si>
-  <si>
-    <t>Min speed at cruise altitude (TAS)</t>
-  </si>
-  <si>
-    <t>Max speed at cruise altitude (TAS)</t>
-  </si>
-  <si>
-    <t>Min Mach number at cruise altitude</t>
-  </si>
-  <si>
-    <t/>
-  </si>
-  <si>
-    <t>Max Mach number at cruise altitude</t>
-  </si>
-  <si>
-    <t>Efficiency at cruise altitude and Mach</t>
-  </si>
-  <si>
-    <t>Specific range at cruise altitude and Mach</t>
-  </si>
-  <si>
-    <t>nmi/lbs</t>
+    <t>Touchdown speed (V_TD)</t>
+  </si>
+  <si>
+    <t>Flare speed (V_Flare)</t>
+  </si>
+  <si>
+    <t>Approach speed (V_A)</t>
+  </si>
+  <si>
+    <t>Landing duration</t>
+  </si>
+  <si>
+    <t>s</t>
   </si>
 </sst>
 </file>
@@ -161,7 +149,7 @@
         <v>4</v>
       </c>
       <c r="C2" t="n">
-        <v>15944.104756602905</v>
+        <v>330.0813581485204</v>
       </c>
     </row>
     <row r="3">
@@ -172,39 +160,45 @@
         <v>4</v>
       </c>
       <c r="C3" t="n">
-        <v>15598.717921590116</v>
+        <v>75.13255097031549</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="s">
         <v>6</v>
       </c>
+      <c r="B4" t="s">
+        <v>4</v>
+      </c>
+      <c r="C4" t="n">
+        <v>253.25600692440025</v>
+      </c>
     </row>
     <row r="5">
       <c r="A5" t="s">
         <v>7</v>
       </c>
       <c r="B5" t="s">
-        <v>8</v>
+        <v>4</v>
       </c>
       <c r="C5" t="n">
-        <v>2119124.297077124</v>
+        <v>658.4699160432363</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B6" t="s">
-        <v>8</v>
+        <v>4</v>
       </c>
       <c r="C6" t="n">
-        <v>2073224.0069692507</v>
+        <v>1097.4498600720603</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="s">
-        <v>6</v>
+        <v>9</v>
       </c>
     </row>
     <row r="8">
@@ -215,7 +209,7 @@
         <v>11</v>
       </c>
       <c r="C8" t="n">
-        <v>59.21373196414706</v>
+        <v>44.59050180027326</v>
       </c>
     </row>
     <row r="9">
@@ -226,7 +220,7 @@
         <v>11</v>
       </c>
       <c r="C9" t="n">
-        <v>101.08569681746206</v>
+        <v>51.279077070314244</v>
       </c>
     </row>
     <row r="10">
@@ -237,7 +231,7 @@
         <v>11</v>
       </c>
       <c r="C10" t="n">
-        <v>80.71397961603734</v>
+        <v>53.06269714232518</v>
       </c>
     </row>
     <row r="11">
@@ -248,61 +242,23 @@
         <v>11</v>
       </c>
       <c r="C11" t="n">
-        <v>137.57143687965652</v>
+        <v>54.84631721433611</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="s">
-        <v>15</v>
-      </c>
-      <c r="B12" t="s">
-        <v>16</v>
-      </c>
-      <c r="C12" t="n">
-        <v>0.2551270717382326</v>
+        <v>9</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="B13" t="s">
         <v>16</v>
       </c>
       <c r="C13" t="n">
-        <v>0.4346859458866881</v>
-      </c>
-    </row>
-    <row r="14">
-      <c r="A14" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="15">
-      <c r="A15" t="s">
-        <v>18</v>
-      </c>
-      <c r="B15" t="s">
-        <v>16</v>
-      </c>
-      <c r="C15" t="n">
-        <v>13.438117335104469</v>
-      </c>
-    </row>
-    <row r="16">
-      <c r="A16" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="17">
-      <c r="A17" t="s">
-        <v>19</v>
-      </c>
-      <c r="B17" t="s">
-        <v>20</v>
-      </c>
-      <c r="C17" t="n">
-        <v>0.17000002258703803</v>
+        <v>9.993589968918442</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
More test on ATR-72
</commit_message>
<xml_diff>
--- a/JPADSandBox_v2/out/ATR-72/PERFORMANCE/Performance.xlsx
+++ b/JPADSandBox_v2/out/ATR-72/PERFORMANCE/Performance.xlsx
@@ -12,13 +12,14 @@
     <sheet name="DESCENT" r:id="rId6" sheetId="4"/>
     <sheet name="LANDING" r:id="rId7" sheetId="5"/>
     <sheet name="MISSION PROFILE" r:id="rId8" sheetId="6"/>
-    <sheet name="V-n DIAGRAM" r:id="rId9" sheetId="7"/>
+    <sheet name="PAYLOAD-RANGE" r:id="rId9" sheetId="7"/>
+    <sheet name="V-n DIAGRAM" r:id="rId10" sheetId="8"/>
   </sheets>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="602" uniqueCount="224">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="806" uniqueCount="310">
   <si>
     <t>Description</t>
   </si>
@@ -548,6 +549,231 @@
     <t>Drag at second climb ending</t>
   </si>
   <si>
+    <t>SECOND CLIMB</t>
+  </si>
+  <si>
+    <t>Speed (TAS) at second climb start</t>
+  </si>
+  <si>
+    <t>Speed (TAS) at second climb ending</t>
+  </si>
+  <si>
+    <t>Mach at second climb start</t>
+  </si>
+  <si>
+    <t>Mach at second climb ending</t>
+  </si>
+  <si>
+    <t>CL at second climb start</t>
+  </si>
+  <si>
+    <t>CL at second climb ending</t>
+  </si>
+  <si>
+    <t>CD at second climb start</t>
+  </si>
+  <si>
+    <t>CD at second climb ending</t>
+  </si>
+  <si>
+    <t>Efficiency at second climb start</t>
+  </si>
+  <si>
+    <t>Efficiency at second climb ending</t>
+  </si>
+  <si>
+    <t>Thrust at second climb start</t>
+  </si>
+  <si>
+    <t>Thrust at second climb ending</t>
+  </si>
+  <si>
+    <t>Drag at first descent start</t>
+  </si>
+  <si>
+    <t>Drag at first descent ending</t>
+  </si>
+  <si>
+    <t>ALTERNATE CRUISE</t>
+  </si>
+  <si>
+    <t>Speed (TAS) at alternate cruise start</t>
+  </si>
+  <si>
+    <t>Speed (TAS) at alternate cruise ending</t>
+  </si>
+  <si>
+    <t>Mach at alternate cruise start</t>
+  </si>
+  <si>
+    <t>Mach at alternate cruise ending</t>
+  </si>
+  <si>
+    <t>CL at alternate cruise start</t>
+  </si>
+  <si>
+    <t>CL at alternate cruise ending</t>
+  </si>
+  <si>
+    <t>CD at alternate cruise start</t>
+  </si>
+  <si>
+    <t>CD at alternate cruise ending</t>
+  </si>
+  <si>
+    <t>Efficiency at alternate cruise start</t>
+  </si>
+  <si>
+    <t>Efficiency at alternate cruise ending</t>
+  </si>
+  <si>
+    <t>Thrust at alternate cruise start</t>
+  </si>
+  <si>
+    <t>Thrust at alternate cruise ending</t>
+  </si>
+  <si>
+    <t>Drag at alternate cruise start</t>
+  </si>
+  <si>
+    <t>Drag at alternate cruise ending</t>
+  </si>
+  <si>
+    <t>SECOND DESCENT</t>
+  </si>
+  <si>
+    <t>Speed (TAS) at second descent start</t>
+  </si>
+  <si>
+    <t>Speed (TAS) at second descent ending</t>
+  </si>
+  <si>
+    <t>Mach at second descent start</t>
+  </si>
+  <si>
+    <t>Mach at second descent ending</t>
+  </si>
+  <si>
+    <t>CL at second descent start</t>
+  </si>
+  <si>
+    <t>CL at second descent ending</t>
+  </si>
+  <si>
+    <t>CD at second descent start</t>
+  </si>
+  <si>
+    <t>CD at second descent ending</t>
+  </si>
+  <si>
+    <t>Efficiency at second descent start</t>
+  </si>
+  <si>
+    <t>Efficiency at second descent ending</t>
+  </si>
+  <si>
+    <t>Thrust at second descent start</t>
+  </si>
+  <si>
+    <t>Thrust at second descent ending</t>
+  </si>
+  <si>
+    <t>Drag at second descent start</t>
+  </si>
+  <si>
+    <t>Drag at second descent ending</t>
+  </si>
+  <si>
+    <t>HOLDING</t>
+  </si>
+  <si>
+    <t>Speed (TAS) at holding start</t>
+  </si>
+  <si>
+    <t>Speed (TAS) at holding ending</t>
+  </si>
+  <si>
+    <t>Mach at holding start</t>
+  </si>
+  <si>
+    <t>Mach at holding ending</t>
+  </si>
+  <si>
+    <t>CL at holding start</t>
+  </si>
+  <si>
+    <t>CL at holding ending</t>
+  </si>
+  <si>
+    <t>CD at holding start</t>
+  </si>
+  <si>
+    <t>CD at holding ending</t>
+  </si>
+  <si>
+    <t>Efficiency at holding start</t>
+  </si>
+  <si>
+    <t>Efficiency at holding ending</t>
+  </si>
+  <si>
+    <t>Thrust at holding start</t>
+  </si>
+  <si>
+    <t>Thrust at holding ending</t>
+  </si>
+  <si>
+    <t>Drag at holding start</t>
+  </si>
+  <si>
+    <t>Drag at holding ending</t>
+  </si>
+  <si>
+    <t>THIRD DESCENT</t>
+  </si>
+  <si>
+    <t>Speed (TAS) at third descent start</t>
+  </si>
+  <si>
+    <t>Speed (TAS) at third descent ending</t>
+  </si>
+  <si>
+    <t>Mach at third descent start</t>
+  </si>
+  <si>
+    <t>Mach at third descent ending</t>
+  </si>
+  <si>
+    <t>CL at third descent start</t>
+  </si>
+  <si>
+    <t>CL at third descent ending</t>
+  </si>
+  <si>
+    <t>CD at third descent start</t>
+  </si>
+  <si>
+    <t>CD at third descent ending</t>
+  </si>
+  <si>
+    <t>Efficiency at third descent start</t>
+  </si>
+  <si>
+    <t>Efficiency at third descent ending</t>
+  </si>
+  <si>
+    <t>Thrust at third descent start</t>
+  </si>
+  <si>
+    <t>Thrust at third descent ending</t>
+  </si>
+  <si>
+    <t>Drag at third descent start</t>
+  </si>
+  <si>
+    <t>Drag at third descent ending</t>
+  </si>
+  <si>
     <t>LANDING</t>
   </si>
   <si>
@@ -591,6 +817,39 @@
   </si>
   <si>
     <t>Drag at landing ending</t>
+  </si>
+  <si>
+    <t>ALTITUDE</t>
+  </si>
+  <si>
+    <t>MACH</t>
+  </si>
+  <si>
+    <t>RANGE AT MAX PAYLOAD</t>
+  </si>
+  <si>
+    <t>Range</t>
+  </si>
+  <si>
+    <t>Aircraft mass</t>
+  </si>
+  <si>
+    <t>Payload mass</t>
+  </si>
+  <si>
+    <t>Passengers number</t>
+  </si>
+  <si>
+    <t>Fuel mass</t>
+  </si>
+  <si>
+    <t>RANGE AT DESIGN PAYLOAD</t>
+  </si>
+  <si>
+    <t>RANGE AT MAX FUEL</t>
+  </si>
+  <si>
+    <t>RANGE AT ZERO PAYLOAD</t>
   </si>
   <si>
     <t>REGULATION</t>
@@ -776,7 +1035,7 @@
         <v>4</v>
       </c>
       <c r="C2" t="n">
-        <v>820.1901944347959</v>
+        <v>763.4976658579075</v>
       </c>
     </row>
     <row r="3">
@@ -787,7 +1046,7 @@
         <v>4</v>
       </c>
       <c r="C3" t="n">
-        <v>171.97099748369703</v>
+        <v>165.49835580099966</v>
       </c>
     </row>
     <row r="4">
@@ -798,7 +1057,7 @@
         <v>4</v>
       </c>
       <c r="C4" t="n">
-        <v>253.4315226066753</v>
+        <v>231.54652743043323</v>
       </c>
     </row>
     <row r="5">
@@ -809,7 +1068,7 @@
         <v>4</v>
       </c>
       <c r="C5" t="n">
-        <v>1245.592714525168</v>
+        <v>1160.5425490893404</v>
       </c>
     </row>
     <row r="6">
@@ -820,7 +1079,7 @@
         <v>4</v>
       </c>
       <c r="C6" t="n">
-        <v>1432.4316217039432</v>
+        <v>1334.623931452741</v>
       </c>
     </row>
     <row r="7">
@@ -831,7 +1090,7 @@
         <v>4</v>
       </c>
       <c r="C7" t="n">
-        <v>1289.124701462595</v>
+        <v>1225.6636069691126</v>
       </c>
     </row>
     <row r="8">
@@ -847,7 +1106,7 @@
         <v>11</v>
       </c>
       <c r="C9" t="n">
-        <v>2690.9127114002495</v>
+        <v>2504.913601896022</v>
       </c>
     </row>
     <row r="10">
@@ -858,7 +1117,7 @@
         <v>11</v>
       </c>
       <c r="C10" t="n">
-        <v>564.2093093297148</v>
+        <v>542.9736082709964</v>
       </c>
     </row>
     <row r="11">
@@ -869,7 +1128,7 @@
         <v>11</v>
       </c>
       <c r="C11" t="n">
-        <v>831.4682500219006</v>
+        <v>759.6670847455159</v>
       </c>
     </row>
     <row r="12">
@@ -880,7 +1139,7 @@
         <v>11</v>
       </c>
       <c r="C12" t="n">
-        <v>4086.5902707518644</v>
+        <v>3807.554294912534</v>
       </c>
     </row>
     <row r="13">
@@ -891,7 +1150,7 @@
         <v>11</v>
       </c>
       <c r="C13" t="n">
-        <v>4699.578811364643</v>
+        <v>4378.687439149413</v>
       </c>
     </row>
     <row r="14">
@@ -902,7 +1161,7 @@
         <v>11</v>
       </c>
       <c r="C14" t="n">
-        <v>4229.411750205365</v>
+        <v>4021.2060596099504</v>
       </c>
     </row>
     <row r="15">
@@ -918,7 +1177,7 @@
         <v>13</v>
       </c>
       <c r="C16" t="n">
-        <v>54.464737105769856</v>
+        <v>53.67149021492679</v>
       </c>
     </row>
     <row r="17">
@@ -929,7 +1188,7 @@
         <v>13</v>
       </c>
       <c r="C17" t="n">
-        <v>56.618247732075716</v>
+        <v>55.82318509291505</v>
       </c>
     </row>
     <row r="18">
@@ -940,7 +1199,7 @@
         <v>13</v>
       </c>
       <c r="C18" t="n">
-        <v>57.187973961058354</v>
+        <v>56.35506472567313</v>
       </c>
     </row>
     <row r="19">
@@ -951,7 +1210,7 @@
         <v>13</v>
       </c>
       <c r="C19" t="n">
-        <v>47.05934230489444</v>
+        <v>46.98027510783356</v>
       </c>
     </row>
     <row r="20">
@@ -962,7 +1221,7 @@
         <v>13</v>
       </c>
       <c r="C20" t="n">
-        <v>61.50624032441149</v>
+        <v>60.77409553733331</v>
       </c>
     </row>
     <row r="21">
@@ -973,7 +1232,7 @@
         <v>13</v>
       </c>
       <c r="C21" t="n">
-        <v>64.90358632965845</v>
+        <v>63.95159766929473</v>
       </c>
     </row>
     <row r="22">
@@ -989,7 +1248,7 @@
         <v>19</v>
       </c>
       <c r="C23" t="n">
-        <v>105.87097925527618</v>
+        <v>104.32903065536526</v>
       </c>
     </row>
     <row r="24">
@@ -1000,7 +1259,7 @@
         <v>19</v>
       </c>
       <c r="C24" t="n">
-        <v>110.05706902563315</v>
+        <v>108.51159089335539</v>
       </c>
     </row>
     <row r="25">
@@ -1011,7 +1270,7 @@
         <v>19</v>
       </c>
       <c r="C25" t="n">
-        <v>111.16452821804</v>
+        <v>109.54548218813352</v>
       </c>
     </row>
     <row r="26">
@@ -1022,7 +1281,7 @@
         <v>19</v>
       </c>
       <c r="C26" t="n">
-        <v>91.47604335724623</v>
+        <v>91.32234902170673</v>
       </c>
     </row>
     <row r="27">
@@ -1033,7 +1292,7 @@
         <v>19</v>
       </c>
       <c r="C27" t="n">
-        <v>119.5585665053355</v>
+        <v>118.13539089330449</v>
       </c>
     </row>
     <row r="28">
@@ -1044,7 +1303,7 @@
         <v>19</v>
       </c>
       <c r="C28" t="n">
-        <v>126.16247882654991</v>
+        <v>124.31196091223597</v>
       </c>
     </row>
     <row r="29">
@@ -1060,7 +1319,7 @@
         <v>21</v>
       </c>
       <c r="C30" t="n">
-        <v>1.0395395395395695</v>
+        <v>1.0400900900901355</v>
       </c>
     </row>
     <row r="31">
@@ -1082,7 +1341,7 @@
         <v>10</v>
       </c>
       <c r="C32" t="n">
-        <v>0.8640332223307305</v>
+        <v>0.8753301784560417</v>
       </c>
     </row>
     <row r="33">
@@ -1093,7 +1352,7 @@
         <v>21</v>
       </c>
       <c r="C33" t="n">
-        <v>1.1292855449750379</v>
+        <v>1.1323347888043394</v>
       </c>
     </row>
     <row r="34">
@@ -1104,7 +1363,7 @@
         <v>21</v>
       </c>
       <c r="C34" t="n">
-        <v>1.1916625284285587</v>
+        <v>1.1915375819303948</v>
       </c>
     </row>
     <row r="35">
@@ -1120,7 +1379,7 @@
         <v>27</v>
       </c>
       <c r="C36" t="n">
-        <v>33.27508147413059</v>
+        <v>31.518246828443218</v>
       </c>
     </row>
   </sheetData>
@@ -1155,7 +1414,7 @@
         <v>4</v>
       </c>
       <c r="C2" t="n">
-        <v>8389.713722230805</v>
+        <v>8634.888420929987</v>
       </c>
     </row>
     <row r="3">
@@ -1166,7 +1425,7 @@
         <v>11</v>
       </c>
       <c r="C3" t="n">
-        <v>27525.307487633865</v>
+        <v>28329.686420373968</v>
       </c>
     </row>
     <row r="4">
@@ -1177,7 +1436,7 @@
         <v>4</v>
       </c>
       <c r="C4" t="n">
-        <v>7887.1549137230795</v>
+        <v>8140.8101902966755</v>
       </c>
     </row>
     <row r="5">
@@ -1188,7 +1447,7 @@
         <v>11</v>
       </c>
       <c r="C5" t="n">
-        <v>25876.492499091466</v>
+        <v>26708.694850054708</v>
       </c>
     </row>
     <row r="6">
@@ -1199,7 +1458,7 @@
         <v>31</v>
       </c>
       <c r="C6" t="n">
-        <v>16.699590742048024</v>
+        <v>15.631361120702934</v>
       </c>
     </row>
     <row r="7">
@@ -1210,7 +1469,7 @@
         <v>31</v>
       </c>
       <c r="C7" t="n">
-        <v>16.872418183790067</v>
+        <v>15.785596169403902</v>
       </c>
     </row>
     <row r="8">
@@ -1221,7 +1480,7 @@
         <v>34</v>
       </c>
       <c r="C8" t="n">
-        <v>247.75473501228663</v>
+        <v>232.1515284295877</v>
       </c>
     </row>
     <row r="9">
@@ -1237,7 +1496,7 @@
         <v>4</v>
       </c>
       <c r="C10" t="n">
-        <v>4831.174938981165</v>
+        <v>5106.702253236044</v>
       </c>
     </row>
     <row r="11">
@@ -1248,7 +1507,7 @@
         <v>11</v>
       </c>
       <c r="C11" t="n">
-        <v>15850.311479596998</v>
+        <v>16754.27248437022</v>
       </c>
     </row>
     <row r="12">
@@ -1259,7 +1518,7 @@
         <v>4</v>
       </c>
       <c r="C12" t="n">
-        <v>4202.371836316846</v>
+        <v>4484.06741607492</v>
       </c>
     </row>
     <row r="13">
@@ -1270,7 +1529,7 @@
         <v>11</v>
       </c>
       <c r="C13" t="n">
-        <v>13787.309174267866</v>
+        <v>14711.507270587008</v>
       </c>
     </row>
   </sheetData>
@@ -1327,7 +1586,7 @@
         <v>38</v>
       </c>
       <c r="C4" t="n">
-        <v>15954.254589964348</v>
+        <v>15739.665100655897</v>
       </c>
     </row>
     <row r="5">
@@ -1338,7 +1597,7 @@
         <v>39</v>
       </c>
       <c r="C5" t="n">
-        <v>3586.65911231359</v>
+        <v>3538.4174760218502</v>
       </c>
     </row>
     <row r="6">
@@ -1376,7 +1635,7 @@
         <v>42</v>
       </c>
       <c r="C9" t="n">
-        <v>2142950.30043518</v>
+        <v>2114126.978857182</v>
       </c>
     </row>
     <row r="10">
@@ -1387,7 +1646,7 @@
         <v>43</v>
       </c>
       <c r="C10" t="n">
-        <v>2913.6005629309884</v>
+        <v>2874.4117651515253</v>
       </c>
     </row>
     <row r="11">
@@ -1403,7 +1662,7 @@
         <v>13</v>
       </c>
       <c r="C12" t="n">
-        <v>62.05954013778687</v>
+        <v>61.15567940371504</v>
       </c>
     </row>
     <row r="13">
@@ -1414,7 +1673,7 @@
         <v>13</v>
       </c>
       <c r="C13" t="n">
-        <v>107.49162397919065</v>
+        <v>108.10352611901291</v>
       </c>
     </row>
     <row r="14">
@@ -1425,7 +1684,7 @@
         <v>19</v>
       </c>
       <c r="C14" t="n">
-        <v>120.63409530023365</v>
+        <v>118.87713059037479</v>
       </c>
     </row>
     <row r="15">
@@ -1436,7 +1695,7 @@
         <v>19</v>
       </c>
       <c r="C15" t="n">
-        <v>208.94700125544614</v>
+        <v>210.1364438598523</v>
       </c>
     </row>
     <row r="16">
@@ -1452,7 +1711,7 @@
         <v>13</v>
       </c>
       <c r="C17" t="n">
-        <v>80.8318141519373</v>
+        <v>79.65454627799696</v>
       </c>
     </row>
     <row r="18">
@@ -1463,7 +1722,7 @@
         <v>13</v>
       </c>
       <c r="C18" t="n">
-        <v>140.00574111161944</v>
+        <v>140.80272224893366</v>
       </c>
     </row>
     <row r="19">
@@ -1474,7 +1733,7 @@
         <v>19</v>
       </c>
       <c r="C19" t="n">
-        <v>157.1244767532258</v>
+        <v>154.83605108033964</v>
       </c>
     </row>
     <row r="20">
@@ -1485,7 +1744,7 @@
         <v>19</v>
       </c>
       <c r="C20" t="n">
-        <v>272.14938876988657</v>
+        <v>273.69859616423383</v>
       </c>
     </row>
     <row r="21">
@@ -1501,7 +1760,7 @@
         <v>21</v>
       </c>
       <c r="C22" t="n">
-        <v>0.25275318816835946</v>
+        <v>0.24907198650799223</v>
       </c>
     </row>
     <row r="23">
@@ -1512,7 +1771,7 @@
         <v>21</v>
       </c>
       <c r="C23" t="n">
-        <v>0.43778367512164784</v>
+        <v>0.4402757469356548</v>
       </c>
     </row>
     <row r="24">
@@ -1528,7 +1787,7 @@
         <v>21</v>
       </c>
       <c r="C25" t="n">
-        <v>13.554284070670356</v>
+        <v>13.343608894007511</v>
       </c>
     </row>
     <row r="26">
@@ -1601,7 +1860,7 @@
         <v>34</v>
       </c>
       <c r="C5" t="n">
-        <v>75.33649432078079</v>
+        <v>76.87260908157373</v>
       </c>
     </row>
   </sheetData>
@@ -1636,7 +1895,7 @@
         <v>4</v>
       </c>
       <c r="C2" t="n">
-        <v>374.25537032206677</v>
+        <v>363.4072353153997</v>
       </c>
     </row>
     <row r="3">
@@ -1647,7 +1906,7 @@
         <v>4</v>
       </c>
       <c r="C3" t="n">
-        <v>88.67725815729722</v>
+        <v>86.1130042528782</v>
       </c>
     </row>
     <row r="4">
@@ -1658,7 +1917,7 @@
         <v>4</v>
       </c>
       <c r="C4" t="n">
-        <v>246.48829715062072</v>
+        <v>247.76954494518867</v>
       </c>
     </row>
     <row r="5">
@@ -1669,7 +1928,7 @@
         <v>4</v>
       </c>
       <c r="C5" t="n">
-        <v>709.4209256299848</v>
+        <v>697.2897845134667</v>
       </c>
     </row>
     <row r="6">
@@ -1680,7 +1939,7 @@
         <v>4</v>
       </c>
       <c r="C6" t="n">
-        <v>1182.3682093833079</v>
+        <v>1162.1496408557775</v>
       </c>
     </row>
     <row r="7">
@@ -1696,7 +1955,7 @@
         <v>11</v>
       </c>
       <c r="C8" t="n">
-        <v>1227.871949875547</v>
+        <v>1192.2809557591854</v>
       </c>
     </row>
     <row r="9">
@@ -1707,7 +1966,7 @@
         <v>11</v>
       </c>
       <c r="C9" t="n">
-        <v>290.9358863428386</v>
+        <v>282.52297983227754</v>
       </c>
     </row>
     <row r="10">
@@ -1718,7 +1977,7 @@
         <v>11</v>
       </c>
       <c r="C10" t="n">
-        <v>808.688638945606</v>
+        <v>812.892207825422</v>
       </c>
     </row>
     <row r="11">
@@ -1729,7 +1988,7 @@
         <v>11</v>
       </c>
       <c r="C11" t="n">
-        <v>2327.496475163992</v>
+        <v>2287.6961434168848</v>
       </c>
     </row>
     <row r="12">
@@ -1740,7 +1999,7 @@
         <v>11</v>
       </c>
       <c r="C12" t="n">
-        <v>3879.1607919399858</v>
+        <v>3812.8269056948084</v>
       </c>
     </row>
     <row r="13">
@@ -1756,7 +2015,7 @@
         <v>13</v>
       </c>
       <c r="C14" t="n">
-        <v>46.8679837441297</v>
+        <v>46.185379101920276</v>
       </c>
     </row>
     <row r="15">
@@ -1767,7 +2026,7 @@
         <v>13</v>
       </c>
       <c r="C15" t="n">
-        <v>53.898181305749155</v>
+        <v>53.11318596720832</v>
       </c>
     </row>
     <row r="16">
@@ -1778,7 +2037,7 @@
         <v>13</v>
       </c>
       <c r="C16" t="n">
-        <v>57.647620005279535</v>
+        <v>56.80801629536194</v>
       </c>
     </row>
     <row r="17">
@@ -1789,7 +2048,7 @@
         <v>13</v>
       </c>
       <c r="C17" t="n">
-        <v>60.928378867368615</v>
+        <v>60.04099283249636</v>
       </c>
     </row>
     <row r="18">
@@ -1805,7 +2064,7 @@
         <v>19</v>
       </c>
       <c r="C19" t="n">
-        <v>91.10407207282232</v>
+        <v>89.77719479854913</v>
       </c>
     </row>
     <row r="20">
@@ -1816,7 +2075,7 @@
         <v>19</v>
       </c>
       <c r="C20" t="n">
-        <v>104.76968288374565</v>
+        <v>103.2437740183315</v>
       </c>
     </row>
     <row r="21">
@@ -1827,7 +2086,7 @@
         <v>19</v>
       </c>
       <c r="C21" t="n">
-        <v>112.05800864957143</v>
+        <v>110.42594960221543</v>
       </c>
     </row>
     <row r="22">
@@ -1838,7 +2097,7 @@
         <v>19</v>
       </c>
       <c r="C22" t="n">
-        <v>118.43529369466901</v>
+        <v>116.71035323811387</v>
       </c>
     </row>
     <row r="23">
@@ -1892,7 +2151,7 @@
         <v>27</v>
       </c>
       <c r="C28" t="n">
-        <v>10.696275141356615</v>
+        <v>10.533536117807454</v>
       </c>
     </row>
   </sheetData>
@@ -1927,7 +2186,7 @@
         <v>53</v>
       </c>
       <c r="C2" t="n">
-        <v>889.9999999999999</v>
+        <v>286.99999999999994</v>
       </c>
     </row>
     <row r="3">
@@ -1938,7 +2197,7 @@
         <v>31</v>
       </c>
       <c r="C3" t="n">
-        <v>199.41438104166684</v>
+        <v>115.16083257114227</v>
       </c>
     </row>
     <row r="4">
@@ -1949,7 +2208,7 @@
         <v>34</v>
       </c>
       <c r="C4" t="n">
-        <v>22242.00184937041</v>
+        <v>21244.515966406383</v>
       </c>
     </row>
     <row r="5">
@@ -1960,7 +2219,7 @@
         <v>34</v>
       </c>
       <c r="C5" t="n">
-        <v>19796.537599805306</v>
+        <v>19945.927592720553</v>
       </c>
     </row>
     <row r="6">
@@ -1971,7 +2230,7 @@
         <v>34</v>
       </c>
       <c r="C6" t="n">
-        <v>2574.001849370414</v>
+        <v>1358.5159664063879</v>
       </c>
     </row>
     <row r="7">
@@ -1982,7 +2241,7 @@
         <v>34</v>
       </c>
       <c r="C7" t="n">
-        <v>2445.301756901894</v>
+        <v>1290.5901680860684</v>
       </c>
     </row>
     <row r="8">
@@ -2031,7 +2290,7 @@
         <v>53</v>
       </c>
       <c r="C12" t="n">
-        <v>0.6128038427281226</v>
+        <v>0.5595260658355462</v>
       </c>
     </row>
     <row r="13">
@@ -2042,7 +2301,7 @@
         <v>53</v>
       </c>
       <c r="C13" t="n">
-        <v>50.43989981482256</v>
+        <v>45.7661957495705</v>
       </c>
     </row>
     <row r="14">
@@ -2053,7 +2312,7 @@
         <v>53</v>
       </c>
       <c r="C14" t="n">
-        <v>789.7656068200988</v>
+        <v>64.01835514932378</v>
       </c>
     </row>
     <row r="15">
@@ -2064,7 +2323,7 @@
         <v>53</v>
       </c>
       <c r="C15" t="n">
-        <v>48.821550358305274</v>
+        <v>45.00256920306859</v>
       </c>
     </row>
     <row r="16">
@@ -2075,7 +2334,7 @@
         <v>53</v>
       </c>
       <c r="C16" t="n">
-        <v>5.3953499445924535E-8</v>
+        <v>17.71563392149615</v>
       </c>
     </row>
     <row r="17">
@@ -2086,7 +2345,7 @@
         <v>53</v>
       </c>
       <c r="C17" t="n">
-        <v>-5.6843418860808015E-14</v>
+        <v>86.99999999999994</v>
       </c>
     </row>
     <row r="18">
@@ -2097,7 +2356,7 @@
         <v>53</v>
       </c>
       <c r="C18" t="n">
-        <v>-5.6843418860808015E-14</v>
+        <v>22.989883486825306</v>
       </c>
     </row>
     <row r="19">
@@ -2119,7 +2378,7 @@
         <v>53</v>
       </c>
       <c r="C20" t="n">
-        <v>-5.6843418860808015E-14</v>
+        <v>3.586709101989584</v>
       </c>
     </row>
     <row r="21">
@@ -2130,7 +2389,7 @@
         <v>53</v>
       </c>
       <c r="C21" t="n">
-        <v>0.36013875031244424</v>
+        <v>0.3616593451248207</v>
       </c>
     </row>
     <row r="22">
@@ -2146,7 +2405,7 @@
         <v>31</v>
       </c>
       <c r="C23" t="n">
-        <v>0.5158269566862803</v>
+        <v>0.47922495840064394</v>
       </c>
     </row>
     <row r="24">
@@ -2157,7 +2416,7 @@
         <v>31</v>
       </c>
       <c r="C24" t="n">
-        <v>15.379457794237194</v>
+        <v>13.980450417403423</v>
       </c>
     </row>
     <row r="25">
@@ -2168,7 +2427,7 @@
         <v>31</v>
       </c>
       <c r="C25" t="n">
-        <v>172.05053230244113</v>
+        <v>13.96627293034787</v>
       </c>
     </row>
     <row r="26">
@@ -2179,7 +2438,7 @@
         <v>31</v>
       </c>
       <c r="C26" t="n">
-        <v>11.299999999999969</v>
+        <v>10.333333333333325</v>
       </c>
     </row>
     <row r="27">
@@ -2190,7 +2449,7 @@
         <v>31</v>
       </c>
       <c r="C27" t="n">
-        <v>1.9176084720129438E-8</v>
+        <v>5.74426203717395</v>
       </c>
     </row>
     <row r="28">
@@ -2201,7 +2460,7 @@
         <v>31</v>
       </c>
       <c r="C28" t="n">
-        <v>-1.4210854715202004E-14</v>
+        <v>18.85473410788719</v>
       </c>
     </row>
     <row r="29">
@@ -2212,7 +2471,7 @@
         <v>31</v>
       </c>
       <c r="C29" t="n">
-        <v>-1.4210854715202004E-14</v>
+        <v>5.666666666666654</v>
       </c>
     </row>
     <row r="30">
@@ -2223,7 +2482,7 @@
         <v>31</v>
       </c>
       <c r="C30" t="n">
-        <v>-1.4210854715202004E-14</v>
+        <v>44.999999999999986</v>
       </c>
     </row>
     <row r="31">
@@ -2234,7 +2493,7 @@
         <v>31</v>
       </c>
       <c r="C31" t="n">
-        <v>-1.4210854715202004E-14</v>
+        <v>0.9666666666666615</v>
       </c>
     </row>
     <row r="32">
@@ -2245,7 +2504,7 @@
         <v>31</v>
       </c>
       <c r="C32" t="n">
-        <v>0.1685639691262253</v>
+        <v>0.16922145326255844</v>
       </c>
     </row>
     <row r="33">
@@ -2261,7 +2520,7 @@
         <v>34</v>
       </c>
       <c r="C34" t="n">
-        <v>9.552727462798055</v>
+        <v>8.873414888612675</v>
       </c>
     </row>
     <row r="35">
@@ -2272,7 +2531,7 @@
         <v>34</v>
       </c>
       <c r="C35" t="n">
-        <v>226.3065221492838</v>
+        <v>206.11321983985948</v>
       </c>
     </row>
     <row r="36">
@@ -2283,7 +2542,7 @@
         <v>34</v>
       </c>
       <c r="C36" t="n">
-        <v>2131.9761732948164</v>
+        <v>173.27197602177455</v>
       </c>
     </row>
     <row r="37">
@@ -2294,7 +2553,7 @@
         <v>34</v>
       </c>
       <c r="C37" t="n">
-        <v>77.0196391472698</v>
+        <v>69.82229920984113</v>
       </c>
     </row>
     <row r="38">
@@ -2305,7 +2564,7 @@
         <v>34</v>
       </c>
       <c r="C38" t="n">
-        <v>3.295419901405694E-7</v>
+        <v>91.60531214164246</v>
       </c>
     </row>
     <row r="39">
@@ -2316,7 +2575,7 @@
         <v>34</v>
       </c>
       <c r="C39" t="n">
-        <v>-2.2737367544323206E-13</v>
+        <v>259.44383659097946</v>
       </c>
     </row>
     <row r="40">
@@ -2327,7 +2586,7 @@
         <v>34</v>
       </c>
       <c r="C40" t="n">
-        <v>-2.2737367544323206E-13</v>
+        <v>39.25435552926234</v>
       </c>
     </row>
     <row r="41">
@@ -2338,7 +2597,7 @@
         <v>34</v>
       </c>
       <c r="C41" t="n">
-        <v>-2.2737367544323206E-13</v>
+        <v>434.99500801305953</v>
       </c>
     </row>
     <row r="42">
@@ -2349,7 +2608,7 @@
         <v>34</v>
       </c>
       <c r="C42" t="n">
-        <v>-2.2737367544323206E-13</v>
+        <v>6.762308999891161</v>
       </c>
     </row>
     <row r="43">
@@ -2360,7 +2619,7 @@
         <v>34</v>
       </c>
       <c r="C43" t="n">
-        <v>0.4466945181841311</v>
+        <v>0.4484368511456296</v>
       </c>
     </row>
     <row r="44">
@@ -2376,7 +2635,7 @@
         <v>34</v>
       </c>
       <c r="C45" t="n">
-        <v>22232.28662924442</v>
+        <v>21227.644345918023</v>
       </c>
     </row>
     <row r="46">
@@ -2387,7 +2646,7 @@
         <v>34</v>
       </c>
       <c r="C46" t="n">
-        <v>22005.980107095136</v>
+        <v>21021.531126078164</v>
       </c>
     </row>
     <row r="47">
@@ -2398,7 +2657,7 @@
         <v>34</v>
       </c>
       <c r="C47" t="n">
-        <v>19874.003933800315</v>
+        <v>20848.259150056387</v>
       </c>
     </row>
     <row r="48">
@@ -2409,7 +2668,7 @@
         <v>34</v>
       </c>
       <c r="C48" t="n">
-        <v>19796.98429465304</v>
+        <v>20778.436850846545</v>
       </c>
     </row>
     <row r="49">
@@ -2420,7 +2679,7 @@
         <v>34</v>
       </c>
       <c r="C49" t="n">
-        <v>19796.984294323498</v>
+        <v>20686.8315387049</v>
       </c>
     </row>
     <row r="50">
@@ -2431,7 +2690,7 @@
         <v>34</v>
       </c>
       <c r="C50" t="n">
-        <v>19796.984294323498</v>
+        <v>20427.38770211392</v>
       </c>
     </row>
     <row r="51">
@@ -2442,7 +2701,7 @@
         <v>34</v>
       </c>
       <c r="C51" t="n">
-        <v>19796.984294323494</v>
+        <v>20388.133346584655</v>
       </c>
     </row>
     <row r="52">
@@ -2453,7 +2712,7 @@
         <v>34</v>
       </c>
       <c r="C52" t="n">
-        <v>19796.98429432349</v>
+        <v>19953.138338571596</v>
       </c>
     </row>
     <row r="53">
@@ -2464,7 +2723,7 @@
         <v>34</v>
       </c>
       <c r="C53" t="n">
-        <v>19796.98429432349</v>
+        <v>19946.3760295717</v>
       </c>
     </row>
     <row r="54">
@@ -2475,7 +2734,7 @@
         <v>34</v>
       </c>
       <c r="C54" t="n">
-        <v>19796.537599805306</v>
+        <v>19945.927592720553</v>
       </c>
     </row>
     <row r="55">
@@ -2507,7 +2766,7 @@
         <v>19</v>
       </c>
       <c r="C58" t="n">
-        <v>123.89567374302489</v>
+        <v>122.10051401488093</v>
       </c>
     </row>
     <row r="59">
@@ -2529,7 +2788,7 @@
         <v>10</v>
       </c>
       <c r="C60" t="n">
-        <v>0.18732366366290265</v>
+        <v>0.18460947771131322</v>
       </c>
     </row>
     <row r="61">
@@ -2551,7 +2810,7 @@
         <v>10</v>
       </c>
       <c r="C62" t="n">
-        <v>1.744269853155924</v>
+        <v>1.744193767604694</v>
       </c>
     </row>
     <row r="63">
@@ -2573,7 +2832,7 @@
         <v>10</v>
       </c>
       <c r="C64" t="n">
-        <v>0.10506502500286752</v>
+        <v>0.10506119205958955</v>
       </c>
     </row>
     <row r="65">
@@ -2595,7 +2854,7 @@
         <v>10</v>
       </c>
       <c r="C66" t="n">
-        <v>16.601812573768655</v>
+        <v>16.601694054788627</v>
       </c>
     </row>
     <row r="67">
@@ -2606,7 +2865,7 @@
         <v>127</v>
       </c>
       <c r="C67" t="n">
-        <v>15377.592657289946</v>
+        <v>15377.591973895382</v>
       </c>
     </row>
     <row r="68">
@@ -2617,7 +2876,7 @@
         <v>127</v>
       </c>
       <c r="C68" t="n">
-        <v>10211.893754387842</v>
+        <v>10301.87436748788</v>
       </c>
     </row>
     <row r="69">
@@ -2639,7 +2898,7 @@
         <v>127</v>
       </c>
       <c r="C70" t="n">
-        <v>3585.2795467772175</v>
+        <v>3482.008929775164</v>
       </c>
     </row>
     <row r="71">
@@ -2704,7 +2963,7 @@
         <v>10</v>
       </c>
       <c r="C77" t="n">
-        <v>0.7629006372652537</v>
+        <v>0.7284263498941497</v>
       </c>
     </row>
     <row r="78">
@@ -2715,7 +2974,7 @@
         <v>10</v>
       </c>
       <c r="C78" t="n">
-        <v>1.2810597242180017</v>
+        <v>1.223750850266885</v>
       </c>
     </row>
     <row r="79">
@@ -2726,7 +2985,7 @@
         <v>10</v>
       </c>
       <c r="C79" t="n">
-        <v>0.04920264659647413</v>
+        <v>0.0475598885442971</v>
       </c>
     </row>
     <row r="80">
@@ -2737,7 +2996,7 @@
         <v>10</v>
       </c>
       <c r="C80" t="n">
-        <v>0.08304200242216361</v>
+        <v>0.07844878633588735</v>
       </c>
     </row>
     <row r="81">
@@ -2748,7 +3007,7 @@
         <v>10</v>
       </c>
       <c r="C81" t="n">
-        <v>15.50527644421313</v>
+        <v>15.315981012354477</v>
       </c>
     </row>
     <row r="82">
@@ -2759,7 +3018,7 @@
         <v>10</v>
       </c>
       <c r="C82" t="n">
-        <v>15.426647802944736</v>
+        <v>15.599359880817753</v>
       </c>
     </row>
     <row r="83">
@@ -2770,7 +3029,7 @@
         <v>127</v>
       </c>
       <c r="C83" t="n">
-        <v>7251.752393790313</v>
+        <v>7251.752393790312</v>
       </c>
     </row>
     <row r="84">
@@ -2792,7 +3051,7 @@
         <v>127</v>
       </c>
       <c r="C85" t="n">
-        <v>3161.195314538425</v>
+        <v>3055.5642363365964</v>
       </c>
     </row>
     <row r="86">
@@ -2803,7 +3062,7 @@
         <v>127</v>
       </c>
       <c r="C86" t="n">
-        <v>3185.8992853351724</v>
+        <v>3006.9181577574936</v>
       </c>
     </row>
     <row r="87">
@@ -2824,7 +3083,7 @@
         <v>19</v>
       </c>
       <c r="C89" t="n">
-        <v>271.96258280390896</v>
+        <v>274.9099468658059</v>
       </c>
     </row>
     <row r="90">
@@ -2835,7 +3094,7 @@
         <v>19</v>
       </c>
       <c r="C90" t="n">
-        <v>279.8678110221731</v>
+        <v>275.37851812423855</v>
       </c>
     </row>
     <row r="91">
@@ -2846,7 +3105,7 @@
         <v>10</v>
       </c>
       <c r="C91" t="n">
-        <v>0.4374831676628926</v>
+        <v>0.44222434254349796</v>
       </c>
     </row>
     <row r="92">
@@ -2857,7 +3116,7 @@
         <v>10</v>
       </c>
       <c r="C92" t="n">
-        <v>0.4501996386066835</v>
+        <v>0.4429780934319527</v>
       </c>
     </row>
     <row r="93">
@@ -2868,7 +3127,7 @@
         <v>10</v>
       </c>
       <c r="C93" t="n">
-        <v>0.500551660297655</v>
+        <v>0.4679613029799353</v>
       </c>
     </row>
     <row r="94">
@@ -2879,7 +3138,7 @@
         <v>10</v>
       </c>
       <c r="C94" t="n">
-        <v>0.4030830105612305</v>
+        <v>0.46059706677249074</v>
       </c>
     </row>
     <row r="95">
@@ -2890,7 +3149,7 @@
         <v>10</v>
       </c>
       <c r="C95" t="n">
-        <v>0.03861113678372894</v>
+        <v>0.03760395098579889</v>
       </c>
     </row>
     <row r="96">
@@ -2901,7 +3160,7 @@
         <v>10</v>
       </c>
       <c r="C96" t="n">
-        <v>0.035800210390200975</v>
+        <v>0.037379706993218506</v>
       </c>
     </row>
     <row r="97">
@@ -2912,7 +3171,7 @@
         <v>10</v>
       </c>
       <c r="C97" t="n">
-        <v>12.963919272860975</v>
+        <v>12.444471676836846</v>
       </c>
     </row>
     <row r="98">
@@ -2923,7 +3182,7 @@
         <v>10</v>
       </c>
       <c r="C98" t="n">
-        <v>11.2592358024678</v>
+        <v>12.322115495877297</v>
       </c>
     </row>
     <row r="99">
@@ -2934,7 +3193,7 @@
         <v>127</v>
       </c>
       <c r="C99" t="n">
-        <v>3742.300498709402</v>
+        <v>3724.10691831234</v>
       </c>
     </row>
     <row r="100">
@@ -2945,7 +3204,7 @@
         <v>127</v>
       </c>
       <c r="C100" t="n">
-        <v>3674.5083292307663</v>
+        <v>3714.529101451155</v>
       </c>
     </row>
     <row r="101">
@@ -2956,7 +3215,7 @@
         <v>127</v>
       </c>
       <c r="C101" t="n">
-        <v>3742.300498709402</v>
+        <v>3724.10691831234</v>
       </c>
     </row>
     <row r="102">
@@ -2967,7 +3226,7 @@
         <v>127</v>
       </c>
       <c r="C102" t="n">
-        <v>3674.5083292307663</v>
+        <v>3714.529101451155</v>
       </c>
     </row>
     <row r="103">
@@ -2999,7 +3258,7 @@
         <v>19</v>
       </c>
       <c r="C106" t="n">
-        <v>234.4604898955982</v>
+        <v>238.34927482104573</v>
       </c>
     </row>
     <row r="107">
@@ -3021,7 +3280,7 @@
         <v>10</v>
       </c>
       <c r="C108" t="n">
-        <v>0.35451006603783813</v>
+        <v>0.3622005138224198</v>
       </c>
     </row>
     <row r="109">
@@ -3032,7 +3291,7 @@
         <v>10</v>
       </c>
       <c r="C109" t="n">
-        <v>0.40666872142055804</v>
+        <v>0.4266042675969548</v>
       </c>
     </row>
     <row r="110">
@@ -3043,7 +3302,7 @@
         <v>10</v>
       </c>
       <c r="C110" t="n">
-        <v>0.4038747831942766</v>
+        <v>0.4240691085739158</v>
       </c>
     </row>
     <row r="111">
@@ -3054,7 +3313,7 @@
         <v>10</v>
       </c>
       <c r="C111" t="n">
-        <v>0.03589349809087134</v>
+        <v>0.036416839198585446</v>
       </c>
     </row>
     <row r="112">
@@ -3065,7 +3324,7 @@
         <v>10</v>
       </c>
       <c r="C112" t="n">
-        <v>0.035820809554854324</v>
+        <v>0.03634619552577141</v>
       </c>
     </row>
     <row r="113">
@@ -3076,7 +3335,7 @@
         <v>10</v>
       </c>
       <c r="C113" t="n">
-        <v>11.329871510182636</v>
+        <v>11.714478164088595</v>
       </c>
     </row>
     <row r="114">
@@ -3087,7 +3346,7 @@
         <v>10</v>
       </c>
       <c r="C114" t="n">
-        <v>11.274864756359053</v>
+        <v>11.667496485931462</v>
       </c>
     </row>
     <row r="115">
@@ -3098,7 +3357,7 @@
         <v>127</v>
       </c>
       <c r="C115" t="n">
-        <v>1597.4725804410991</v>
+        <v>1544.7060950880432</v>
       </c>
     </row>
     <row r="116">
@@ -3109,7 +3368,7 @@
         <v>127</v>
       </c>
       <c r="C116" t="n">
-        <v>1105.2541827082787</v>
+        <v>1092.4254312491216</v>
       </c>
     </row>
     <row r="117">
@@ -3120,7 +3379,7 @@
         <v>127</v>
       </c>
       <c r="C117" t="n">
-        <v>3862.012220316379</v>
+        <v>3918.32185467603</v>
       </c>
     </row>
     <row r="118">
@@ -3131,7 +3390,7 @@
         <v>127</v>
       </c>
       <c r="C118" t="n">
-        <v>3854.191193408835</v>
+        <v>3910.7208477470003</v>
       </c>
     </row>
     <row r="119">
@@ -3152,7 +3411,7 @@
         <v>19</v>
       </c>
       <c r="C121" t="n">
-        <v>112.31967575827062</v>
+        <v>173.79162760888562</v>
       </c>
     </row>
     <row r="122">
@@ -3163,7 +3422,7 @@
         <v>19</v>
       </c>
       <c r="C122" t="n">
-        <v>0.0</v>
+        <v>197.80949693813608</v>
       </c>
     </row>
     <row r="123">
@@ -3174,7 +3433,7 @@
         <v>10</v>
       </c>
       <c r="C123" t="n">
-        <v>0.16983013081710976</v>
+        <v>0.26409737082369705</v>
       </c>
     </row>
     <row r="124">
@@ -3185,7 +3444,7 @@
         <v>10</v>
       </c>
       <c r="C124" t="n">
-        <v>0.0</v>
+        <v>0.3098788369360525</v>
       </c>
     </row>
     <row r="125">
@@ -3196,7 +3455,7 @@
         <v>10</v>
       </c>
       <c r="C125" t="n">
-        <v>1.558491941001957</v>
+        <v>0.7130118234530495</v>
       </c>
     </row>
     <row r="126">
@@ -3207,7 +3466,7 @@
         <v>10</v>
       </c>
       <c r="C126" t="n">
-        <v>1.4387</v>
+        <v>0.9196327151349645</v>
       </c>
     </row>
     <row r="127">
@@ -3218,7 +3477,7 @@
         <v>10</v>
       </c>
       <c r="C127" t="n">
-        <v>0.20344099009247918</v>
+        <v>0.04685129770945638</v>
       </c>
     </row>
     <row r="128">
@@ -3229,7 +3488,7 @@
         <v>10</v>
       </c>
       <c r="C128" t="n">
-        <v>0.19153799598718918</v>
+        <v>0.05762859327321252</v>
       </c>
     </row>
     <row r="129">
@@ -3240,7 +3499,7 @@
         <v>10</v>
       </c>
       <c r="C129" t="n">
-        <v>7.660658455768947</v>
+        <v>15.218614175315286</v>
       </c>
     </row>
     <row r="130">
@@ -3251,7 +3510,7 @@
         <v>10</v>
       </c>
       <c r="C130" t="n">
-        <v>7.511303397453454</v>
+        <v>15.957924059937744</v>
       </c>
     </row>
     <row r="131">
@@ -3262,7 +3521,7 @@
         <v>127</v>
       </c>
       <c r="C131" t="n">
-        <v>-651.5472391333013</v>
+        <v>7199.414490810044</v>
       </c>
     </row>
     <row r="132">
@@ -3273,7 +3532,7 @@
         <v>127</v>
       </c>
       <c r="C132" t="n">
-        <v>49.50742544941821</v>
+        <v>6274.189210039074</v>
       </c>
     </row>
     <row r="133">
@@ -3284,7 +3543,7 @@
         <v>127</v>
       </c>
       <c r="C133" t="n">
-        <v>3349.2242670285573</v>
+        <v>2972.1749957884977</v>
       </c>
     </row>
     <row r="134">
@@ -3295,6 +3554,826 @@
         <v>127</v>
       </c>
       <c r="C134" t="n">
+        <v>2865.3751901435826</v>
+      </c>
+    </row>
+    <row r="135">
+      <c r="A135" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="136">
+      <c r="A136" t="s">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="137">
+      <c r="A137" t="s">
+        <v>192</v>
+      </c>
+      <c r="B137" t="s">
+        <v>19</v>
+      </c>
+      <c r="C137" t="n">
+        <v>276.3512340638369</v>
+      </c>
+    </row>
+    <row r="138">
+      <c r="A138" t="s">
+        <v>193</v>
+      </c>
+      <c r="B138" t="s">
+        <v>19</v>
+      </c>
+      <c r="C138" t="n">
+        <v>276.3512340638369</v>
+      </c>
+    </row>
+    <row r="139">
+      <c r="A139" t="s">
+        <v>194</v>
+      </c>
+      <c r="B139" t="s">
+        <v>10</v>
+      </c>
+      <c r="C139" t="n">
+        <v>0.4329185419460757</v>
+      </c>
+    </row>
+    <row r="140">
+      <c r="A140" t="s">
+        <v>195</v>
+      </c>
+      <c r="B140" t="s">
+        <v>10</v>
+      </c>
+      <c r="C140" t="n">
+        <v>0.4329185419460757</v>
+      </c>
+    </row>
+    <row r="141">
+      <c r="A141" t="s">
+        <v>196</v>
+      </c>
+      <c r="B141" t="s">
+        <v>10</v>
+      </c>
+      <c r="C141" t="n">
+        <v>0.36370502134069727</v>
+      </c>
+    </row>
+    <row r="142">
+      <c r="A142" t="s">
+        <v>197</v>
+      </c>
+      <c r="B142" t="s">
+        <v>10</v>
+      </c>
+      <c r="C142" t="n">
+        <v>0.3542744415142043</v>
+      </c>
+    </row>
+    <row r="143">
+      <c r="A143" t="s">
+        <v>198</v>
+      </c>
+      <c r="B143" t="s">
+        <v>10</v>
+      </c>
+      <c r="C143" t="n">
+        <v>0.03483357445319331</v>
+      </c>
+    </row>
+    <row r="144">
+      <c r="A144" t="s">
+        <v>199</v>
+      </c>
+      <c r="B144" t="s">
+        <v>10</v>
+      </c>
+      <c r="C144" t="n">
+        <v>0.034610965461557945</v>
+      </c>
+    </row>
+    <row r="145">
+      <c r="A145" t="s">
+        <v>200</v>
+      </c>
+      <c r="B145" t="s">
+        <v>10</v>
+      </c>
+      <c r="C145" t="n">
+        <v>10.441220203496952</v>
+      </c>
+    </row>
+    <row r="146">
+      <c r="A146" t="s">
+        <v>201</v>
+      </c>
+      <c r="B146" t="s">
+        <v>10</v>
+      </c>
+      <c r="C146" t="n">
+        <v>10.235901737779994</v>
+      </c>
+    </row>
+    <row r="147">
+      <c r="A147" t="s">
+        <v>202</v>
+      </c>
+      <c r="B147" t="s">
+        <v>127</v>
+      </c>
+      <c r="C147" t="n">
+        <v>4367.943199716163</v>
+      </c>
+    </row>
+    <row r="148">
+      <c r="A148" t="s">
+        <v>203</v>
+      </c>
+      <c r="B148" t="s">
+        <v>127</v>
+      </c>
+      <c r="C148" t="n">
+        <v>4371.670125974292</v>
+      </c>
+    </row>
+    <row r="149">
+      <c r="A149" t="s">
+        <v>204</v>
+      </c>
+      <c r="B149" t="s">
+        <v>127</v>
+      </c>
+      <c r="C149" t="n">
+        <v>4367.943199716163</v>
+      </c>
+    </row>
+    <row r="150">
+      <c r="A150" t="s">
+        <v>205</v>
+      </c>
+      <c r="B150" t="s">
+        <v>127</v>
+      </c>
+      <c r="C150" t="n">
+        <v>4371.670125974292</v>
+      </c>
+    </row>
+    <row r="151">
+      <c r="A151" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="152">
+      <c r="A152" t="s">
+        <v>206</v>
+      </c>
+    </row>
+    <row r="153">
+      <c r="A153" t="s">
+        <v>207</v>
+      </c>
+      <c r="B153" t="s">
+        <v>19</v>
+      </c>
+      <c r="C153" t="n">
+        <v>255.9887426167415</v>
+      </c>
+    </row>
+    <row r="154">
+      <c r="A154" t="s">
+        <v>208</v>
+      </c>
+      <c r="B154" t="s">
+        <v>19</v>
+      </c>
+      <c r="C154" t="n">
+        <v>232.1368190562223</v>
+      </c>
+    </row>
+    <row r="155">
+      <c r="A155" t="s">
+        <v>209</v>
+      </c>
+      <c r="B155" t="s">
+        <v>10</v>
+      </c>
+      <c r="C155" t="n">
+        <v>0.4010196429325484</v>
+      </c>
+    </row>
+    <row r="156">
+      <c r="A156" t="s">
+        <v>210</v>
+      </c>
+      <c r="B156" t="s">
+        <v>10</v>
+      </c>
+      <c r="C156" t="n">
+        <v>0.35275993687160867</v>
+      </c>
+    </row>
+    <row r="157">
+      <c r="A157" t="s">
+        <v>211</v>
+      </c>
+      <c r="B157" t="s">
+        <v>10</v>
+      </c>
+      <c r="C157" t="n">
+        <v>0.4178505659080089</v>
+      </c>
+    </row>
+    <row r="158">
+      <c r="A158" t="s">
+        <v>212</v>
+      </c>
+      <c r="B158" t="s">
+        <v>10</v>
+      </c>
+      <c r="C158" t="n">
+        <v>0.4164639410984637</v>
+      </c>
+    </row>
+    <row r="159">
+      <c r="A159" t="s">
+        <v>213</v>
+      </c>
+      <c r="B159" t="s">
+        <v>10</v>
+      </c>
+      <c r="C159" t="n">
+        <v>0.03618441071668287</v>
+      </c>
+    </row>
+    <row r="160">
+      <c r="A160" t="s">
+        <v>214</v>
+      </c>
+      <c r="B160" t="s">
+        <v>10</v>
+      </c>
+      <c r="C160" t="n">
+        <v>0.03614833557140492</v>
+      </c>
+    </row>
+    <row r="161">
+      <c r="A161" t="s">
+        <v>215</v>
+      </c>
+      <c r="B161" t="s">
+        <v>10</v>
+      </c>
+      <c r="C161" t="n">
+        <v>11.54780629646563</v>
+      </c>
+    </row>
+    <row r="162">
+      <c r="A162" t="s">
+        <v>216</v>
+      </c>
+      <c r="B162" t="s">
+        <v>10</v>
+      </c>
+      <c r="C162" t="n">
+        <v>11.520971422759137</v>
+      </c>
+    </row>
+    <row r="163">
+      <c r="A163" t="s">
+        <v>217</v>
+      </c>
+      <c r="B163" t="s">
+        <v>127</v>
+      </c>
+      <c r="C163" t="n">
+        <v>1290.1074946981</v>
+      </c>
+    </row>
+    <row r="164">
+      <c r="A164" t="s">
+        <v>218</v>
+      </c>
+      <c r="B164" t="s">
+        <v>127</v>
+      </c>
+      <c r="C164" t="n">
+        <v>1009.4902177851326</v>
+      </c>
+    </row>
+    <row r="165">
+      <c r="A165" t="s">
+        <v>219</v>
+      </c>
+      <c r="B165" t="s">
+        <v>127</v>
+      </c>
+      <c r="C165" t="n">
+        <v>3893.313380016225</v>
+      </c>
+    </row>
+    <row r="166">
+      <c r="A166" t="s">
+        <v>220</v>
+      </c>
+      <c r="B166" t="s">
+        <v>127</v>
+      </c>
+      <c r="C166" t="n">
+        <v>3889.4318232072346</v>
+      </c>
+    </row>
+    <row r="167">
+      <c r="A167" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="168">
+      <c r="A168" t="s">
+        <v>221</v>
+      </c>
+    </row>
+    <row r="169">
+      <c r="A169" t="s">
+        <v>222</v>
+      </c>
+      <c r="B169" t="s">
+        <v>19</v>
+      </c>
+      <c r="C169" t="n">
+        <v>197.41767258058383</v>
+      </c>
+    </row>
+    <row r="170">
+      <c r="A170" t="s">
+        <v>223</v>
+      </c>
+      <c r="B170" t="s">
+        <v>19</v>
+      </c>
+      <c r="C170" t="n">
+        <v>197.41767258058383</v>
+      </c>
+    </row>
+    <row r="171">
+      <c r="A171" t="s">
+        <v>224</v>
+      </c>
+      <c r="B171" t="s">
+        <v>10</v>
+      </c>
+      <c r="C171" t="n">
+        <v>0.29999999999999993</v>
+      </c>
+    </row>
+    <row r="172">
+      <c r="A172" t="s">
+        <v>225</v>
+      </c>
+      <c r="B172" t="s">
+        <v>10</v>
+      </c>
+      <c r="C172" t="n">
+        <v>0.29999999999999993</v>
+      </c>
+    </row>
+    <row r="173">
+      <c r="A173" t="s">
+        <v>226</v>
+      </c>
+      <c r="B173" t="s">
+        <v>10</v>
+      </c>
+      <c r="C173" t="n">
+        <v>0.5421843406340271</v>
+      </c>
+    </row>
+    <row r="174">
+      <c r="A174" t="s">
+        <v>227</v>
+      </c>
+      <c r="B174" t="s">
+        <v>10</v>
+      </c>
+      <c r="C174" t="n">
+        <v>0.5334974438987716</v>
+      </c>
+    </row>
+    <row r="175">
+      <c r="A175" t="s">
+        <v>228</v>
+      </c>
+      <c r="B175" t="s">
+        <v>10</v>
+      </c>
+      <c r="C175" t="n">
+        <v>0.040001345363663586</v>
+      </c>
+    </row>
+    <row r="176">
+      <c r="A176" t="s">
+        <v>229</v>
+      </c>
+      <c r="B176" t="s">
+        <v>10</v>
+      </c>
+      <c r="C176" t="n">
+        <v>0.03969830905467518</v>
+      </c>
+    </row>
+    <row r="177">
+      <c r="A177" t="s">
+        <v>230</v>
+      </c>
+      <c r="B177" t="s">
+        <v>10</v>
+      </c>
+      <c r="C177" t="n">
+        <v>13.554152634239557</v>
+      </c>
+    </row>
+    <row r="178">
+      <c r="A178" t="s">
+        <v>231</v>
+      </c>
+      <c r="B178" t="s">
+        <v>10</v>
+      </c>
+      <c r="C178" t="n">
+        <v>13.438795167925239</v>
+      </c>
+    </row>
+    <row r="179">
+      <c r="A179" t="s">
+        <v>232</v>
+      </c>
+      <c r="B179" t="s">
+        <v>127</v>
+      </c>
+      <c r="C179" t="n">
+        <v>3316.189599311804</v>
+      </c>
+    </row>
+    <row r="180">
+      <c r="A180" t="s">
+        <v>233</v>
+      </c>
+      <c r="B180" t="s">
+        <v>127</v>
+      </c>
+      <c r="C180" t="n">
+        <v>3291.067297875562</v>
+      </c>
+    </row>
+    <row r="181">
+      <c r="A181" t="s">
+        <v>234</v>
+      </c>
+      <c r="B181" t="s">
+        <v>127</v>
+      </c>
+      <c r="C181" t="n">
+        <v>3316.189599311804</v>
+      </c>
+    </row>
+    <row r="182">
+      <c r="A182" t="s">
+        <v>235</v>
+      </c>
+      <c r="B182" t="s">
+        <v>127</v>
+      </c>
+      <c r="C182" t="n">
+        <v>3291.067297875562</v>
+      </c>
+    </row>
+    <row r="183">
+      <c r="A183" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="184">
+      <c r="A184" t="s">
+        <v>236</v>
+      </c>
+    </row>
+    <row r="185">
+      <c r="A185" t="s">
+        <v>237</v>
+      </c>
+      <c r="B185" t="s">
+        <v>19</v>
+      </c>
+      <c r="C185" t="n">
+        <v>224.90679627393837</v>
+      </c>
+    </row>
+    <row r="186">
+      <c r="A186" t="s">
+        <v>238</v>
+      </c>
+      <c r="B186" t="s">
+        <v>19</v>
+      </c>
+      <c r="C186" t="n">
+        <v>221.33361546517457</v>
+      </c>
+    </row>
+    <row r="187">
+      <c r="A187" t="s">
+        <v>239</v>
+      </c>
+      <c r="B187" t="s">
+        <v>10</v>
+      </c>
+      <c r="C187" t="n">
+        <v>0.3417730439236138</v>
+      </c>
+    </row>
+    <row r="188">
+      <c r="A188" t="s">
+        <v>240</v>
+      </c>
+      <c r="B188" t="s">
+        <v>10</v>
+      </c>
+      <c r="C188" t="n">
+        <v>0.3346619068734856</v>
+      </c>
+    </row>
+    <row r="189">
+      <c r="A189" t="s">
+        <v>241</v>
+      </c>
+      <c r="B189" t="s">
+        <v>10</v>
+      </c>
+      <c r="C189" t="n">
+        <v>0.4079469736554963</v>
+      </c>
+    </row>
+    <row r="190">
+      <c r="A190" t="s">
+        <v>242</v>
+      </c>
+      <c r="B190" t="s">
+        <v>10</v>
+      </c>
+      <c r="C190" t="n">
+        <v>0.40771013939086814</v>
+      </c>
+    </row>
+    <row r="191">
+      <c r="A191" t="s">
+        <v>243</v>
+      </c>
+      <c r="B191" t="s">
+        <v>10</v>
+      </c>
+      <c r="C191" t="n">
+        <v>0.03592675375942698</v>
+      </c>
+    </row>
+    <row r="192">
+      <c r="A192" t="s">
+        <v>244</v>
+      </c>
+      <c r="B192" t="s">
+        <v>10</v>
+      </c>
+      <c r="C192" t="n">
+        <v>0.03592059215720809</v>
+      </c>
+    </row>
+    <row r="193">
+      <c r="A193" t="s">
+        <v>245</v>
+      </c>
+      <c r="B193" t="s">
+        <v>10</v>
+      </c>
+      <c r="C193" t="n">
+        <v>11.354963389879146</v>
+      </c>
+    </row>
+    <row r="194">
+      <c r="A194" t="s">
+        <v>246</v>
+      </c>
+      <c r="B194" t="s">
+        <v>10</v>
+      </c>
+      <c r="C194" t="n">
+        <v>11.35031787912923</v>
+      </c>
+    </row>
+    <row r="195">
+      <c r="A195" t="s">
+        <v>247</v>
+      </c>
+      <c r="B195" t="s">
+        <v>127</v>
+      </c>
+      <c r="C195" t="n">
+        <v>966.6125065433948</v>
+      </c>
+    </row>
+    <row r="196">
+      <c r="A196" t="s">
+        <v>248</v>
+      </c>
+      <c r="B196" t="s">
+        <v>127</v>
+      </c>
+      <c r="C196" t="n">
+        <v>907.8566743950048</v>
+      </c>
+    </row>
+    <row r="197">
+      <c r="A197" t="s">
+        <v>249</v>
+      </c>
+      <c r="B197" t="s">
+        <v>127</v>
+      </c>
+      <c r="C197" t="n">
+        <v>3865.5904114982905</v>
+      </c>
+    </row>
+    <row r="198">
+      <c r="A198" t="s">
+        <v>250</v>
+      </c>
+      <c r="B198" t="s">
+        <v>127</v>
+      </c>
+      <c r="C198" t="n">
+        <v>3864.927445102374</v>
+      </c>
+    </row>
+    <row r="199">
+      <c r="A199" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="200">
+      <c r="A200" t="s">
+        <v>251</v>
+      </c>
+    </row>
+    <row r="201">
+      <c r="A201" t="s">
+        <v>252</v>
+      </c>
+      <c r="B201" t="s">
+        <v>19</v>
+      </c>
+      <c r="C201" t="n">
+        <v>112.74267186559192</v>
+      </c>
+    </row>
+    <row r="202">
+      <c r="A202" t="s">
+        <v>253</v>
+      </c>
+      <c r="B202" t="s">
+        <v>19</v>
+      </c>
+      <c r="C202" t="n">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="203">
+      <c r="A203" t="s">
+        <v>254</v>
+      </c>
+      <c r="B203" t="s">
+        <v>10</v>
+      </c>
+      <c r="C203" t="n">
+        <v>0.1704697114048966</v>
+      </c>
+    </row>
+    <row r="204">
+      <c r="A204" t="s">
+        <v>255</v>
+      </c>
+      <c r="B204" t="s">
+        <v>10</v>
+      </c>
+      <c r="C204" t="n">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="205">
+      <c r="A205" t="s">
+        <v>256</v>
+      </c>
+      <c r="B205" t="s">
+        <v>10</v>
+      </c>
+      <c r="C205" t="n">
+        <v>1.5584919410019569</v>
+      </c>
+    </row>
+    <row r="206">
+      <c r="A206" t="s">
+        <v>257</v>
+      </c>
+      <c r="B206" t="s">
+        <v>10</v>
+      </c>
+      <c r="C206" t="n">
+        <v>1.4387</v>
+      </c>
+    </row>
+    <row r="207">
+      <c r="A207" t="s">
+        <v>258</v>
+      </c>
+      <c r="B207" t="s">
+        <v>10</v>
+      </c>
+      <c r="C207" t="n">
+        <v>0.20344099009247915</v>
+      </c>
+    </row>
+    <row r="208">
+      <c r="A208" t="s">
+        <v>259</v>
+      </c>
+      <c r="B208" t="s">
+        <v>10</v>
+      </c>
+      <c r="C208" t="n">
+        <v>0.19153799598718918</v>
+      </c>
+    </row>
+    <row r="209">
+      <c r="A209" t="s">
+        <v>260</v>
+      </c>
+      <c r="B209" t="s">
+        <v>10</v>
+      </c>
+      <c r="C209" t="n">
+        <v>7.660658455768947</v>
+      </c>
+    </row>
+    <row r="210">
+      <c r="A210" t="s">
+        <v>261</v>
+      </c>
+      <c r="B210" t="s">
+        <v>10</v>
+      </c>
+      <c r="C210" t="n">
+        <v>7.511303397453454</v>
+      </c>
+    </row>
+    <row r="211">
+      <c r="A211" t="s">
+        <v>262</v>
+      </c>
+      <c r="B211" t="s">
+        <v>127</v>
+      </c>
+      <c r="C211" t="n">
+        <v>-655.0452159829897</v>
+      </c>
+    </row>
+    <row r="212">
+      <c r="A212" t="s">
+        <v>263</v>
+      </c>
+      <c r="B212" t="s">
+        <v>127</v>
+      </c>
+      <c r="C212" t="n">
+        <v>49.50742544941821</v>
+      </c>
+    </row>
+    <row r="213">
+      <c r="A213" t="s">
+        <v>264</v>
+      </c>
+      <c r="B213" t="s">
+        <v>127</v>
+      </c>
+      <c r="C213" t="n">
+        <v>3374.506823719656</v>
+      </c>
+    </row>
+    <row r="214">
+      <c r="A214" t="s">
+        <v>265</v>
+      </c>
+      <c r="B214" t="s">
+        <v>127</v>
+      </c>
+      <c r="C214" t="n">
         <v>0.0</v>
       </c>
     </row>
@@ -3324,24 +4403,24 @@
     </row>
     <row r="2">
       <c r="A2" t="s">
-        <v>191</v>
+        <v>266</v>
       </c>
       <c r="B2" t="s">
-        <v>10</v>
-      </c>
-      <c r="C2" t="s">
-        <v>192</v>
+        <v>11</v>
+      </c>
+      <c r="C2" t="n">
+        <v>16999.999999999993</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="s">
-        <v>193</v>
+        <v>267</v>
       </c>
       <c r="B3" t="s">
         <v>10</v>
       </c>
-      <c r="C3" t="s">
-        <v>194</v>
+      <c r="C3" t="n">
+        <v>0.42</v>
       </c>
     </row>
     <row r="4">
@@ -3351,88 +4430,389 @@
     </row>
     <row r="5">
       <c r="A5" t="s">
-        <v>10</v>
+        <v>268</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="s">
-        <v>195</v>
+        <v>269</v>
+      </c>
+      <c r="B6" t="s">
+        <v>53</v>
+      </c>
+      <c r="C6" t="n">
+        <v>559.4420029593741</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="s">
-        <v>196</v>
+        <v>270</v>
+      </c>
+      <c r="B7" t="s">
+        <v>34</v>
+      </c>
+      <c r="C7" t="n">
+        <v>22500.0</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="s">
+        <v>271</v>
+      </c>
+      <c r="B8" t="s">
+        <v>34</v>
+      </c>
+      <c r="C8" t="n">
+        <v>7344.0</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="s">
+        <v>272</v>
+      </c>
+      <c r="B9" t="s">
+        <v>21</v>
+      </c>
+      <c r="C9" t="n">
+        <v>72.0</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="s">
+        <v>273</v>
+      </c>
+      <c r="B10" t="s">
+        <v>34</v>
+      </c>
+      <c r="C10" t="n">
+        <v>2205.999999999998</v>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" t="s">
+        <v>274</v>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" t="s">
+        <v>269</v>
+      </c>
+      <c r="B13" t="s">
+        <v>53</v>
+      </c>
+      <c r="C13" t="n">
+        <v>706.3244922863962</v>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" t="s">
+        <v>270</v>
+      </c>
+      <c r="B14" t="s">
+        <v>34</v>
+      </c>
+      <c r="C14" t="n">
+        <v>22500.0</v>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" t="s">
+        <v>271</v>
+      </c>
+      <c r="B15" t="s">
+        <v>34</v>
+      </c>
+      <c r="C15" t="n">
+        <v>6936.0</v>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" t="s">
+        <v>272</v>
+      </c>
+      <c r="B16" t="s">
+        <v>21</v>
+      </c>
+      <c r="C16" t="n">
+        <v>68.0</v>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" t="s">
+        <v>273</v>
+      </c>
+      <c r="B17" t="s">
+        <v>34</v>
+      </c>
+      <c r="C17" t="n">
+        <v>2613.999999999998</v>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" t="s">
+        <v>275</v>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" t="s">
+        <v>269</v>
+      </c>
+      <c r="B20" t="s">
+        <v>53</v>
+      </c>
+      <c r="C20" t="n">
+        <v>1565.6847666890321</v>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" t="s">
+        <v>270</v>
+      </c>
+      <c r="B21" t="s">
+        <v>34</v>
+      </c>
+      <c r="C21" t="n">
+        <v>22500.0</v>
+      </c>
+    </row>
+    <row r="22">
+      <c r="A22" t="s">
+        <v>271</v>
+      </c>
+      <c r="B22" t="s">
+        <v>34</v>
+      </c>
+      <c r="C22" t="n">
+        <v>4549.999999999998</v>
+      </c>
+    </row>
+    <row r="23">
+      <c r="A23" t="s">
+        <v>272</v>
+      </c>
+      <c r="B23" t="s">
+        <v>21</v>
+      </c>
+      <c r="C23" t="n">
+        <v>45.0</v>
+      </c>
+    </row>
+    <row r="24">
+      <c r="A24" t="s">
+        <v>273</v>
+      </c>
+      <c r="B24" t="s">
+        <v>34</v>
+      </c>
+      <c r="C24" t="n">
+        <v>5000.0</v>
+      </c>
+    </row>
+    <row r="25">
+      <c r="A25" t="s">
+        <v>276</v>
+      </c>
+    </row>
+    <row r="26">
+      <c r="A26" t="s">
+        <v>269</v>
+      </c>
+      <c r="B26" t="s">
+        <v>53</v>
+      </c>
+      <c r="C26" t="n">
+        <v>1703.7801237952058</v>
+      </c>
+    </row>
+    <row r="27">
+      <c r="A27" t="s">
+        <v>270</v>
+      </c>
+      <c r="B27" t="s">
+        <v>34</v>
+      </c>
+      <c r="C27" t="n">
+        <v>17949.999999999996</v>
+      </c>
+    </row>
+    <row r="28">
+      <c r="A28" t="s">
+        <v>271</v>
+      </c>
+      <c r="B28" t="s">
+        <v>34</v>
+      </c>
+      <c r="C28" t="n">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="29">
+      <c r="A29" t="s">
+        <v>272</v>
+      </c>
+      <c r="B29" t="s">
+        <v>21</v>
+      </c>
+      <c r="C29" t="n">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="30">
+      <c r="A30" t="s">
+        <v>273</v>
+      </c>
+      <c r="B30" t="s">
+        <v>34</v>
+      </c>
+      <c r="C30" t="n">
+        <v>5000.0</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15.0" baseColWidth="35"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="s">
+        <v>277</v>
+      </c>
+      <c r="B2" t="s">
+        <v>10</v>
+      </c>
+      <c r="C2" t="s">
+        <v>278</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="s">
+        <v>279</v>
+      </c>
+      <c r="B3" t="s">
+        <v>10</v>
+      </c>
+      <c r="C3" t="s">
+        <v>280</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="s">
+        <v>281</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="s">
+        <v>282</v>
       </c>
       <c r="B7" t="s">
         <v>13</v>
       </c>
       <c r="C7" t="n">
-        <v>63.67173918048353</v>
+        <v>62.74439771473102</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="s">
-        <v>196</v>
+        <v>282</v>
       </c>
       <c r="B8" t="s">
         <v>19</v>
       </c>
       <c r="C8" t="n">
-        <v>123.76795953009756</v>
+        <v>121.96535192928275</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="s">
-        <v>197</v>
+        <v>283</v>
       </c>
       <c r="B9" t="s">
         <v>13</v>
       </c>
       <c r="C9" t="n">
-        <v>77.98163601388009</v>
+        <v>76.84587930967095</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="s">
-        <v>197</v>
+        <v>283</v>
       </c>
       <c r="B10" t="s">
         <v>19</v>
       </c>
       <c r="C10" t="n">
-        <v>151.58417367708873</v>
+        <v>149.37643926285926</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="s">
-        <v>198</v>
+        <v>284</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="s">
-        <v>199</v>
+        <v>285</v>
       </c>
       <c r="B12" t="s">
         <v>13</v>
       </c>
       <c r="C12" t="n">
-        <v>100.67385919725538</v>
+        <v>99.20760359700691</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="s">
-        <v>199</v>
+        <v>285</v>
       </c>
       <c r="B13" t="s">
         <v>19</v>
       </c>
       <c r="C13" t="n">
-        <v>195.6943267333258</v>
+        <v>192.8441538602726</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="s">
-        <v>200</v>
+        <v>286</v>
       </c>
       <c r="B14" t="s">
         <v>21</v>
@@ -3443,12 +4823,12 @@
     </row>
     <row r="15">
       <c r="A15" t="s">
-        <v>201</v>
+        <v>287</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="s">
-        <v>202</v>
+        <v>288</v>
       </c>
       <c r="B16" t="s">
         <v>13</v>
@@ -3459,7 +4839,7 @@
     </row>
     <row r="17">
       <c r="A17" t="s">
-        <v>202</v>
+        <v>288</v>
       </c>
       <c r="B17" t="s">
         <v>19</v>
@@ -3470,7 +4850,7 @@
     </row>
     <row r="18">
       <c r="A18" t="s">
-        <v>200</v>
+        <v>286</v>
       </c>
       <c r="B18" t="s">
         <v>21</v>
@@ -3481,12 +4861,12 @@
     </row>
     <row r="19">
       <c r="A19" t="s">
-        <v>203</v>
+        <v>289</v>
       </c>
     </row>
     <row r="20">
       <c r="A20" t="s">
-        <v>204</v>
+        <v>290</v>
       </c>
       <c r="B20" t="s">
         <v>13</v>
@@ -3497,7 +4877,7 @@
     </row>
     <row r="21">
       <c r="A21" t="s">
-        <v>204</v>
+        <v>290</v>
       </c>
       <c r="B21" t="s">
         <v>19</v>
@@ -3508,7 +4888,7 @@
     </row>
     <row r="22">
       <c r="A22" t="s">
-        <v>200</v>
+        <v>286</v>
       </c>
       <c r="B22" t="s">
         <v>21</v>
@@ -3519,12 +4899,12 @@
     </row>
     <row r="23">
       <c r="A23" t="s">
-        <v>205</v>
+        <v>291</v>
       </c>
     </row>
     <row r="24">
       <c r="A24" t="s">
-        <v>204</v>
+        <v>290</v>
       </c>
       <c r="B24" t="s">
         <v>13</v>
@@ -3535,7 +4915,7 @@
     </row>
     <row r="25">
       <c r="A25" t="s">
-        <v>204</v>
+        <v>290</v>
       </c>
       <c r="B25" t="s">
         <v>19</v>
@@ -3546,7 +4926,7 @@
     </row>
     <row r="26">
       <c r="A26" t="s">
-        <v>200</v>
+        <v>286</v>
       </c>
       <c r="B26" t="s">
         <v>21</v>
@@ -3557,12 +4937,12 @@
     </row>
     <row r="27">
       <c r="A27" t="s">
-        <v>206</v>
+        <v>292</v>
       </c>
     </row>
     <row r="28">
       <c r="A28" t="s">
-        <v>202</v>
+        <v>288</v>
       </c>
       <c r="B28" t="s">
         <v>13</v>
@@ -3573,7 +4953,7 @@
     </row>
     <row r="29">
       <c r="A29" t="s">
-        <v>202</v>
+        <v>288</v>
       </c>
       <c r="B29" t="s">
         <v>19</v>
@@ -3584,7 +4964,7 @@
     </row>
     <row r="30">
       <c r="A30" t="s">
-        <v>200</v>
+        <v>286</v>
       </c>
       <c r="B30" t="s">
         <v>21</v>
@@ -3595,34 +4975,34 @@
     </row>
     <row r="31">
       <c r="A31" t="s">
-        <v>207</v>
+        <v>293</v>
       </c>
     </row>
     <row r="32">
       <c r="A32" t="s">
-        <v>208</v>
+        <v>294</v>
       </c>
       <c r="B32" t="s">
         <v>13</v>
       </c>
       <c r="C32" t="n">
-        <v>77.98163601388009</v>
+        <v>76.84587930967093</v>
       </c>
     </row>
     <row r="33">
       <c r="A33" t="s">
-        <v>208</v>
+        <v>294</v>
       </c>
       <c r="B33" t="s">
         <v>19</v>
       </c>
       <c r="C33" t="n">
-        <v>151.58417367708873</v>
+        <v>149.37643926285926</v>
       </c>
     </row>
     <row r="34">
       <c r="A34" t="s">
-        <v>200</v>
+        <v>286</v>
       </c>
       <c r="B34" t="s">
         <v>21</v>
@@ -3638,55 +5018,55 @@
     </row>
     <row r="36">
       <c r="A36" t="s">
-        <v>209</v>
+        <v>295</v>
       </c>
     </row>
     <row r="37">
       <c r="A37" t="s">
-        <v>210</v>
+        <v>296</v>
       </c>
     </row>
     <row r="38">
       <c r="A38" t="s">
-        <v>199</v>
+        <v>285</v>
       </c>
       <c r="B38" t="s">
         <v>13</v>
       </c>
       <c r="C38" t="n">
-        <v>100.67385919725538</v>
+        <v>99.20760359700691</v>
       </c>
     </row>
     <row r="39">
       <c r="A39" t="s">
-        <v>199</v>
+        <v>285</v>
       </c>
       <c r="B39" t="s">
         <v>19</v>
       </c>
       <c r="C39" t="n">
-        <v>195.6943267333258</v>
+        <v>192.8441538602726</v>
       </c>
     </row>
     <row r="40">
       <c r="A40" t="s">
-        <v>200</v>
+        <v>286</v>
       </c>
       <c r="B40" t="s">
         <v>21</v>
       </c>
       <c r="C40" t="n">
-        <v>1.933638517645491</v>
+        <v>1.945847745415077</v>
       </c>
     </row>
     <row r="41">
       <c r="A41" t="s">
-        <v>211</v>
+        <v>297</v>
       </c>
     </row>
     <row r="42">
       <c r="A42" t="s">
-        <v>202</v>
+        <v>288</v>
       </c>
       <c r="B42" t="s">
         <v>13</v>
@@ -3697,7 +5077,7 @@
     </row>
     <row r="43">
       <c r="A43" t="s">
-        <v>202</v>
+        <v>288</v>
       </c>
       <c r="B43" t="s">
         <v>19</v>
@@ -3708,23 +5088,23 @@
     </row>
     <row r="44">
       <c r="A44" t="s">
-        <v>200</v>
+        <v>286</v>
       </c>
       <c r="B44" t="s">
         <v>21</v>
       </c>
       <c r="C44" t="n">
-        <v>2.245654566065172</v>
+        <v>2.280595155953703</v>
       </c>
     </row>
     <row r="45">
       <c r="A45" t="s">
-        <v>212</v>
+        <v>298</v>
       </c>
     </row>
     <row r="46">
       <c r="A46" t="s">
-        <v>204</v>
+        <v>290</v>
       </c>
       <c r="B46" t="s">
         <v>13</v>
@@ -3735,7 +5115,7 @@
     </row>
     <row r="47">
       <c r="A47" t="s">
-        <v>204</v>
+        <v>290</v>
       </c>
       <c r="B47" t="s">
         <v>19</v>
@@ -3746,23 +5126,23 @@
     </row>
     <row r="48">
       <c r="A48" t="s">
-        <v>200</v>
+        <v>286</v>
       </c>
       <c r="B48" t="s">
         <v>21</v>
       </c>
       <c r="C48" t="n">
-        <v>1.7479245778994392</v>
+        <v>1.768903849886927</v>
       </c>
     </row>
     <row r="49">
       <c r="A49" t="s">
-        <v>213</v>
+        <v>299</v>
       </c>
     </row>
     <row r="50">
       <c r="A50" t="s">
-        <v>204</v>
+        <v>290</v>
       </c>
       <c r="B50" t="s">
         <v>13</v>
@@ -3773,7 +5153,7 @@
     </row>
     <row r="51">
       <c r="A51" t="s">
-        <v>204</v>
+        <v>290</v>
       </c>
       <c r="B51" t="s">
         <v>19</v>
@@ -3784,23 +5164,23 @@
     </row>
     <row r="52">
       <c r="A52" t="s">
-        <v>200</v>
+        <v>286</v>
       </c>
       <c r="B52" t="s">
         <v>21</v>
       </c>
       <c r="C52" t="n">
-        <v>0.25207542210056066</v>
+        <v>0.23109615011307305</v>
       </c>
     </row>
     <row r="53">
       <c r="A53" t="s">
-        <v>214</v>
+        <v>300</v>
       </c>
     </row>
     <row r="54">
       <c r="A54" t="s">
-        <v>202</v>
+        <v>288</v>
       </c>
       <c r="B54" t="s">
         <v>13</v>
@@ -3811,7 +5191,7 @@
     </row>
     <row r="55">
       <c r="A55" t="s">
-        <v>202</v>
+        <v>288</v>
       </c>
       <c r="B55" t="s">
         <v>19</v>
@@ -3822,51 +5202,51 @@
     </row>
     <row r="56">
       <c r="A56" t="s">
-        <v>200</v>
+        <v>286</v>
       </c>
       <c r="B56" t="s">
         <v>21</v>
       </c>
       <c r="C56" t="n">
-        <v>-0.2456545660651721</v>
+        <v>-0.2805951559537032</v>
       </c>
     </row>
     <row r="57">
       <c r="A57" t="s">
-        <v>215</v>
+        <v>301</v>
       </c>
     </row>
     <row r="58">
       <c r="A58" t="s">
-        <v>208</v>
+        <v>294</v>
       </c>
       <c r="B58" t="s">
         <v>13</v>
       </c>
       <c r="C58" t="n">
-        <v>77.98163601388009</v>
+        <v>76.84587930967093</v>
       </c>
     </row>
     <row r="59">
       <c r="A59" t="s">
-        <v>208</v>
+        <v>294</v>
       </c>
       <c r="B59" t="s">
         <v>19</v>
       </c>
       <c r="C59" t="n">
-        <v>151.58417367708873</v>
+        <v>149.37643926285926</v>
       </c>
     </row>
     <row r="60">
       <c r="A60" t="s">
-        <v>200</v>
+        <v>286</v>
       </c>
       <c r="B60" t="s">
         <v>21</v>
       </c>
       <c r="C60" t="n">
-        <v>0.06636148235450878</v>
+        <v>0.0541522545849229</v>
       </c>
     </row>
     <row r="61">
@@ -3881,61 +5261,61 @@
     </row>
     <row r="63">
       <c r="A63" t="s">
-        <v>216</v>
+        <v>302</v>
       </c>
     </row>
     <row r="64">
       <c r="A64" t="s">
-        <v>217</v>
+        <v>303</v>
       </c>
       <c r="B64" t="s">
         <v>13</v>
       </c>
       <c r="C64" t="n">
-        <v>48.085536727355986</v>
+        <v>47.385199141416294</v>
       </c>
     </row>
     <row r="65">
       <c r="A65" t="s">
-        <v>217</v>
+        <v>303</v>
       </c>
       <c r="B65" t="s">
         <v>19</v>
       </c>
       <c r="C65" t="n">
-        <v>93.47080573352136</v>
+        <v>92.10945837424333</v>
       </c>
     </row>
     <row r="66">
       <c r="A66" t="s">
-        <v>218</v>
+        <v>304</v>
       </c>
     </row>
     <row r="67">
       <c r="A67" t="s">
-        <v>219</v>
+        <v>305</v>
       </c>
       <c r="B67" t="s">
         <v>13</v>
       </c>
       <c r="C67" t="n">
-        <v>68.00321819381641</v>
+        <v>67.01279128154086</v>
       </c>
     </row>
     <row r="68">
       <c r="A68" t="s">
-        <v>219</v>
+        <v>305</v>
       </c>
       <c r="B68" t="s">
         <v>19</v>
       </c>
       <c r="C68" t="n">
-        <v>132.18768115428674</v>
+        <v>130.26244525569496</v>
       </c>
     </row>
     <row r="69">
       <c r="A69" t="s">
-        <v>200</v>
+        <v>286</v>
       </c>
       <c r="B69" t="s">
         <v>21</v>
@@ -3946,34 +5326,34 @@
     </row>
     <row r="70">
       <c r="A70" t="s">
-        <v>220</v>
+        <v>306</v>
       </c>
     </row>
     <row r="71">
       <c r="A71" t="s">
-        <v>199</v>
+        <v>285</v>
       </c>
       <c r="B71" t="s">
         <v>13</v>
       </c>
       <c r="C71" t="n">
-        <v>84.36237073943346</v>
+        <v>83.13368238345649</v>
       </c>
     </row>
     <row r="72">
       <c r="A72" t="s">
-        <v>199</v>
+        <v>285</v>
       </c>
       <c r="B72" t="s">
         <v>19</v>
       </c>
       <c r="C72" t="n">
-        <v>163.98732973108014</v>
+        <v>161.5989506373884</v>
       </c>
     </row>
     <row r="73">
       <c r="A73" t="s">
-        <v>200</v>
+        <v>286</v>
       </c>
       <c r="B73" t="s">
         <v>21</v>
@@ -3989,83 +5369,83 @@
     </row>
     <row r="75">
       <c r="A75" t="s">
-        <v>221</v>
+        <v>307</v>
       </c>
     </row>
     <row r="76">
       <c r="A76" t="s">
-        <v>222</v>
+        <v>308</v>
       </c>
     </row>
     <row r="77">
       <c r="A77" t="s">
-        <v>219</v>
+        <v>305</v>
       </c>
       <c r="B77" t="s">
         <v>13</v>
       </c>
       <c r="C77" t="n">
-        <v>68.00321819381641</v>
+        <v>67.01279128154086</v>
       </c>
     </row>
     <row r="78">
       <c r="A78" t="s">
-        <v>219</v>
+        <v>305</v>
       </c>
       <c r="B78" t="s">
         <v>19</v>
       </c>
       <c r="C78" t="n">
-        <v>132.18768115428674</v>
+        <v>130.26244525569496</v>
       </c>
     </row>
     <row r="79">
       <c r="A79" t="s">
-        <v>200</v>
+        <v>286</v>
       </c>
       <c r="B79" t="s">
         <v>21</v>
       </c>
       <c r="C79" t="n">
-        <v>1.4526227825256133</v>
+        <v>1.4585417485291745</v>
       </c>
     </row>
     <row r="80">
       <c r="A80" t="s">
-        <v>223</v>
+        <v>309</v>
       </c>
     </row>
     <row r="81">
       <c r="A81" t="s">
-        <v>199</v>
+        <v>285</v>
       </c>
       <c r="B81" t="s">
         <v>13</v>
       </c>
       <c r="C81" t="n">
-        <v>84.36237073943346</v>
+        <v>83.13368238345649</v>
       </c>
     </row>
     <row r="82">
       <c r="A82" t="s">
-        <v>199</v>
+        <v>285</v>
       </c>
       <c r="B82" t="s">
         <v>19</v>
       </c>
       <c r="C82" t="n">
-        <v>163.98732973108014</v>
+        <v>161.5989506373884</v>
       </c>
     </row>
     <row r="83">
       <c r="A83" t="s">
-        <v>200</v>
+        <v>286</v>
       </c>
       <c r="B83" t="s">
         <v>21</v>
       </c>
       <c r="C83" t="n">
-        <v>1.4526227825256133</v>
+        <v>1.4585417485291745</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Work on high lift modifed stall path in executable.
</commit_message>
<xml_diff>
--- a/JPADSandBox_v2/out/ATR-72/PERFORMANCE/Performance.xlsx
+++ b/JPADSandBox_v2/out/ATR-72/PERFORMANCE/Performance.xlsx
@@ -12,13 +12,14 @@
     <sheet name="DESCENT" r:id="rId6" sheetId="4"/>
     <sheet name="LANDING" r:id="rId7" sheetId="5"/>
     <sheet name="MISSION PROFILE" r:id="rId8" sheetId="6"/>
-    <sheet name="V-n DIAGRAM" r:id="rId9" sheetId="7"/>
+    <sheet name="PAYLOAD-RANGE" r:id="rId9" sheetId="7"/>
+    <sheet name="V-n DIAGRAM" r:id="rId10" sheetId="8"/>
   </sheets>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="602" uniqueCount="224">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="806" uniqueCount="310">
   <si>
     <t>Description</t>
   </si>
@@ -548,6 +549,231 @@
     <t>Drag at second climb ending</t>
   </si>
   <si>
+    <t>SECOND CLIMB</t>
+  </si>
+  <si>
+    <t>Speed (TAS) at second climb start</t>
+  </si>
+  <si>
+    <t>Speed (TAS) at second climb ending</t>
+  </si>
+  <si>
+    <t>Mach at second climb start</t>
+  </si>
+  <si>
+    <t>Mach at second climb ending</t>
+  </si>
+  <si>
+    <t>CL at second climb start</t>
+  </si>
+  <si>
+    <t>CL at second climb ending</t>
+  </si>
+  <si>
+    <t>CD at second climb start</t>
+  </si>
+  <si>
+    <t>CD at second climb ending</t>
+  </si>
+  <si>
+    <t>Efficiency at second climb start</t>
+  </si>
+  <si>
+    <t>Efficiency at second climb ending</t>
+  </si>
+  <si>
+    <t>Thrust at second climb start</t>
+  </si>
+  <si>
+    <t>Thrust at second climb ending</t>
+  </si>
+  <si>
+    <t>Drag at first descent start</t>
+  </si>
+  <si>
+    <t>Drag at first descent ending</t>
+  </si>
+  <si>
+    <t>ALTERNATE CRUISE</t>
+  </si>
+  <si>
+    <t>Speed (TAS) at alternate cruise start</t>
+  </si>
+  <si>
+    <t>Speed (TAS) at alternate cruise ending</t>
+  </si>
+  <si>
+    <t>Mach at alternate cruise start</t>
+  </si>
+  <si>
+    <t>Mach at alternate cruise ending</t>
+  </si>
+  <si>
+    <t>CL at alternate cruise start</t>
+  </si>
+  <si>
+    <t>CL at alternate cruise ending</t>
+  </si>
+  <si>
+    <t>CD at alternate cruise start</t>
+  </si>
+  <si>
+    <t>CD at alternate cruise ending</t>
+  </si>
+  <si>
+    <t>Efficiency at alternate cruise start</t>
+  </si>
+  <si>
+    <t>Efficiency at alternate cruise ending</t>
+  </si>
+  <si>
+    <t>Thrust at alternate cruise start</t>
+  </si>
+  <si>
+    <t>Thrust at alternate cruise ending</t>
+  </si>
+  <si>
+    <t>Drag at alternate cruise start</t>
+  </si>
+  <si>
+    <t>Drag at alternate cruise ending</t>
+  </si>
+  <si>
+    <t>SECOND DESCENT</t>
+  </si>
+  <si>
+    <t>Speed (TAS) at second descent start</t>
+  </si>
+  <si>
+    <t>Speed (TAS) at second descent ending</t>
+  </si>
+  <si>
+    <t>Mach at second descent start</t>
+  </si>
+  <si>
+    <t>Mach at second descent ending</t>
+  </si>
+  <si>
+    <t>CL at second descent start</t>
+  </si>
+  <si>
+    <t>CL at second descent ending</t>
+  </si>
+  <si>
+    <t>CD at second descent start</t>
+  </si>
+  <si>
+    <t>CD at second descent ending</t>
+  </si>
+  <si>
+    <t>Efficiency at second descent start</t>
+  </si>
+  <si>
+    <t>Efficiency at second descent ending</t>
+  </si>
+  <si>
+    <t>Thrust at second descent start</t>
+  </si>
+  <si>
+    <t>Thrust at second descent ending</t>
+  </si>
+  <si>
+    <t>Drag at second descent start</t>
+  </si>
+  <si>
+    <t>Drag at second descent ending</t>
+  </si>
+  <si>
+    <t>HOLDING</t>
+  </si>
+  <si>
+    <t>Speed (TAS) at holding start</t>
+  </si>
+  <si>
+    <t>Speed (TAS) at holding ending</t>
+  </si>
+  <si>
+    <t>Mach at holding start</t>
+  </si>
+  <si>
+    <t>Mach at holding ending</t>
+  </si>
+  <si>
+    <t>CL at holding start</t>
+  </si>
+  <si>
+    <t>CL at holding ending</t>
+  </si>
+  <si>
+    <t>CD at holding start</t>
+  </si>
+  <si>
+    <t>CD at holding ending</t>
+  </si>
+  <si>
+    <t>Efficiency at holding start</t>
+  </si>
+  <si>
+    <t>Efficiency at holding ending</t>
+  </si>
+  <si>
+    <t>Thrust at holding start</t>
+  </si>
+  <si>
+    <t>Thrust at holding ending</t>
+  </si>
+  <si>
+    <t>Drag at holding start</t>
+  </si>
+  <si>
+    <t>Drag at holding ending</t>
+  </si>
+  <si>
+    <t>THIRD DESCENT</t>
+  </si>
+  <si>
+    <t>Speed (TAS) at third descent start</t>
+  </si>
+  <si>
+    <t>Speed (TAS) at third descent ending</t>
+  </si>
+  <si>
+    <t>Mach at third descent start</t>
+  </si>
+  <si>
+    <t>Mach at third descent ending</t>
+  </si>
+  <si>
+    <t>CL at third descent start</t>
+  </si>
+  <si>
+    <t>CL at third descent ending</t>
+  </si>
+  <si>
+    <t>CD at third descent start</t>
+  </si>
+  <si>
+    <t>CD at third descent ending</t>
+  </si>
+  <si>
+    <t>Efficiency at third descent start</t>
+  </si>
+  <si>
+    <t>Efficiency at third descent ending</t>
+  </si>
+  <si>
+    <t>Thrust at third descent start</t>
+  </si>
+  <si>
+    <t>Thrust at third descent ending</t>
+  </si>
+  <si>
+    <t>Drag at third descent start</t>
+  </si>
+  <si>
+    <t>Drag at third descent ending</t>
+  </si>
+  <si>
     <t>LANDING</t>
   </si>
   <si>
@@ -591,6 +817,39 @@
   </si>
   <si>
     <t>Drag at landing ending</t>
+  </si>
+  <si>
+    <t>ALTITUDE</t>
+  </si>
+  <si>
+    <t>MACH</t>
+  </si>
+  <si>
+    <t>RANGE AT MAX PAYLOAD</t>
+  </si>
+  <si>
+    <t>Range</t>
+  </si>
+  <si>
+    <t>Aircraft mass</t>
+  </si>
+  <si>
+    <t>Payload mass</t>
+  </si>
+  <si>
+    <t>Passengers number</t>
+  </si>
+  <si>
+    <t>Fuel mass</t>
+  </si>
+  <si>
+    <t>RANGE AT DESIGN PAYLOAD</t>
+  </si>
+  <si>
+    <t>RANGE AT MAX FUEL</t>
+  </si>
+  <si>
+    <t>RANGE AT ZERO PAYLOAD</t>
   </si>
   <si>
     <t>REGULATION</t>
@@ -776,7 +1035,7 @@
         <v>4</v>
       </c>
       <c r="C2" t="n">
-        <v>820.1901944347959</v>
+        <v>763.4976658579075</v>
       </c>
     </row>
     <row r="3">
@@ -787,7 +1046,7 @@
         <v>4</v>
       </c>
       <c r="C3" t="n">
-        <v>171.97099748369703</v>
+        <v>165.49835580099966</v>
       </c>
     </row>
     <row r="4">
@@ -798,7 +1057,7 @@
         <v>4</v>
       </c>
       <c r="C4" t="n">
-        <v>253.4315226066753</v>
+        <v>231.54652743043323</v>
       </c>
     </row>
     <row r="5">
@@ -809,7 +1068,7 @@
         <v>4</v>
       </c>
       <c r="C5" t="n">
-        <v>1245.592714525168</v>
+        <v>1160.5425490893404</v>
       </c>
     </row>
     <row r="6">
@@ -820,7 +1079,7 @@
         <v>4</v>
       </c>
       <c r="C6" t="n">
-        <v>1432.4316217039432</v>
+        <v>1334.623931452741</v>
       </c>
     </row>
     <row r="7">
@@ -831,7 +1090,7 @@
         <v>4</v>
       </c>
       <c r="C7" t="n">
-        <v>1289.124701462595</v>
+        <v>1225.6636069691126</v>
       </c>
     </row>
     <row r="8">
@@ -847,7 +1106,7 @@
         <v>11</v>
       </c>
       <c r="C9" t="n">
-        <v>2690.9127114002495</v>
+        <v>2504.913601896022</v>
       </c>
     </row>
     <row r="10">
@@ -858,7 +1117,7 @@
         <v>11</v>
       </c>
       <c r="C10" t="n">
-        <v>564.2093093297148</v>
+        <v>542.9736082709964</v>
       </c>
     </row>
     <row r="11">
@@ -869,7 +1128,7 @@
         <v>11</v>
       </c>
       <c r="C11" t="n">
-        <v>831.4682500219006</v>
+        <v>759.6670847455159</v>
       </c>
     </row>
     <row r="12">
@@ -880,7 +1139,7 @@
         <v>11</v>
       </c>
       <c r="C12" t="n">
-        <v>4086.5902707518644</v>
+        <v>3807.554294912534</v>
       </c>
     </row>
     <row r="13">
@@ -891,7 +1150,7 @@
         <v>11</v>
       </c>
       <c r="C13" t="n">
-        <v>4699.578811364643</v>
+        <v>4378.687439149413</v>
       </c>
     </row>
     <row r="14">
@@ -902,7 +1161,7 @@
         <v>11</v>
       </c>
       <c r="C14" t="n">
-        <v>4229.411750205365</v>
+        <v>4021.2060596099504</v>
       </c>
     </row>
     <row r="15">
@@ -918,7 +1177,7 @@
         <v>13</v>
       </c>
       <c r="C16" t="n">
-        <v>54.464737105769856</v>
+        <v>53.67149021492679</v>
       </c>
     </row>
     <row r="17">
@@ -929,7 +1188,7 @@
         <v>13</v>
       </c>
       <c r="C17" t="n">
-        <v>56.618247732075716</v>
+        <v>55.82318509291505</v>
       </c>
     </row>
     <row r="18">
@@ -940,7 +1199,7 @@
         <v>13</v>
       </c>
       <c r="C18" t="n">
-        <v>57.187973961058354</v>
+        <v>56.35506472567313</v>
       </c>
     </row>
     <row r="19">
@@ -951,7 +1210,7 @@
         <v>13</v>
       </c>
       <c r="C19" t="n">
-        <v>47.05934230489444</v>
+        <v>46.98027510783356</v>
       </c>
     </row>
     <row r="20">
@@ -962,7 +1221,7 @@
         <v>13</v>
       </c>
       <c r="C20" t="n">
-        <v>61.50624032441149</v>
+        <v>60.77409553733331</v>
       </c>
     </row>
     <row r="21">
@@ -973,7 +1232,7 @@
         <v>13</v>
       </c>
       <c r="C21" t="n">
-        <v>64.90358632965845</v>
+        <v>63.95159766929473</v>
       </c>
     </row>
     <row r="22">
@@ -989,7 +1248,7 @@
         <v>19</v>
       </c>
       <c r="C23" t="n">
-        <v>105.87097925527618</v>
+        <v>104.32903065536526</v>
       </c>
     </row>
     <row r="24">
@@ -1000,7 +1259,7 @@
         <v>19</v>
       </c>
       <c r="C24" t="n">
-        <v>110.05706902563315</v>
+        <v>108.51159089335539</v>
       </c>
     </row>
     <row r="25">
@@ -1011,7 +1270,7 @@
         <v>19</v>
       </c>
       <c r="C25" t="n">
-        <v>111.16452821804</v>
+        <v>109.54548218813352</v>
       </c>
     </row>
     <row r="26">
@@ -1022,7 +1281,7 @@
         <v>19</v>
       </c>
       <c r="C26" t="n">
-        <v>91.47604335724623</v>
+        <v>91.32234902170673</v>
       </c>
     </row>
     <row r="27">
@@ -1033,7 +1292,7 @@
         <v>19</v>
       </c>
       <c r="C27" t="n">
-        <v>119.5585665053355</v>
+        <v>118.13539089330449</v>
       </c>
     </row>
     <row r="28">
@@ -1044,7 +1303,7 @@
         <v>19</v>
       </c>
       <c r="C28" t="n">
-        <v>126.16247882654991</v>
+        <v>124.31196091223597</v>
       </c>
     </row>
     <row r="29">
@@ -1060,7 +1319,7 @@
         <v>21</v>
       </c>
       <c r="C30" t="n">
-        <v>1.0395395395395695</v>
+        <v>1.0400900900901355</v>
       </c>
     </row>
     <row r="31">
@@ -1082,7 +1341,7 @@
         <v>10</v>
       </c>
       <c r="C32" t="n">
-        <v>0.8640332223307305</v>
+        <v>0.8753301784560417</v>
       </c>
     </row>
     <row r="33">
@@ -1093,7 +1352,7 @@
         <v>21</v>
       </c>
       <c r="C33" t="n">
-        <v>1.1292855449750379</v>
+        <v>1.1323347888043394</v>
       </c>
     </row>
     <row r="34">
@@ -1104,7 +1363,7 @@
         <v>21</v>
       </c>
       <c r="C34" t="n">
-        <v>1.1916625284285587</v>
+        <v>1.1915375819303948</v>
       </c>
     </row>
     <row r="35">
@@ -1120,7 +1379,7 @@
         <v>27</v>
       </c>
       <c r="C36" t="n">
-        <v>33.27508147413059</v>
+        <v>31.518246828443218</v>
       </c>
     </row>
   </sheetData>
@@ -1155,7 +1414,7 @@
         <v>4</v>
       </c>
       <c r="C2" t="n">
-        <v>8389.713722230805</v>
+        <v>8634.888420929987</v>
       </c>
     </row>
     <row r="3">
@@ -1166,7 +1425,7 @@
         <v>11</v>
       </c>
       <c r="C3" t="n">
-        <v>27525.307487633865</v>
+        <v>28329.686420373968</v>
       </c>
     </row>
     <row r="4">
@@ -1177,7 +1436,7 @@
         <v>4</v>
       </c>
       <c r="C4" t="n">
-        <v>7887.1549137230795</v>
+        <v>8140.8101902966755</v>
       </c>
     </row>
     <row r="5">
@@ -1188,7 +1447,7 @@
         <v>11</v>
       </c>
       <c r="C5" t="n">
-        <v>25876.492499091466</v>
+        <v>26708.694850054708</v>
       </c>
     </row>
     <row r="6">
@@ -1199,7 +1458,7 @@
         <v>31</v>
       </c>
       <c r="C6" t="n">
-        <v>16.699590742048024</v>
+        <v>15.631361120702934</v>
       </c>
     </row>
     <row r="7">
@@ -1210,7 +1469,7 @@
         <v>31</v>
       </c>
       <c r="C7" t="n">
-        <v>16.872418183790067</v>
+        <v>15.785596169403902</v>
       </c>
     </row>
     <row r="8">
@@ -1221,7 +1480,7 @@
         <v>34</v>
       </c>
       <c r="C8" t="n">
-        <v>247.75473501228663</v>
+        <v>232.1515284295877</v>
       </c>
     </row>
     <row r="9">
@@ -1237,7 +1496,7 @@
         <v>4</v>
       </c>
       <c r="C10" t="n">
-        <v>4831.174938981165</v>
+        <v>5106.702253236044</v>
       </c>
     </row>
     <row r="11">
@@ -1248,7 +1507,7 @@
         <v>11</v>
       </c>
       <c r="C11" t="n">
-        <v>15850.311479596998</v>
+        <v>16754.27248437022</v>
       </c>
     </row>
     <row r="12">
@@ -1259,7 +1518,7 @@
         <v>4</v>
       </c>
       <c r="C12" t="n">
-        <v>4202.371836316846</v>
+        <v>4484.06741607492</v>
       </c>
     </row>
     <row r="13">
@@ -1270,7 +1529,7 @@
         <v>11</v>
       </c>
       <c r="C13" t="n">
-        <v>13787.309174267866</v>
+        <v>14711.507270587008</v>
       </c>
     </row>
   </sheetData>
@@ -1327,7 +1586,7 @@
         <v>38</v>
       </c>
       <c r="C4" t="n">
-        <v>15954.254589964348</v>
+        <v>15739.665100655897</v>
       </c>
     </row>
     <row r="5">
@@ -1338,7 +1597,7 @@
         <v>39</v>
       </c>
       <c r="C5" t="n">
-        <v>3586.65911231359</v>
+        <v>3538.4174760218502</v>
       </c>
     </row>
     <row r="6">
@@ -1376,7 +1635,7 @@
         <v>42</v>
       </c>
       <c r="C9" t="n">
-        <v>2142950.30043518</v>
+        <v>2114126.978857182</v>
       </c>
     </row>
     <row r="10">
@@ -1387,7 +1646,7 @@
         <v>43</v>
       </c>
       <c r="C10" t="n">
-        <v>2913.6005629309884</v>
+        <v>2874.4117651515253</v>
       </c>
     </row>
     <row r="11">
@@ -1403,7 +1662,7 @@
         <v>13</v>
       </c>
       <c r="C12" t="n">
-        <v>62.05954013778687</v>
+        <v>61.15567940371504</v>
       </c>
     </row>
     <row r="13">
@@ -1414,7 +1673,7 @@
         <v>13</v>
       </c>
       <c r="C13" t="n">
-        <v>107.49162397919065</v>
+        <v>108.10352611901291</v>
       </c>
     </row>
     <row r="14">
@@ -1425,7 +1684,7 @@
         <v>19</v>
       </c>
       <c r="C14" t="n">
-        <v>120.63409530023365</v>
+        <v>118.87713059037479</v>
       </c>
     </row>
     <row r="15">
@@ -1436,7 +1695,7 @@
         <v>19</v>
       </c>
       <c r="C15" t="n">
-        <v>208.94700125544614</v>
+        <v>210.1364438598523</v>
       </c>
     </row>
     <row r="16">
@@ -1452,7 +1711,7 @@
         <v>13</v>
       </c>
       <c r="C17" t="n">
-        <v>80.8318141519373</v>
+        <v>79.65454627799696</v>
       </c>
     </row>
     <row r="18">
@@ -1463,7 +1722,7 @@
         <v>13</v>
       </c>
       <c r="C18" t="n">
-        <v>140.00574111161944</v>
+        <v>140.80272224893366</v>
       </c>
     </row>
     <row r="19">
@@ -1474,7 +1733,7 @@
         <v>19</v>
       </c>
       <c r="C19" t="n">
-        <v>157.1244767532258</v>
+        <v>154.83605108033964</v>
       </c>
     </row>
     <row r="20">
@@ -1485,7 +1744,7 @@
         <v>19</v>
       </c>
       <c r="C20" t="n">
-        <v>272.14938876988657</v>
+        <v>273.69859616423383</v>
       </c>
     </row>
     <row r="21">
@@ -1501,7 +1760,7 @@
         <v>21</v>
       </c>
       <c r="C22" t="n">
-        <v>0.25275318816835946</v>
+        <v>0.24907198650799223</v>
       </c>
     </row>
     <row r="23">
@@ -1512,7 +1771,7 @@
         <v>21</v>
       </c>
       <c r="C23" t="n">
-        <v>0.43778367512164784</v>
+        <v>0.4402757469356548</v>
       </c>
     </row>
     <row r="24">
@@ -1528,7 +1787,7 @@
         <v>21</v>
       </c>
       <c r="C25" t="n">
-        <v>13.554284070670356</v>
+        <v>13.343608894007511</v>
       </c>
     </row>
     <row r="26">
@@ -1601,7 +1860,7 @@
         <v>34</v>
       </c>
       <c r="C5" t="n">
-        <v>75.33649432078079</v>
+        <v>76.87260908157373</v>
       </c>
     </row>
   </sheetData>
@@ -1636,7 +1895,7 @@
         <v>4</v>
       </c>
       <c r="C2" t="n">
-        <v>374.25537032206677</v>
+        <v>363.4072353153997</v>
       </c>
     </row>
     <row r="3">
@@ -1647,7 +1906,7 @@
         <v>4</v>
       </c>
       <c r="C3" t="n">
-        <v>88.67725815729722</v>
+        <v>86.1130042528782</v>
       </c>
     </row>
     <row r="4">
@@ -1658,7 +1917,7 @@
         <v>4</v>
       </c>
       <c r="C4" t="n">
-        <v>246.48829715062072</v>
+        <v>247.76954494518867</v>
       </c>
     </row>
     <row r="5">
@@ -1669,7 +1928,7 @@
         <v>4</v>
       </c>
       <c r="C5" t="n">
-        <v>709.4209256299848</v>
+        <v>697.2897845134667</v>
       </c>
     </row>
     <row r="6">
@@ -1680,7 +1939,7 @@
         <v>4</v>
       </c>
       <c r="C6" t="n">
-        <v>1182.3682093833079</v>
+        <v>1162.1496408557775</v>
       </c>
     </row>
     <row r="7">
@@ -1696,7 +1955,7 @@
         <v>11</v>
       </c>
       <c r="C8" t="n">
-        <v>1227.871949875547</v>
+        <v>1192.2809557591854</v>
       </c>
     </row>
     <row r="9">
@@ -1707,7 +1966,7 @@
         <v>11</v>
       </c>
       <c r="C9" t="n">
-        <v>290.9358863428386</v>
+        <v>282.52297983227754</v>
       </c>
     </row>
     <row r="10">
@@ -1718,7 +1977,7 @@
         <v>11</v>
       </c>
       <c r="C10" t="n">
-        <v>808.688638945606</v>
+        <v>812.892207825422</v>
       </c>
     </row>
     <row r="11">
@@ -1729,7 +1988,7 @@
         <v>11</v>
       </c>
       <c r="C11" t="n">
-        <v>2327.496475163992</v>
+        <v>2287.6961434168848</v>
       </c>
     </row>
     <row r="12">
@@ -1740,7 +1999,7 @@
         <v>11</v>
       </c>
       <c r="C12" t="n">
-        <v>3879.1607919399858</v>
+        <v>3812.8269056948084</v>
       </c>
     </row>
     <row r="13">
@@ -1756,7 +2015,7 @@
         <v>13</v>
       </c>
       <c r="C14" t="n">
-        <v>46.8679837441297</v>
+        <v>46.185379101920276</v>
       </c>
     </row>
     <row r="15">
@@ -1767,7 +2026,7 @@
         <v>13</v>
       </c>
       <c r="C15" t="n">
-        <v>53.898181305749155</v>
+        <v>53.11318596720832</v>
       </c>
     </row>
     <row r="16">
@@ -1778,7 +2037,7 @@
         <v>13</v>
       </c>
       <c r="C16" t="n">
-        <v>57.647620005279535</v>
+        <v>56.80801629536194</v>
       </c>
     </row>
     <row r="17">
@@ -1789,7 +2048,7 @@
         <v>13</v>
       </c>
       <c r="C17" t="n">
-        <v>60.928378867368615</v>
+        <v>60.04099283249636</v>
       </c>
     </row>
     <row r="18">
@@ -1805,7 +2064,7 @@
         <v>19</v>
       </c>
       <c r="C19" t="n">
-        <v>91.10407207282232</v>
+        <v>89.77719479854913</v>
       </c>
     </row>
     <row r="20">
@@ -1816,7 +2075,7 @@
         <v>19</v>
       </c>
       <c r="C20" t="n">
-        <v>104.76968288374565</v>
+        <v>103.2437740183315</v>
       </c>
     </row>
     <row r="21">
@@ -1827,7 +2086,7 @@
         <v>19</v>
       </c>
       <c r="C21" t="n">
-        <v>112.05800864957143</v>
+        <v>110.42594960221543</v>
       </c>
     </row>
     <row r="22">
@@ -1838,7 +2097,7 @@
         <v>19</v>
       </c>
       <c r="C22" t="n">
-        <v>118.43529369466901</v>
+        <v>116.71035323811387</v>
       </c>
     </row>
     <row r="23">
@@ -1892,7 +2151,7 @@
         <v>27</v>
       </c>
       <c r="C28" t="n">
-        <v>10.696275141356615</v>
+        <v>10.533536117807454</v>
       </c>
     </row>
   </sheetData>
@@ -1927,7 +2186,7 @@
         <v>53</v>
       </c>
       <c r="C2" t="n">
-        <v>889.9999999999999</v>
+        <v>286.99999999999994</v>
       </c>
     </row>
     <row r="3">
@@ -1938,7 +2197,7 @@
         <v>31</v>
       </c>
       <c r="C3" t="n">
-        <v>199.41438104166684</v>
+        <v>115.16083257114227</v>
       </c>
     </row>
     <row r="4">
@@ -1949,7 +2208,7 @@
         <v>34</v>
       </c>
       <c r="C4" t="n">
-        <v>22242.00184937041</v>
+        <v>21244.515966406383</v>
       </c>
     </row>
     <row r="5">
@@ -1960,7 +2219,7 @@
         <v>34</v>
       </c>
       <c r="C5" t="n">
-        <v>19796.537599805306</v>
+        <v>19945.927592720553</v>
       </c>
     </row>
     <row r="6">
@@ -1971,7 +2230,7 @@
         <v>34</v>
       </c>
       <c r="C6" t="n">
-        <v>2574.001849370414</v>
+        <v>1358.5159664063879</v>
       </c>
     </row>
     <row r="7">
@@ -1982,7 +2241,7 @@
         <v>34</v>
       </c>
       <c r="C7" t="n">
-        <v>2445.301756901894</v>
+        <v>1290.5901680860684</v>
       </c>
     </row>
     <row r="8">
@@ -2031,7 +2290,7 @@
         <v>53</v>
       </c>
       <c r="C12" t="n">
-        <v>0.6128038427281226</v>
+        <v>0.5595260658355462</v>
       </c>
     </row>
     <row r="13">
@@ -2042,7 +2301,7 @@
         <v>53</v>
       </c>
       <c r="C13" t="n">
-        <v>50.43989981482256</v>
+        <v>45.7661957495705</v>
       </c>
     </row>
     <row r="14">
@@ -2053,7 +2312,7 @@
         <v>53</v>
       </c>
       <c r="C14" t="n">
-        <v>789.7656068200988</v>
+        <v>64.01835514932378</v>
       </c>
     </row>
     <row r="15">
@@ -2064,7 +2323,7 @@
         <v>53</v>
       </c>
       <c r="C15" t="n">
-        <v>48.821550358305274</v>
+        <v>45.00256920306859</v>
       </c>
     </row>
     <row r="16">
@@ -2075,7 +2334,7 @@
         <v>53</v>
       </c>
       <c r="C16" t="n">
-        <v>5.3953499445924535E-8</v>
+        <v>17.71563392149615</v>
       </c>
     </row>
     <row r="17">
@@ -2086,7 +2345,7 @@
         <v>53</v>
       </c>
       <c r="C17" t="n">
-        <v>-5.6843418860808015E-14</v>
+        <v>86.99999999999994</v>
       </c>
     </row>
     <row r="18">
@@ -2097,7 +2356,7 @@
         <v>53</v>
       </c>
       <c r="C18" t="n">
-        <v>-5.6843418860808015E-14</v>
+        <v>22.989883486825306</v>
       </c>
     </row>
     <row r="19">
@@ -2119,7 +2378,7 @@
         <v>53</v>
       </c>
       <c r="C20" t="n">
-        <v>-5.6843418860808015E-14</v>
+        <v>3.586709101989584</v>
       </c>
     </row>
     <row r="21">
@@ -2130,7 +2389,7 @@
         <v>53</v>
       </c>
       <c r="C21" t="n">
-        <v>0.36013875031244424</v>
+        <v>0.3616593451248207</v>
       </c>
     </row>
     <row r="22">
@@ -2146,7 +2405,7 @@
         <v>31</v>
       </c>
       <c r="C23" t="n">
-        <v>0.5158269566862803</v>
+        <v>0.47922495840064394</v>
       </c>
     </row>
     <row r="24">
@@ -2157,7 +2416,7 @@
         <v>31</v>
       </c>
       <c r="C24" t="n">
-        <v>15.379457794237194</v>
+        <v>13.980450417403423</v>
       </c>
     </row>
     <row r="25">
@@ -2168,7 +2427,7 @@
         <v>31</v>
       </c>
       <c r="C25" t="n">
-        <v>172.05053230244113</v>
+        <v>13.96627293034787</v>
       </c>
     </row>
     <row r="26">
@@ -2179,7 +2438,7 @@
         <v>31</v>
       </c>
       <c r="C26" t="n">
-        <v>11.299999999999969</v>
+        <v>10.333333333333325</v>
       </c>
     </row>
     <row r="27">
@@ -2190,7 +2449,7 @@
         <v>31</v>
       </c>
       <c r="C27" t="n">
-        <v>1.9176084720129438E-8</v>
+        <v>5.74426203717395</v>
       </c>
     </row>
     <row r="28">
@@ -2201,7 +2460,7 @@
         <v>31</v>
       </c>
       <c r="C28" t="n">
-        <v>-1.4210854715202004E-14</v>
+        <v>18.85473410788719</v>
       </c>
     </row>
     <row r="29">
@@ -2212,7 +2471,7 @@
         <v>31</v>
       </c>
       <c r="C29" t="n">
-        <v>-1.4210854715202004E-14</v>
+        <v>5.666666666666654</v>
       </c>
     </row>
     <row r="30">
@@ -2223,7 +2482,7 @@
         <v>31</v>
       </c>
       <c r="C30" t="n">
-        <v>-1.4210854715202004E-14</v>
+        <v>44.999999999999986</v>
       </c>
     </row>
     <row r="31">
@@ -2234,7 +2493,7 @@
         <v>31</v>
       </c>
       <c r="C31" t="n">
-        <v>-1.4210854715202004E-14</v>
+        <v>0.9666666666666615</v>
       </c>
     </row>
     <row r="32">
@@ -2245,7 +2504,7 @@
         <v>31</v>
       </c>
       <c r="C32" t="n">
-        <v>0.1685639691262253</v>
+        <v>0.16922145326255844</v>
       </c>
     </row>
     <row r="33">
@@ -2261,7 +2520,7 @@
         <v>34</v>
       </c>
       <c r="C34" t="n">
-        <v>9.552727462798055</v>
+        <v>8.873414888612675</v>
       </c>
     </row>
     <row r="35">
@@ -2272,7 +2531,7 @@
         <v>34</v>
       </c>
       <c r="C35" t="n">
-        <v>226.3065221492838</v>
+        <v>206.11321983985948</v>
       </c>
     </row>
     <row r="36">
@@ -2283,7 +2542,7 @@
         <v>34</v>
       </c>
       <c r="C36" t="n">
-        <v>2131.9761732948164</v>
+        <v>173.27197602177455</v>
       </c>
     </row>
     <row r="37">
@@ -2294,7 +2553,7 @@
         <v>34</v>
       </c>
       <c r="C37" t="n">
-        <v>77.0196391472698</v>
+        <v>69.82229920984113</v>
       </c>
     </row>
     <row r="38">
@@ -2305,7 +2564,7 @@
         <v>34</v>
       </c>
       <c r="C38" t="n">
-        <v>3.295419901405694E-7</v>
+        <v>91.60531214164246</v>
       </c>
     </row>
     <row r="39">
@@ -2316,7 +2575,7 @@
         <v>34</v>
       </c>
       <c r="C39" t="n">
-        <v>-2.2737367544323206E-13</v>
+        <v>259.44383659097946</v>
       </c>
     </row>
     <row r="40">
@@ -2327,7 +2586,7 @@
         <v>34</v>
       </c>
       <c r="C40" t="n">
-        <v>-2.2737367544323206E-13</v>
+        <v>39.25435552926234</v>
       </c>
     </row>
     <row r="41">
@@ -2338,7 +2597,7 @@
         <v>34</v>
       </c>
       <c r="C41" t="n">
-        <v>-2.2737367544323206E-13</v>
+        <v>434.99500801305953</v>
       </c>
     </row>
     <row r="42">
@@ -2349,7 +2608,7 @@
         <v>34</v>
       </c>
       <c r="C42" t="n">
-        <v>-2.2737367544323206E-13</v>
+        <v>6.762308999891161</v>
       </c>
     </row>
     <row r="43">
@@ -2360,7 +2619,7 @@
         <v>34</v>
       </c>
       <c r="C43" t="n">
-        <v>0.4466945181841311</v>
+        <v>0.4484368511456296</v>
       </c>
     </row>
     <row r="44">
@@ -2376,7 +2635,7 @@
         <v>34</v>
       </c>
       <c r="C45" t="n">
-        <v>22232.28662924442</v>
+        <v>21227.644345918023</v>
       </c>
     </row>
     <row r="46">
@@ -2387,7 +2646,7 @@
         <v>34</v>
       </c>
       <c r="C46" t="n">
-        <v>22005.980107095136</v>
+        <v>21021.531126078164</v>
       </c>
     </row>
     <row r="47">
@@ -2398,7 +2657,7 @@
         <v>34</v>
       </c>
       <c r="C47" t="n">
-        <v>19874.003933800315</v>
+        <v>20848.259150056387</v>
       </c>
     </row>
     <row r="48">
@@ -2409,7 +2668,7 @@
         <v>34</v>
       </c>
       <c r="C48" t="n">
-        <v>19796.98429465304</v>
+        <v>20778.436850846545</v>
       </c>
     </row>
     <row r="49">
@@ -2420,7 +2679,7 @@
         <v>34</v>
       </c>
       <c r="C49" t="n">
-        <v>19796.984294323498</v>
+        <v>20686.8315387049</v>
       </c>
     </row>
     <row r="50">
@@ -2431,7 +2690,7 @@
         <v>34</v>
       </c>
       <c r="C50" t="n">
-        <v>19796.984294323498</v>
+        <v>20427.38770211392</v>
       </c>
     </row>
     <row r="51">
@@ -2442,7 +2701,7 @@
         <v>34</v>
       </c>
       <c r="C51" t="n">
-        <v>19796.984294323494</v>
+        <v>20388.133346584655</v>
       </c>
     </row>
     <row r="52">
@@ -2453,7 +2712,7 @@
         <v>34</v>
       </c>
       <c r="C52" t="n">
-        <v>19796.98429432349</v>
+        <v>19953.138338571596</v>
       </c>
     </row>
     <row r="53">
@@ -2464,7 +2723,7 @@
         <v>34</v>
       </c>
       <c r="C53" t="n">
-        <v>19796.98429432349</v>
+        <v>19946.3760295717</v>
       </c>
     </row>
     <row r="54">
@@ -2475,7 +2734,7 @@
         <v>34</v>
       </c>
       <c r="C54" t="n">
-        <v>19796.537599805306</v>
+        <v>19945.927592720553</v>
       </c>
     </row>
     <row r="55">
@@ -2507,7 +2766,7 @@
         <v>19</v>
       </c>
       <c r="C58" t="n">
-        <v>123.89567374302489</v>
+        <v>122.10051401488093</v>
       </c>
     </row>
     <row r="59">
@@ -2529,7 +2788,7 @@
         <v>10</v>
       </c>
       <c r="C60" t="n">
-        <v>0.18732366366290265</v>
+        <v>0.18460947771131322</v>
       </c>
     </row>
     <row r="61">
@@ -2551,7 +2810,7 @@
         <v>10</v>
       </c>
       <c r="C62" t="n">
-        <v>1.744269853155924</v>
+        <v>1.744193767604694</v>
       </c>
     </row>
     <row r="63">
@@ -2573,7 +2832,7 @@
         <v>10</v>
       </c>
       <c r="C64" t="n">
-        <v>0.10506502500286752</v>
+        <v>0.10506119205958955</v>
       </c>
     </row>
     <row r="65">
@@ -2595,7 +2854,7 @@
         <v>10</v>
       </c>
       <c r="C66" t="n">
-        <v>16.601812573768655</v>
+        <v>16.601694054788627</v>
       </c>
     </row>
     <row r="67">
@@ -2606,7 +2865,7 @@
         <v>127</v>
       </c>
       <c r="C67" t="n">
-        <v>15377.592657289946</v>
+        <v>15377.591973895382</v>
       </c>
     </row>
     <row r="68">
@@ -2617,7 +2876,7 @@
         <v>127</v>
       </c>
       <c r="C68" t="n">
-        <v>10211.893754387842</v>
+        <v>10301.87436748788</v>
       </c>
     </row>
     <row r="69">
@@ -2639,7 +2898,7 @@
         <v>127</v>
       </c>
       <c r="C70" t="n">
-        <v>3585.2795467772175</v>
+        <v>3482.008929775164</v>
       </c>
     </row>
     <row r="71">
@@ -2704,7 +2963,7 @@
         <v>10</v>
       </c>
       <c r="C77" t="n">
-        <v>0.7629006372652537</v>
+        <v>0.7284263498941497</v>
       </c>
     </row>
     <row r="78">
@@ -2715,7 +2974,7 @@
         <v>10</v>
       </c>
       <c r="C78" t="n">
-        <v>1.2810597242180017</v>
+        <v>1.223750850266885</v>
       </c>
     </row>
     <row r="79">
@@ -2726,7 +2985,7 @@
         <v>10</v>
       </c>
       <c r="C79" t="n">
-        <v>0.04920264659647413</v>
+        <v>0.0475598885442971</v>
       </c>
     </row>
     <row r="80">
@@ -2737,7 +2996,7 @@
         <v>10</v>
       </c>
       <c r="C80" t="n">
-        <v>0.08304200242216361</v>
+        <v>0.07844878633588735</v>
       </c>
     </row>
     <row r="81">
@@ -2748,7 +3007,7 @@
         <v>10</v>
       </c>
       <c r="C81" t="n">
-        <v>15.50527644421313</v>
+        <v>15.315981012354477</v>
       </c>
     </row>
     <row r="82">
@@ -2759,7 +3018,7 @@
         <v>10</v>
       </c>
       <c r="C82" t="n">
-        <v>15.426647802944736</v>
+        <v>15.599359880817753</v>
       </c>
     </row>
     <row r="83">
@@ -2770,7 +3029,7 @@
         <v>127</v>
       </c>
       <c r="C83" t="n">
-        <v>7251.752393790313</v>
+        <v>7251.752393790312</v>
       </c>
     </row>
     <row r="84">
@@ -2792,7 +3051,7 @@
         <v>127</v>
       </c>
       <c r="C85" t="n">
-        <v>3161.195314538425</v>
+        <v>3055.5642363365964</v>
       </c>
     </row>
     <row r="86">
@@ -2803,7 +3062,7 @@
         <v>127</v>
       </c>
       <c r="C86" t="n">
-        <v>3185.8992853351724</v>
+        <v>3006.9181577574936</v>
       </c>
     </row>
     <row r="87">
@@ -2824,7 +3083,7 @@
         <v>19</v>
       </c>
       <c r="C89" t="n">
-        <v>271.96258280390896</v>
+        <v>274.9099468658059</v>
       </c>
     </row>
     <row r="90">
@@ -2835,7 +3094,7 @@
         <v>19</v>
       </c>
       <c r="C90" t="n">
-        <v>279.8678110221731</v>
+        <v>275.37851812423855</v>
       </c>
     </row>
     <row r="91">
@@ -2846,7 +3105,7 @@
         <v>10</v>
       </c>
       <c r="C91" t="n">
-        <v>0.4374831676628926</v>
+        <v>0.44222434254349796</v>
       </c>
     </row>
     <row r="92">
@@ -2857,7 +3116,7 @@
         <v>10</v>
       </c>
       <c r="C92" t="n">
-        <v>0.4501996386066835</v>
+        <v>0.4429780934319527</v>
       </c>
     </row>
     <row r="93">
@@ -2868,7 +3127,7 @@
         <v>10</v>
       </c>
       <c r="C93" t="n">
-        <v>0.500551660297655</v>
+        <v>0.4679613029799353</v>
       </c>
     </row>
     <row r="94">
@@ -2879,7 +3138,7 @@
         <v>10</v>
       </c>
       <c r="C94" t="n">
-        <v>0.4030830105612305</v>
+        <v>0.46059706677249074</v>
       </c>
     </row>
     <row r="95">
@@ -2890,7 +3149,7 @@
         <v>10</v>
       </c>
       <c r="C95" t="n">
-        <v>0.03861113678372894</v>
+        <v>0.03760395098579889</v>
       </c>
     </row>
     <row r="96">
@@ -2901,7 +3160,7 @@
         <v>10</v>
       </c>
       <c r="C96" t="n">
-        <v>0.035800210390200975</v>
+        <v>0.037379706993218506</v>
       </c>
     </row>
     <row r="97">
@@ -2912,7 +3171,7 @@
         <v>10</v>
       </c>
       <c r="C97" t="n">
-        <v>12.963919272860975</v>
+        <v>12.444471676836846</v>
       </c>
     </row>
     <row r="98">
@@ -2923,7 +3182,7 @@
         <v>10</v>
       </c>
       <c r="C98" t="n">
-        <v>11.2592358024678</v>
+        <v>12.322115495877297</v>
       </c>
     </row>
     <row r="99">
@@ -2934,7 +3193,7 @@
         <v>127</v>
       </c>
       <c r="C99" t="n">
-        <v>3742.300498709402</v>
+        <v>3724.10691831234</v>
       </c>
     </row>
     <row r="100">
@@ -2945,7 +3204,7 @@
         <v>127</v>
       </c>
       <c r="C100" t="n">
-        <v>3674.5083292307663</v>
+        <v>3714.529101451155</v>
       </c>
     </row>
     <row r="101">
@@ -2956,7 +3215,7 @@
         <v>127</v>
       </c>
       <c r="C101" t="n">
-        <v>3742.300498709402</v>
+        <v>3724.10691831234</v>
       </c>
     </row>
     <row r="102">
@@ -2967,7 +3226,7 @@
         <v>127</v>
       </c>
       <c r="C102" t="n">
-        <v>3674.5083292307663</v>
+        <v>3714.529101451155</v>
       </c>
     </row>
     <row r="103">
@@ -2999,7 +3258,7 @@
         <v>19</v>
       </c>
       <c r="C106" t="n">
-        <v>234.4604898955982</v>
+        <v>238.34927482104573</v>
       </c>
     </row>
     <row r="107">
@@ -3021,7 +3280,7 @@
         <v>10</v>
       </c>
       <c r="C108" t="n">
-        <v>0.35451006603783813</v>
+        <v>0.3622005138224198</v>
       </c>
     </row>
     <row r="109">
@@ -3032,7 +3291,7 @@
         <v>10</v>
       </c>
       <c r="C109" t="n">
-        <v>0.40666872142055804</v>
+        <v>0.4266042675969548</v>
       </c>
     </row>
     <row r="110">
@@ -3043,7 +3302,7 @@
         <v>10</v>
       </c>
       <c r="C110" t="n">
-        <v>0.4038747831942766</v>
+        <v>0.4240691085739158</v>
       </c>
     </row>
     <row r="111">
@@ -3054,7 +3313,7 @@
         <v>10</v>
       </c>
       <c r="C111" t="n">
-        <v>0.03589349809087134</v>
+        <v>0.036416839198585446</v>
       </c>
     </row>
     <row r="112">
@@ -3065,7 +3324,7 @@
         <v>10</v>
       </c>
       <c r="C112" t="n">
-        <v>0.035820809554854324</v>
+        <v>0.03634619552577141</v>
       </c>
     </row>
     <row r="113">
@@ -3076,7 +3335,7 @@
         <v>10</v>
       </c>
       <c r="C113" t="n">
-        <v>11.329871510182636</v>
+        <v>11.714478164088595</v>
       </c>
     </row>
     <row r="114">
@@ -3087,7 +3346,7 @@
         <v>10</v>
       </c>
       <c r="C114" t="n">
-        <v>11.274864756359053</v>
+        <v>11.667496485931462</v>
       </c>
     </row>
     <row r="115">
@@ -3098,7 +3357,7 @@
         <v>127</v>
       </c>
       <c r="C115" t="n">
-        <v>1597.4725804410991</v>
+        <v>1544.7060950880432</v>
       </c>
     </row>
     <row r="116">
@@ -3109,7 +3368,7 @@
         <v>127</v>
       </c>
       <c r="C116" t="n">
-        <v>1105.2541827082787</v>
+        <v>1092.4254312491216</v>
       </c>
     </row>
     <row r="117">
@@ -3120,7 +3379,7 @@
         <v>127</v>
       </c>
       <c r="C117" t="n">
-        <v>3862.012220316379</v>
+        <v>3918.32185467603</v>
       </c>
     </row>
     <row r="118">
@@ -3131,7 +3390,7 @@
         <v>127</v>
       </c>
       <c r="C118" t="n">
-        <v>3854.191193408835</v>
+        <v>3910.7208477470003</v>
       </c>
     </row>
     <row r="119">
@@ -3152,7 +3411,7 @@
         <v>19</v>
       </c>
       <c r="C121" t="n">
-        <v>112.31967575827062</v>
+        <v>173.79162760888562</v>
       </c>
     </row>
     <row r="122">
@@ -3163,7 +3422,7 @@
         <v>19</v>
       </c>
       <c r="C122" t="n">
-        <v>0.0</v>
+        <v>197.80949693813608</v>
       </c>
     </row>
     <row r="123">
@@ -3174,7 +3433,7 @@
         <v>10</v>
       </c>
       <c r="C123" t="n">
-        <v>0.16983013081710976</v>
+        <v>0.26409737082369705</v>
       </c>
     </row>
     <row r="124">
@@ -3185,7 +3444,7 @@
         <v>10</v>
       </c>
       <c r="C124" t="n">
-        <v>0.0</v>
+        <v>0.3098788369360525</v>
       </c>
     </row>
     <row r="125">
@@ -3196,7 +3455,7 @@
         <v>10</v>
       </c>
       <c r="C125" t="n">
-        <v>1.558491941001957</v>
+        <v>0.7130118234530495</v>
       </c>
     </row>
     <row r="126">
@@ -3207,7 +3466,7 @@
         <v>10</v>
       </c>
       <c r="C126" t="n">
-        <v>1.4387</v>
+        <v>0.9196327151349645</v>
       </c>
     </row>
     <row r="127">
@@ -3218,7 +3477,7 @@
         <v>10</v>
       </c>
       <c r="C127" t="n">
-        <v>0.20344099009247918</v>
+        <v>0.04685129770945638</v>
       </c>
     </row>
     <row r="128">
@@ -3229,7 +3488,7 @@
         <v>10</v>
       </c>
       <c r="C128" t="n">
-        <v>0.19153799598718918</v>
+        <v>0.05762859327321252</v>
       </c>
     </row>
     <row r="129">
@@ -3240,7 +3499,7 @@
         <v>10</v>
       </c>
       <c r="C129" t="n">
-        <v>7.660658455768947</v>
+        <v>15.218614175315286</v>
       </c>
     </row>
     <row r="130">
@@ -3251,7 +3510,7 @@
         <v>10</v>
       </c>
       <c r="C130" t="n">
-        <v>7.511303397453454</v>
+        <v>15.957924059937744</v>
       </c>
     </row>
     <row r="131">
@@ -3262,7 +3521,7 @@
         <v>127</v>
       </c>
       <c r="C131" t="n">
-        <v>-651.5472391333013</v>
+        <v>7199.414490810044</v>
       </c>
     </row>
     <row r="132">
@@ -3273,7 +3532,7 @@
         <v>127</v>
       </c>
       <c r="C132" t="n">
-        <v>49.50742544941821</v>
+        <v>6274.189210039074</v>
       </c>
     </row>
     <row r="133">
@@ -3284,7 +3543,7 @@
         <v>127</v>
       </c>
       <c r="C133" t="n">
-        <v>3349.2242670285573</v>
+        <v>2972.1749957884977</v>
       </c>
     </row>
     <row r="134">
@@ -3295,6 +3554,826 @@
         <v>127</v>
       </c>
       <c r="C134" t="n">
+        <v>2865.3751901435826</v>
+      </c>
+    </row>
+    <row r="135">
+      <c r="A135" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="136">
+      <c r="A136" t="s">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="137">
+      <c r="A137" t="s">
+        <v>192</v>
+      </c>
+      <c r="B137" t="s">
+        <v>19</v>
+      </c>
+      <c r="C137" t="n">
+        <v>276.3512340638369</v>
+      </c>
+    </row>
+    <row r="138">
+      <c r="A138" t="s">
+        <v>193</v>
+      </c>
+      <c r="B138" t="s">
+        <v>19</v>
+      </c>
+      <c r="C138" t="n">
+        <v>276.3512340638369</v>
+      </c>
+    </row>
+    <row r="139">
+      <c r="A139" t="s">
+        <v>194</v>
+      </c>
+      <c r="B139" t="s">
+        <v>10</v>
+      </c>
+      <c r="C139" t="n">
+        <v>0.4329185419460757</v>
+      </c>
+    </row>
+    <row r="140">
+      <c r="A140" t="s">
+        <v>195</v>
+      </c>
+      <c r="B140" t="s">
+        <v>10</v>
+      </c>
+      <c r="C140" t="n">
+        <v>0.4329185419460757</v>
+      </c>
+    </row>
+    <row r="141">
+      <c r="A141" t="s">
+        <v>196</v>
+      </c>
+      <c r="B141" t="s">
+        <v>10</v>
+      </c>
+      <c r="C141" t="n">
+        <v>0.36370502134069727</v>
+      </c>
+    </row>
+    <row r="142">
+      <c r="A142" t="s">
+        <v>197</v>
+      </c>
+      <c r="B142" t="s">
+        <v>10</v>
+      </c>
+      <c r="C142" t="n">
+        <v>0.3542744415142043</v>
+      </c>
+    </row>
+    <row r="143">
+      <c r="A143" t="s">
+        <v>198</v>
+      </c>
+      <c r="B143" t="s">
+        <v>10</v>
+      </c>
+      <c r="C143" t="n">
+        <v>0.03483357445319331</v>
+      </c>
+    </row>
+    <row r="144">
+      <c r="A144" t="s">
+        <v>199</v>
+      </c>
+      <c r="B144" t="s">
+        <v>10</v>
+      </c>
+      <c r="C144" t="n">
+        <v>0.034610965461557945</v>
+      </c>
+    </row>
+    <row r="145">
+      <c r="A145" t="s">
+        <v>200</v>
+      </c>
+      <c r="B145" t="s">
+        <v>10</v>
+      </c>
+      <c r="C145" t="n">
+        <v>10.441220203496952</v>
+      </c>
+    </row>
+    <row r="146">
+      <c r="A146" t="s">
+        <v>201</v>
+      </c>
+      <c r="B146" t="s">
+        <v>10</v>
+      </c>
+      <c r="C146" t="n">
+        <v>10.235901737779994</v>
+      </c>
+    </row>
+    <row r="147">
+      <c r="A147" t="s">
+        <v>202</v>
+      </c>
+      <c r="B147" t="s">
+        <v>127</v>
+      </c>
+      <c r="C147" t="n">
+        <v>4367.943199716163</v>
+      </c>
+    </row>
+    <row r="148">
+      <c r="A148" t="s">
+        <v>203</v>
+      </c>
+      <c r="B148" t="s">
+        <v>127</v>
+      </c>
+      <c r="C148" t="n">
+        <v>4371.670125974292</v>
+      </c>
+    </row>
+    <row r="149">
+      <c r="A149" t="s">
+        <v>204</v>
+      </c>
+      <c r="B149" t="s">
+        <v>127</v>
+      </c>
+      <c r="C149" t="n">
+        <v>4367.943199716163</v>
+      </c>
+    </row>
+    <row r="150">
+      <c r="A150" t="s">
+        <v>205</v>
+      </c>
+      <c r="B150" t="s">
+        <v>127</v>
+      </c>
+      <c r="C150" t="n">
+        <v>4371.670125974292</v>
+      </c>
+    </row>
+    <row r="151">
+      <c r="A151" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="152">
+      <c r="A152" t="s">
+        <v>206</v>
+      </c>
+    </row>
+    <row r="153">
+      <c r="A153" t="s">
+        <v>207</v>
+      </c>
+      <c r="B153" t="s">
+        <v>19</v>
+      </c>
+      <c r="C153" t="n">
+        <v>255.9887426167415</v>
+      </c>
+    </row>
+    <row r="154">
+      <c r="A154" t="s">
+        <v>208</v>
+      </c>
+      <c r="B154" t="s">
+        <v>19</v>
+      </c>
+      <c r="C154" t="n">
+        <v>232.1368190562223</v>
+      </c>
+    </row>
+    <row r="155">
+      <c r="A155" t="s">
+        <v>209</v>
+      </c>
+      <c r="B155" t="s">
+        <v>10</v>
+      </c>
+      <c r="C155" t="n">
+        <v>0.4010196429325484</v>
+      </c>
+    </row>
+    <row r="156">
+      <c r="A156" t="s">
+        <v>210</v>
+      </c>
+      <c r="B156" t="s">
+        <v>10</v>
+      </c>
+      <c r="C156" t="n">
+        <v>0.35275993687160867</v>
+      </c>
+    </row>
+    <row r="157">
+      <c r="A157" t="s">
+        <v>211</v>
+      </c>
+      <c r="B157" t="s">
+        <v>10</v>
+      </c>
+      <c r="C157" t="n">
+        <v>0.4178505659080089</v>
+      </c>
+    </row>
+    <row r="158">
+      <c r="A158" t="s">
+        <v>212</v>
+      </c>
+      <c r="B158" t="s">
+        <v>10</v>
+      </c>
+      <c r="C158" t="n">
+        <v>0.4164639410984637</v>
+      </c>
+    </row>
+    <row r="159">
+      <c r="A159" t="s">
+        <v>213</v>
+      </c>
+      <c r="B159" t="s">
+        <v>10</v>
+      </c>
+      <c r="C159" t="n">
+        <v>0.03618441071668287</v>
+      </c>
+    </row>
+    <row r="160">
+      <c r="A160" t="s">
+        <v>214</v>
+      </c>
+      <c r="B160" t="s">
+        <v>10</v>
+      </c>
+      <c r="C160" t="n">
+        <v>0.03614833557140492</v>
+      </c>
+    </row>
+    <row r="161">
+      <c r="A161" t="s">
+        <v>215</v>
+      </c>
+      <c r="B161" t="s">
+        <v>10</v>
+      </c>
+      <c r="C161" t="n">
+        <v>11.54780629646563</v>
+      </c>
+    </row>
+    <row r="162">
+      <c r="A162" t="s">
+        <v>216</v>
+      </c>
+      <c r="B162" t="s">
+        <v>10</v>
+      </c>
+      <c r="C162" t="n">
+        <v>11.520971422759137</v>
+      </c>
+    </row>
+    <row r="163">
+      <c r="A163" t="s">
+        <v>217</v>
+      </c>
+      <c r="B163" t="s">
+        <v>127</v>
+      </c>
+      <c r="C163" t="n">
+        <v>1290.1074946981</v>
+      </c>
+    </row>
+    <row r="164">
+      <c r="A164" t="s">
+        <v>218</v>
+      </c>
+      <c r="B164" t="s">
+        <v>127</v>
+      </c>
+      <c r="C164" t="n">
+        <v>1009.4902177851326</v>
+      </c>
+    </row>
+    <row r="165">
+      <c r="A165" t="s">
+        <v>219</v>
+      </c>
+      <c r="B165" t="s">
+        <v>127</v>
+      </c>
+      <c r="C165" t="n">
+        <v>3893.313380016225</v>
+      </c>
+    </row>
+    <row r="166">
+      <c r="A166" t="s">
+        <v>220</v>
+      </c>
+      <c r="B166" t="s">
+        <v>127</v>
+      </c>
+      <c r="C166" t="n">
+        <v>3889.4318232072346</v>
+      </c>
+    </row>
+    <row r="167">
+      <c r="A167" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="168">
+      <c r="A168" t="s">
+        <v>221</v>
+      </c>
+    </row>
+    <row r="169">
+      <c r="A169" t="s">
+        <v>222</v>
+      </c>
+      <c r="B169" t="s">
+        <v>19</v>
+      </c>
+      <c r="C169" t="n">
+        <v>197.41767258058383</v>
+      </c>
+    </row>
+    <row r="170">
+      <c r="A170" t="s">
+        <v>223</v>
+      </c>
+      <c r="B170" t="s">
+        <v>19</v>
+      </c>
+      <c r="C170" t="n">
+        <v>197.41767258058383</v>
+      </c>
+    </row>
+    <row r="171">
+      <c r="A171" t="s">
+        <v>224</v>
+      </c>
+      <c r="B171" t="s">
+        <v>10</v>
+      </c>
+      <c r="C171" t="n">
+        <v>0.29999999999999993</v>
+      </c>
+    </row>
+    <row r="172">
+      <c r="A172" t="s">
+        <v>225</v>
+      </c>
+      <c r="B172" t="s">
+        <v>10</v>
+      </c>
+      <c r="C172" t="n">
+        <v>0.29999999999999993</v>
+      </c>
+    </row>
+    <row r="173">
+      <c r="A173" t="s">
+        <v>226</v>
+      </c>
+      <c r="B173" t="s">
+        <v>10</v>
+      </c>
+      <c r="C173" t="n">
+        <v>0.5421843406340271</v>
+      </c>
+    </row>
+    <row r="174">
+      <c r="A174" t="s">
+        <v>227</v>
+      </c>
+      <c r="B174" t="s">
+        <v>10</v>
+      </c>
+      <c r="C174" t="n">
+        <v>0.5334974438987716</v>
+      </c>
+    </row>
+    <row r="175">
+      <c r="A175" t="s">
+        <v>228</v>
+      </c>
+      <c r="B175" t="s">
+        <v>10</v>
+      </c>
+      <c r="C175" t="n">
+        <v>0.040001345363663586</v>
+      </c>
+    </row>
+    <row r="176">
+      <c r="A176" t="s">
+        <v>229</v>
+      </c>
+      <c r="B176" t="s">
+        <v>10</v>
+      </c>
+      <c r="C176" t="n">
+        <v>0.03969830905467518</v>
+      </c>
+    </row>
+    <row r="177">
+      <c r="A177" t="s">
+        <v>230</v>
+      </c>
+      <c r="B177" t="s">
+        <v>10</v>
+      </c>
+      <c r="C177" t="n">
+        <v>13.554152634239557</v>
+      </c>
+    </row>
+    <row r="178">
+      <c r="A178" t="s">
+        <v>231</v>
+      </c>
+      <c r="B178" t="s">
+        <v>10</v>
+      </c>
+      <c r="C178" t="n">
+        <v>13.438795167925239</v>
+      </c>
+    </row>
+    <row r="179">
+      <c r="A179" t="s">
+        <v>232</v>
+      </c>
+      <c r="B179" t="s">
+        <v>127</v>
+      </c>
+      <c r="C179" t="n">
+        <v>3316.189599311804</v>
+      </c>
+    </row>
+    <row r="180">
+      <c r="A180" t="s">
+        <v>233</v>
+      </c>
+      <c r="B180" t="s">
+        <v>127</v>
+      </c>
+      <c r="C180" t="n">
+        <v>3291.067297875562</v>
+      </c>
+    </row>
+    <row r="181">
+      <c r="A181" t="s">
+        <v>234</v>
+      </c>
+      <c r="B181" t="s">
+        <v>127</v>
+      </c>
+      <c r="C181" t="n">
+        <v>3316.189599311804</v>
+      </c>
+    </row>
+    <row r="182">
+      <c r="A182" t="s">
+        <v>235</v>
+      </c>
+      <c r="B182" t="s">
+        <v>127</v>
+      </c>
+      <c r="C182" t="n">
+        <v>3291.067297875562</v>
+      </c>
+    </row>
+    <row r="183">
+      <c r="A183" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="184">
+      <c r="A184" t="s">
+        <v>236</v>
+      </c>
+    </row>
+    <row r="185">
+      <c r="A185" t="s">
+        <v>237</v>
+      </c>
+      <c r="B185" t="s">
+        <v>19</v>
+      </c>
+      <c r="C185" t="n">
+        <v>224.90679627393837</v>
+      </c>
+    </row>
+    <row r="186">
+      <c r="A186" t="s">
+        <v>238</v>
+      </c>
+      <c r="B186" t="s">
+        <v>19</v>
+      </c>
+      <c r="C186" t="n">
+        <v>221.33361546517457</v>
+      </c>
+    </row>
+    <row r="187">
+      <c r="A187" t="s">
+        <v>239</v>
+      </c>
+      <c r="B187" t="s">
+        <v>10</v>
+      </c>
+      <c r="C187" t="n">
+        <v>0.3417730439236138</v>
+      </c>
+    </row>
+    <row r="188">
+      <c r="A188" t="s">
+        <v>240</v>
+      </c>
+      <c r="B188" t="s">
+        <v>10</v>
+      </c>
+      <c r="C188" t="n">
+        <v>0.3346619068734856</v>
+      </c>
+    </row>
+    <row r="189">
+      <c r="A189" t="s">
+        <v>241</v>
+      </c>
+      <c r="B189" t="s">
+        <v>10</v>
+      </c>
+      <c r="C189" t="n">
+        <v>0.4079469736554963</v>
+      </c>
+    </row>
+    <row r="190">
+      <c r="A190" t="s">
+        <v>242</v>
+      </c>
+      <c r="B190" t="s">
+        <v>10</v>
+      </c>
+      <c r="C190" t="n">
+        <v>0.40771013939086814</v>
+      </c>
+    </row>
+    <row r="191">
+      <c r="A191" t="s">
+        <v>243</v>
+      </c>
+      <c r="B191" t="s">
+        <v>10</v>
+      </c>
+      <c r="C191" t="n">
+        <v>0.03592675375942698</v>
+      </c>
+    </row>
+    <row r="192">
+      <c r="A192" t="s">
+        <v>244</v>
+      </c>
+      <c r="B192" t="s">
+        <v>10</v>
+      </c>
+      <c r="C192" t="n">
+        <v>0.03592059215720809</v>
+      </c>
+    </row>
+    <row r="193">
+      <c r="A193" t="s">
+        <v>245</v>
+      </c>
+      <c r="B193" t="s">
+        <v>10</v>
+      </c>
+      <c r="C193" t="n">
+        <v>11.354963389879146</v>
+      </c>
+    </row>
+    <row r="194">
+      <c r="A194" t="s">
+        <v>246</v>
+      </c>
+      <c r="B194" t="s">
+        <v>10</v>
+      </c>
+      <c r="C194" t="n">
+        <v>11.35031787912923</v>
+      </c>
+    </row>
+    <row r="195">
+      <c r="A195" t="s">
+        <v>247</v>
+      </c>
+      <c r="B195" t="s">
+        <v>127</v>
+      </c>
+      <c r="C195" t="n">
+        <v>966.6125065433948</v>
+      </c>
+    </row>
+    <row r="196">
+      <c r="A196" t="s">
+        <v>248</v>
+      </c>
+      <c r="B196" t="s">
+        <v>127</v>
+      </c>
+      <c r="C196" t="n">
+        <v>907.8566743950048</v>
+      </c>
+    </row>
+    <row r="197">
+      <c r="A197" t="s">
+        <v>249</v>
+      </c>
+      <c r="B197" t="s">
+        <v>127</v>
+      </c>
+      <c r="C197" t="n">
+        <v>3865.5904114982905</v>
+      </c>
+    </row>
+    <row r="198">
+      <c r="A198" t="s">
+        <v>250</v>
+      </c>
+      <c r="B198" t="s">
+        <v>127</v>
+      </c>
+      <c r="C198" t="n">
+        <v>3864.927445102374</v>
+      </c>
+    </row>
+    <row r="199">
+      <c r="A199" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="200">
+      <c r="A200" t="s">
+        <v>251</v>
+      </c>
+    </row>
+    <row r="201">
+      <c r="A201" t="s">
+        <v>252</v>
+      </c>
+      <c r="B201" t="s">
+        <v>19</v>
+      </c>
+      <c r="C201" t="n">
+        <v>112.74267186559192</v>
+      </c>
+    </row>
+    <row r="202">
+      <c r="A202" t="s">
+        <v>253</v>
+      </c>
+      <c r="B202" t="s">
+        <v>19</v>
+      </c>
+      <c r="C202" t="n">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="203">
+      <c r="A203" t="s">
+        <v>254</v>
+      </c>
+      <c r="B203" t="s">
+        <v>10</v>
+      </c>
+      <c r="C203" t="n">
+        <v>0.1704697114048966</v>
+      </c>
+    </row>
+    <row r="204">
+      <c r="A204" t="s">
+        <v>255</v>
+      </c>
+      <c r="B204" t="s">
+        <v>10</v>
+      </c>
+      <c r="C204" t="n">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="205">
+      <c r="A205" t="s">
+        <v>256</v>
+      </c>
+      <c r="B205" t="s">
+        <v>10</v>
+      </c>
+      <c r="C205" t="n">
+        <v>1.5584919410019569</v>
+      </c>
+    </row>
+    <row r="206">
+      <c r="A206" t="s">
+        <v>257</v>
+      </c>
+      <c r="B206" t="s">
+        <v>10</v>
+      </c>
+      <c r="C206" t="n">
+        <v>1.4387</v>
+      </c>
+    </row>
+    <row r="207">
+      <c r="A207" t="s">
+        <v>258</v>
+      </c>
+      <c r="B207" t="s">
+        <v>10</v>
+      </c>
+      <c r="C207" t="n">
+        <v>0.20344099009247915</v>
+      </c>
+    </row>
+    <row r="208">
+      <c r="A208" t="s">
+        <v>259</v>
+      </c>
+      <c r="B208" t="s">
+        <v>10</v>
+      </c>
+      <c r="C208" t="n">
+        <v>0.19153799598718918</v>
+      </c>
+    </row>
+    <row r="209">
+      <c r="A209" t="s">
+        <v>260</v>
+      </c>
+      <c r="B209" t="s">
+        <v>10</v>
+      </c>
+      <c r="C209" t="n">
+        <v>7.660658455768947</v>
+      </c>
+    </row>
+    <row r="210">
+      <c r="A210" t="s">
+        <v>261</v>
+      </c>
+      <c r="B210" t="s">
+        <v>10</v>
+      </c>
+      <c r="C210" t="n">
+        <v>7.511303397453454</v>
+      </c>
+    </row>
+    <row r="211">
+      <c r="A211" t="s">
+        <v>262</v>
+      </c>
+      <c r="B211" t="s">
+        <v>127</v>
+      </c>
+      <c r="C211" t="n">
+        <v>-655.0452159829897</v>
+      </c>
+    </row>
+    <row r="212">
+      <c r="A212" t="s">
+        <v>263</v>
+      </c>
+      <c r="B212" t="s">
+        <v>127</v>
+      </c>
+      <c r="C212" t="n">
+        <v>49.50742544941821</v>
+      </c>
+    </row>
+    <row r="213">
+      <c r="A213" t="s">
+        <v>264</v>
+      </c>
+      <c r="B213" t="s">
+        <v>127</v>
+      </c>
+      <c r="C213" t="n">
+        <v>3374.506823719656</v>
+      </c>
+    </row>
+    <row r="214">
+      <c r="A214" t="s">
+        <v>265</v>
+      </c>
+      <c r="B214" t="s">
+        <v>127</v>
+      </c>
+      <c r="C214" t="n">
         <v>0.0</v>
       </c>
     </row>
@@ -3324,24 +4403,24 @@
     </row>
     <row r="2">
       <c r="A2" t="s">
-        <v>191</v>
+        <v>266</v>
       </c>
       <c r="B2" t="s">
-        <v>10</v>
-      </c>
-      <c r="C2" t="s">
-        <v>192</v>
+        <v>11</v>
+      </c>
+      <c r="C2" t="n">
+        <v>16999.999999999993</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="s">
-        <v>193</v>
+        <v>267</v>
       </c>
       <c r="B3" t="s">
         <v>10</v>
       </c>
-      <c r="C3" t="s">
-        <v>194</v>
+      <c r="C3" t="n">
+        <v>0.42</v>
       </c>
     </row>
     <row r="4">
@@ -3351,88 +4430,389 @@
     </row>
     <row r="5">
       <c r="A5" t="s">
-        <v>10</v>
+        <v>268</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="s">
-        <v>195</v>
+        <v>269</v>
+      </c>
+      <c r="B6" t="s">
+        <v>53</v>
+      </c>
+      <c r="C6" t="n">
+        <v>559.4420029593741</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="s">
-        <v>196</v>
+        <v>270</v>
+      </c>
+      <c r="B7" t="s">
+        <v>34</v>
+      </c>
+      <c r="C7" t="n">
+        <v>22500.0</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="s">
+        <v>271</v>
+      </c>
+      <c r="B8" t="s">
+        <v>34</v>
+      </c>
+      <c r="C8" t="n">
+        <v>7344.0</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="s">
+        <v>272</v>
+      </c>
+      <c r="B9" t="s">
+        <v>21</v>
+      </c>
+      <c r="C9" t="n">
+        <v>72.0</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="s">
+        <v>273</v>
+      </c>
+      <c r="B10" t="s">
+        <v>34</v>
+      </c>
+      <c r="C10" t="n">
+        <v>2205.999999999998</v>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" t="s">
+        <v>274</v>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" t="s">
+        <v>269</v>
+      </c>
+      <c r="B13" t="s">
+        <v>53</v>
+      </c>
+      <c r="C13" t="n">
+        <v>706.3244922863962</v>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" t="s">
+        <v>270</v>
+      </c>
+      <c r="B14" t="s">
+        <v>34</v>
+      </c>
+      <c r="C14" t="n">
+        <v>22500.0</v>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" t="s">
+        <v>271</v>
+      </c>
+      <c r="B15" t="s">
+        <v>34</v>
+      </c>
+      <c r="C15" t="n">
+        <v>6936.0</v>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" t="s">
+        <v>272</v>
+      </c>
+      <c r="B16" t="s">
+        <v>21</v>
+      </c>
+      <c r="C16" t="n">
+        <v>68.0</v>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" t="s">
+        <v>273</v>
+      </c>
+      <c r="B17" t="s">
+        <v>34</v>
+      </c>
+      <c r="C17" t="n">
+        <v>2613.999999999998</v>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" t="s">
+        <v>275</v>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" t="s">
+        <v>269</v>
+      </c>
+      <c r="B20" t="s">
+        <v>53</v>
+      </c>
+      <c r="C20" t="n">
+        <v>1565.6847666890321</v>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" t="s">
+        <v>270</v>
+      </c>
+      <c r="B21" t="s">
+        <v>34</v>
+      </c>
+      <c r="C21" t="n">
+        <v>22500.0</v>
+      </c>
+    </row>
+    <row r="22">
+      <c r="A22" t="s">
+        <v>271</v>
+      </c>
+      <c r="B22" t="s">
+        <v>34</v>
+      </c>
+      <c r="C22" t="n">
+        <v>4549.999999999998</v>
+      </c>
+    </row>
+    <row r="23">
+      <c r="A23" t="s">
+        <v>272</v>
+      </c>
+      <c r="B23" t="s">
+        <v>21</v>
+      </c>
+      <c r="C23" t="n">
+        <v>45.0</v>
+      </c>
+    </row>
+    <row r="24">
+      <c r="A24" t="s">
+        <v>273</v>
+      </c>
+      <c r="B24" t="s">
+        <v>34</v>
+      </c>
+      <c r="C24" t="n">
+        <v>5000.0</v>
+      </c>
+    </row>
+    <row r="25">
+      <c r="A25" t="s">
+        <v>276</v>
+      </c>
+    </row>
+    <row r="26">
+      <c r="A26" t="s">
+        <v>269</v>
+      </c>
+      <c r="B26" t="s">
+        <v>53</v>
+      </c>
+      <c r="C26" t="n">
+        <v>1703.7801237952058</v>
+      </c>
+    </row>
+    <row r="27">
+      <c r="A27" t="s">
+        <v>270</v>
+      </c>
+      <c r="B27" t="s">
+        <v>34</v>
+      </c>
+      <c r="C27" t="n">
+        <v>17949.999999999996</v>
+      </c>
+    </row>
+    <row r="28">
+      <c r="A28" t="s">
+        <v>271</v>
+      </c>
+      <c r="B28" t="s">
+        <v>34</v>
+      </c>
+      <c r="C28" t="n">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="29">
+      <c r="A29" t="s">
+        <v>272</v>
+      </c>
+      <c r="B29" t="s">
+        <v>21</v>
+      </c>
+      <c r="C29" t="n">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="30">
+      <c r="A30" t="s">
+        <v>273</v>
+      </c>
+      <c r="B30" t="s">
+        <v>34</v>
+      </c>
+      <c r="C30" t="n">
+        <v>5000.0</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15.0" baseColWidth="35"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="s">
+        <v>277</v>
+      </c>
+      <c r="B2" t="s">
+        <v>10</v>
+      </c>
+      <c r="C2" t="s">
+        <v>278</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="s">
+        <v>279</v>
+      </c>
+      <c r="B3" t="s">
+        <v>10</v>
+      </c>
+      <c r="C3" t="s">
+        <v>280</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="s">
+        <v>281</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="s">
+        <v>282</v>
       </c>
       <c r="B7" t="s">
         <v>13</v>
       </c>
       <c r="C7" t="n">
-        <v>63.67173918048353</v>
+        <v>62.74439771473102</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="s">
-        <v>196</v>
+        <v>282</v>
       </c>
       <c r="B8" t="s">
         <v>19</v>
       </c>
       <c r="C8" t="n">
-        <v>123.76795953009756</v>
+        <v>121.96535192928275</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="s">
-        <v>197</v>
+        <v>283</v>
       </c>
       <c r="B9" t="s">
         <v>13</v>
       </c>
       <c r="C9" t="n">
-        <v>77.98163601388009</v>
+        <v>76.84587930967095</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="s">
-        <v>197</v>
+        <v>283</v>
       </c>
       <c r="B10" t="s">
         <v>19</v>
       </c>
       <c r="C10" t="n">
-        <v>151.58417367708873</v>
+        <v>149.37643926285926</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="s">
-        <v>198</v>
+        <v>284</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="s">
-        <v>199</v>
+        <v>285</v>
       </c>
       <c r="B12" t="s">
         <v>13</v>
       </c>
       <c r="C12" t="n">
-        <v>100.67385919725538</v>
+        <v>99.20760359700691</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="s">
-        <v>199</v>
+        <v>285</v>
       </c>
       <c r="B13" t="s">
         <v>19</v>
       </c>
       <c r="C13" t="n">
-        <v>195.6943267333258</v>
+        <v>192.8441538602726</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="s">
-        <v>200</v>
+        <v>286</v>
       </c>
       <c r="B14" t="s">
         <v>21</v>
@@ -3443,12 +4823,12 @@
     </row>
     <row r="15">
       <c r="A15" t="s">
-        <v>201</v>
+        <v>287</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="s">
-        <v>202</v>
+        <v>288</v>
       </c>
       <c r="B16" t="s">
         <v>13</v>
@@ -3459,7 +4839,7 @@
     </row>
     <row r="17">
       <c r="A17" t="s">
-        <v>202</v>
+        <v>288</v>
       </c>
       <c r="B17" t="s">
         <v>19</v>
@@ -3470,7 +4850,7 @@
     </row>
     <row r="18">
       <c r="A18" t="s">
-        <v>200</v>
+        <v>286</v>
       </c>
       <c r="B18" t="s">
         <v>21</v>
@@ -3481,12 +4861,12 @@
     </row>
     <row r="19">
       <c r="A19" t="s">
-        <v>203</v>
+        <v>289</v>
       </c>
     </row>
     <row r="20">
       <c r="A20" t="s">
-        <v>204</v>
+        <v>290</v>
       </c>
       <c r="B20" t="s">
         <v>13</v>
@@ -3497,7 +4877,7 @@
     </row>
     <row r="21">
       <c r="A21" t="s">
-        <v>204</v>
+        <v>290</v>
       </c>
       <c r="B21" t="s">
         <v>19</v>
@@ -3508,7 +4888,7 @@
     </row>
     <row r="22">
       <c r="A22" t="s">
-        <v>200</v>
+        <v>286</v>
       </c>
       <c r="B22" t="s">
         <v>21</v>
@@ -3519,12 +4899,12 @@
     </row>
     <row r="23">
       <c r="A23" t="s">
-        <v>205</v>
+        <v>291</v>
       </c>
     </row>
     <row r="24">
       <c r="A24" t="s">
-        <v>204</v>
+        <v>290</v>
       </c>
       <c r="B24" t="s">
         <v>13</v>
@@ -3535,7 +4915,7 @@
     </row>
     <row r="25">
       <c r="A25" t="s">
-        <v>204</v>
+        <v>290</v>
       </c>
       <c r="B25" t="s">
         <v>19</v>
@@ -3546,7 +4926,7 @@
     </row>
     <row r="26">
       <c r="A26" t="s">
-        <v>200</v>
+        <v>286</v>
       </c>
       <c r="B26" t="s">
         <v>21</v>
@@ -3557,12 +4937,12 @@
     </row>
     <row r="27">
       <c r="A27" t="s">
-        <v>206</v>
+        <v>292</v>
       </c>
     </row>
     <row r="28">
       <c r="A28" t="s">
-        <v>202</v>
+        <v>288</v>
       </c>
       <c r="B28" t="s">
         <v>13</v>
@@ -3573,7 +4953,7 @@
     </row>
     <row r="29">
       <c r="A29" t="s">
-        <v>202</v>
+        <v>288</v>
       </c>
       <c r="B29" t="s">
         <v>19</v>
@@ -3584,7 +4964,7 @@
     </row>
     <row r="30">
       <c r="A30" t="s">
-        <v>200</v>
+        <v>286</v>
       </c>
       <c r="B30" t="s">
         <v>21</v>
@@ -3595,34 +4975,34 @@
     </row>
     <row r="31">
       <c r="A31" t="s">
-        <v>207</v>
+        <v>293</v>
       </c>
     </row>
     <row r="32">
       <c r="A32" t="s">
-        <v>208</v>
+        <v>294</v>
       </c>
       <c r="B32" t="s">
         <v>13</v>
       </c>
       <c r="C32" t="n">
-        <v>77.98163601388009</v>
+        <v>76.84587930967093</v>
       </c>
     </row>
     <row r="33">
       <c r="A33" t="s">
-        <v>208</v>
+        <v>294</v>
       </c>
       <c r="B33" t="s">
         <v>19</v>
       </c>
       <c r="C33" t="n">
-        <v>151.58417367708873</v>
+        <v>149.37643926285926</v>
       </c>
     </row>
     <row r="34">
       <c r="A34" t="s">
-        <v>200</v>
+        <v>286</v>
       </c>
       <c r="B34" t="s">
         <v>21</v>
@@ -3638,55 +5018,55 @@
     </row>
     <row r="36">
       <c r="A36" t="s">
-        <v>209</v>
+        <v>295</v>
       </c>
     </row>
     <row r="37">
       <c r="A37" t="s">
-        <v>210</v>
+        <v>296</v>
       </c>
     </row>
     <row r="38">
       <c r="A38" t="s">
-        <v>199</v>
+        <v>285</v>
       </c>
       <c r="B38" t="s">
         <v>13</v>
       </c>
       <c r="C38" t="n">
-        <v>100.67385919725538</v>
+        <v>99.20760359700691</v>
       </c>
     </row>
     <row r="39">
       <c r="A39" t="s">
-        <v>199</v>
+        <v>285</v>
       </c>
       <c r="B39" t="s">
         <v>19</v>
       </c>
       <c r="C39" t="n">
-        <v>195.6943267333258</v>
+        <v>192.8441538602726</v>
       </c>
     </row>
     <row r="40">
       <c r="A40" t="s">
-        <v>200</v>
+        <v>286</v>
       </c>
       <c r="B40" t="s">
         <v>21</v>
       </c>
       <c r="C40" t="n">
-        <v>1.933638517645491</v>
+        <v>1.945847745415077</v>
       </c>
     </row>
     <row r="41">
       <c r="A41" t="s">
-        <v>211</v>
+        <v>297</v>
       </c>
     </row>
     <row r="42">
       <c r="A42" t="s">
-        <v>202</v>
+        <v>288</v>
       </c>
       <c r="B42" t="s">
         <v>13</v>
@@ -3697,7 +5077,7 @@
     </row>
     <row r="43">
       <c r="A43" t="s">
-        <v>202</v>
+        <v>288</v>
       </c>
       <c r="B43" t="s">
         <v>19</v>
@@ -3708,23 +5088,23 @@
     </row>
     <row r="44">
       <c r="A44" t="s">
-        <v>200</v>
+        <v>286</v>
       </c>
       <c r="B44" t="s">
         <v>21</v>
       </c>
       <c r="C44" t="n">
-        <v>2.245654566065172</v>
+        <v>2.280595155953703</v>
       </c>
     </row>
     <row r="45">
       <c r="A45" t="s">
-        <v>212</v>
+        <v>298</v>
       </c>
     </row>
     <row r="46">
       <c r="A46" t="s">
-        <v>204</v>
+        <v>290</v>
       </c>
       <c r="B46" t="s">
         <v>13</v>
@@ -3735,7 +5115,7 @@
     </row>
     <row r="47">
       <c r="A47" t="s">
-        <v>204</v>
+        <v>290</v>
       </c>
       <c r="B47" t="s">
         <v>19</v>
@@ -3746,23 +5126,23 @@
     </row>
     <row r="48">
       <c r="A48" t="s">
-        <v>200</v>
+        <v>286</v>
       </c>
       <c r="B48" t="s">
         <v>21</v>
       </c>
       <c r="C48" t="n">
-        <v>1.7479245778994392</v>
+        <v>1.768903849886927</v>
       </c>
     </row>
     <row r="49">
       <c r="A49" t="s">
-        <v>213</v>
+        <v>299</v>
       </c>
     </row>
     <row r="50">
       <c r="A50" t="s">
-        <v>204</v>
+        <v>290</v>
       </c>
       <c r="B50" t="s">
         <v>13</v>
@@ -3773,7 +5153,7 @@
     </row>
     <row r="51">
       <c r="A51" t="s">
-        <v>204</v>
+        <v>290</v>
       </c>
       <c r="B51" t="s">
         <v>19</v>
@@ -3784,23 +5164,23 @@
     </row>
     <row r="52">
       <c r="A52" t="s">
-        <v>200</v>
+        <v>286</v>
       </c>
       <c r="B52" t="s">
         <v>21</v>
       </c>
       <c r="C52" t="n">
-        <v>0.25207542210056066</v>
+        <v>0.23109615011307305</v>
       </c>
     </row>
     <row r="53">
       <c r="A53" t="s">
-        <v>214</v>
+        <v>300</v>
       </c>
     </row>
     <row r="54">
       <c r="A54" t="s">
-        <v>202</v>
+        <v>288</v>
       </c>
       <c r="B54" t="s">
         <v>13</v>
@@ -3811,7 +5191,7 @@
     </row>
     <row r="55">
       <c r="A55" t="s">
-        <v>202</v>
+        <v>288</v>
       </c>
       <c r="B55" t="s">
         <v>19</v>
@@ -3822,51 +5202,51 @@
     </row>
     <row r="56">
       <c r="A56" t="s">
-        <v>200</v>
+        <v>286</v>
       </c>
       <c r="B56" t="s">
         <v>21</v>
       </c>
       <c r="C56" t="n">
-        <v>-0.2456545660651721</v>
+        <v>-0.2805951559537032</v>
       </c>
     </row>
     <row r="57">
       <c r="A57" t="s">
-        <v>215</v>
+        <v>301</v>
       </c>
     </row>
     <row r="58">
       <c r="A58" t="s">
-        <v>208</v>
+        <v>294</v>
       </c>
       <c r="B58" t="s">
         <v>13</v>
       </c>
       <c r="C58" t="n">
-        <v>77.98163601388009</v>
+        <v>76.84587930967093</v>
       </c>
     </row>
     <row r="59">
       <c r="A59" t="s">
-        <v>208</v>
+        <v>294</v>
       </c>
       <c r="B59" t="s">
         <v>19</v>
       </c>
       <c r="C59" t="n">
-        <v>151.58417367708873</v>
+        <v>149.37643926285926</v>
       </c>
     </row>
     <row r="60">
       <c r="A60" t="s">
-        <v>200</v>
+        <v>286</v>
       </c>
       <c r="B60" t="s">
         <v>21</v>
       </c>
       <c r="C60" t="n">
-        <v>0.06636148235450878</v>
+        <v>0.0541522545849229</v>
       </c>
     </row>
     <row r="61">
@@ -3881,61 +5261,61 @@
     </row>
     <row r="63">
       <c r="A63" t="s">
-        <v>216</v>
+        <v>302</v>
       </c>
     </row>
     <row r="64">
       <c r="A64" t="s">
-        <v>217</v>
+        <v>303</v>
       </c>
       <c r="B64" t="s">
         <v>13</v>
       </c>
       <c r="C64" t="n">
-        <v>48.085536727355986</v>
+        <v>47.385199141416294</v>
       </c>
     </row>
     <row r="65">
       <c r="A65" t="s">
-        <v>217</v>
+        <v>303</v>
       </c>
       <c r="B65" t="s">
         <v>19</v>
       </c>
       <c r="C65" t="n">
-        <v>93.47080573352136</v>
+        <v>92.10945837424333</v>
       </c>
     </row>
     <row r="66">
       <c r="A66" t="s">
-        <v>218</v>
+        <v>304</v>
       </c>
     </row>
     <row r="67">
       <c r="A67" t="s">
-        <v>219</v>
+        <v>305</v>
       </c>
       <c r="B67" t="s">
         <v>13</v>
       </c>
       <c r="C67" t="n">
-        <v>68.00321819381641</v>
+        <v>67.01279128154086</v>
       </c>
     </row>
     <row r="68">
       <c r="A68" t="s">
-        <v>219</v>
+        <v>305</v>
       </c>
       <c r="B68" t="s">
         <v>19</v>
       </c>
       <c r="C68" t="n">
-        <v>132.18768115428674</v>
+        <v>130.26244525569496</v>
       </c>
     </row>
     <row r="69">
       <c r="A69" t="s">
-        <v>200</v>
+        <v>286</v>
       </c>
       <c r="B69" t="s">
         <v>21</v>
@@ -3946,34 +5326,34 @@
     </row>
     <row r="70">
       <c r="A70" t="s">
-        <v>220</v>
+        <v>306</v>
       </c>
     </row>
     <row r="71">
       <c r="A71" t="s">
-        <v>199</v>
+        <v>285</v>
       </c>
       <c r="B71" t="s">
         <v>13</v>
       </c>
       <c r="C71" t="n">
-        <v>84.36237073943346</v>
+        <v>83.13368238345649</v>
       </c>
     </row>
     <row r="72">
       <c r="A72" t="s">
-        <v>199</v>
+        <v>285</v>
       </c>
       <c r="B72" t="s">
         <v>19</v>
       </c>
       <c r="C72" t="n">
-        <v>163.98732973108014</v>
+        <v>161.5989506373884</v>
       </c>
     </row>
     <row r="73">
       <c r="A73" t="s">
-        <v>200</v>
+        <v>286</v>
       </c>
       <c r="B73" t="s">
         <v>21</v>
@@ -3989,83 +5369,83 @@
     </row>
     <row r="75">
       <c r="A75" t="s">
-        <v>221</v>
+        <v>307</v>
       </c>
     </row>
     <row r="76">
       <c r="A76" t="s">
-        <v>222</v>
+        <v>308</v>
       </c>
     </row>
     <row r="77">
       <c r="A77" t="s">
-        <v>219</v>
+        <v>305</v>
       </c>
       <c r="B77" t="s">
         <v>13</v>
       </c>
       <c r="C77" t="n">
-        <v>68.00321819381641</v>
+        <v>67.01279128154086</v>
       </c>
     </row>
     <row r="78">
       <c r="A78" t="s">
-        <v>219</v>
+        <v>305</v>
       </c>
       <c r="B78" t="s">
         <v>19</v>
       </c>
       <c r="C78" t="n">
-        <v>132.18768115428674</v>
+        <v>130.26244525569496</v>
       </c>
     </row>
     <row r="79">
       <c r="A79" t="s">
-        <v>200</v>
+        <v>286</v>
       </c>
       <c r="B79" t="s">
         <v>21</v>
       </c>
       <c r="C79" t="n">
-        <v>1.4526227825256133</v>
+        <v>1.4585417485291745</v>
       </c>
     </row>
     <row r="80">
       <c r="A80" t="s">
-        <v>223</v>
+        <v>309</v>
       </c>
     </row>
     <row r="81">
       <c r="A81" t="s">
-        <v>199</v>
+        <v>285</v>
       </c>
       <c r="B81" t="s">
         <v>13</v>
       </c>
       <c r="C81" t="n">
-        <v>84.36237073943346</v>
+        <v>83.13368238345649</v>
       </c>
     </row>
     <row r="82">
       <c r="A82" t="s">
-        <v>199</v>
+        <v>285</v>
       </c>
       <c r="B82" t="s">
         <v>19</v>
       </c>
       <c r="C82" t="n">
-        <v>163.98732973108014</v>
+        <v>161.5989506373884</v>
       </c>
     </row>
     <row r="83">
       <c r="A83" t="s">
-        <v>200</v>
+        <v>286</v>
       </c>
       <c r="B83" t="s">
         <v>21</v>
       </c>
       <c r="C83" t="n">
-        <v>1.4526227825256133</v>
+        <v>1.4585417485291745</v>
       </c>
     </row>
   </sheetData>

</xml_diff>